<commit_message>
add a semi-working translation skip list
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -471,12 +471,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>检查#[allow]属性的使用情况，并建议将其替换为#[expect]（请参阅RFC 2383）expect属性仍然不稳定，并且每晚都需要lint_reasonon。可以通过添加#来启用它！[feature（lint_reasons）]到机箱根。此lint仅警告外部属性（#[allow]），因为内部属性（#！[allow]]）通常用于在全局范围内启用或禁用lint。</t>
+          <t>检查#[allow]属性的使用情况，并建议将其替换为#[expect]（请参阅RFC 2383）expect属性仍然不稳定，并且每晚都需要lint_reasonon。可以通过添加#来启用它！[feature（lint_reasons）]到crate根。此lint仅警告外部属性（#[allow]），因为内部属性（#！[allow]]）通常用于在全局范围内启用或禁用lints。</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>#[expect]属性会抑制皮棉的发射，但如果预期未实现，则会发出警告。这对于在不再触发该命令时得到通知非常有用。</t>
+          <t>#[expect]属性抑制lint发射，但如果预期未实现，则会发出警告。这对于在不再触发该命令时得到通知非常有用。</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -577,7 +577,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>lint已被启用，表示首选AT&amp;T x86程序集语法。</t>
+          <t>已启用lint以指示首选AT&amp;T x86程序集语法。</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -617,7 +617,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>lint已被启用，以指示英特尔x86程序集语法的首选项。</t>
+          <t>lint已启用，表示首选英特尔x86程序集语法。</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -710,12 +710,12 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>检查异步块是否产生可等待的类型值。</t>
+          <t>检查是否有async块产生了可以等待的类型值。</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>等待可能会丢失。</t>
+          <t>可能缺少wait。</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -750,12 +750,12 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>检查as转换的使用情况。请注意，无论是否存在好的替代品，该lint都专门用于对as的每次使用进行lint处理。如果您想要更精确的as lint，请考虑使用这些单独的lint：unnecessary_cast、cast_lossless/cast_possible_trunation/cast_possible _wrap/cast_precision_loss/cast_sign_loss、fn_to_numeric_cast（_with_trunation），char_lit_as_u8、ref_to_mut和ptr_as_ptr。这里有一个很好的解释，解释了为什么这个lint应该以这种方式工作，以及它在这个问题中是如何使用的。</t>
+          <t>检查as转换的使用情况。请注意，无论是否存在好的替代方案，这个lint都专门用于对as的每一次使用进行lints处理。如果您想对as使用更精确的lints，请考虑使用这些单独的lints：unnecessary_cast、cast_lossless/cast_possible_trunation/cast_possible _wrap/cast_prision_loss/cast_sign_loss、fn_to_numeric_cast（_with_trunation），char_lit_as_u8、ref_to_mut和ptr_as_ptr。下面很好地解释了这个lint应该以这种方式工作的原因，以及它在这个问题上的用处。</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>as转换将执行许多类型的转换，包括无声的有损转换和危险的强制转换。在某些情况下，使用as是有意义的，所以lint默认为Allow。</t>
+          <t>as转换将执行多种转换，包括无声有损转换和危险的强制转换。在某些情况下，使用as是有意义的，所以默认情况下lint为Allow。</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -811,12 +811,12 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>检查外部板条箱和使用带lint属性注释的物品。此lint允许物品本身发出的lint属性。对于使用物品，这些lint为：depletedunreachable_pubunused_importsclippy:：enum_glob_useclippy:：macro_use_importsclippy::：wildcard_import对于外部板条箱物品，这些lint为：unused_mports on items with#[mmacro_use</t>
+          <t>检查externcrate和使用带lint属性注释的项。此lint允许在项本身上发出的lints具有linnt属性。对于使用项，这些lints为：depletedunreachable_pubunused_importsclippy:：enum_glob_useclippy:：macro_use_importsclippy::：wildcard_import对于extern_crate项，这些[ments]为：在带#[mmacro_use的项上未使用_imports</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>绒毛属性对板条箱导入没有影响。大多数情况下！被遗忘了。</t>
+          <t>Lint属性对crate导入没有影响。大多数情况下！被遗忘了。</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -953,7 +953,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>限制性短绒有时会与其他短绒形成对比，甚至会产生习惯性锈蚀。这些短绒只能在逐个短绒的基础上使用，并经过仔细考虑。</t>
+          <t>限制性lints有时与其他lint形成对比，甚至与惯用的铁锈相反。这些linth只能在逐个皮棉的基础上启用，并经过仔细考虑。</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1010,7 +1010,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>检查在目标族位置中是否使用了操作系统的cfg属性。</t>
+          <t>检查cfg属性是否在目标系列位置中使用了操作系统。</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1048,12 +1048,12 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>检查允许无理由进行lint的属性。（这需要lint_reasons功能）</t>
+          <t>检查允许无理由使用lints的属性。（这需要lint_reasons功能）</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>允许棉绒总是有原因的。应记录此原因，以确保其他人理解其原因</t>
+          <t>允许lint应该总是有原因的。应记录此原因，以确保其他人理解其原因</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1112,12 +1112,12 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>在持有非异步感知MutexGuard时检查等待的调用。</t>
+          <t>在持有非异步感知MutexGuard时，检查对wait的调用。</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>std:：sync和parking_lot中的Mutex类型并不是为了在等待点之间的异步上下文中操作而设计的。有两种潜在的解决方案。一种是使用异步感知Mutextype。许多异步基础板条箱都提供这种Mutex类型。另一种解决方案是通过引入作用域或显式调用Drop:：Drop来确保互斥锁在调用wait之前解锁。</t>
+          <t>std:：sync和parking_lot中的Mutex类型并不是为了在await点之间的async上下文中操作而设计的。有两种潜在的解决方案。一种是使用异步感知Mutextype。许多异步基础crates都提供这种Mutex类型。另一种解决方案是通过引入作用域或显式调用Drop:：Drop来确保互斥锁在调用wait之前解锁。</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1169,12 +1169,12 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>在持有RefCell Ref或RefMut时检查等待的调用。</t>
+          <t>在持有RefCell Ref或RefMut时检查是否调用了wait。</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>RefCell引用仅在运行时检查独占可变访问。在等待挂起点上保留一个RefCell引用可能会导致在其他引用未完成时共享的可变引用引发恐慌。</t>
+          <t>RefCell引用仅在运行时检查独占可变访问。在wait挂起点上保持RefCell引用可能会导致在其他引用未完成时共享的可变引用引发恐慌。</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1911,12 +1911,12 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>在宏定义中检查crate与$crate的使用情况。</t>
+          <t>检查宏定义中crate与$crate的用法。</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>crate指宏调用的crate，而$crate指的是宏定义的crate。前者的意图很少。请参阅：https://doc.rust-lang.org/reference/macros-by-example.html#hygiene</t>
+          <t>crate是指宏调用的crate，而$crate是指宏定义的crate。前者的意图很少。请参阅：https://doc.rust-lang.org/reference/macros-by-example.html#hygiene</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
@@ -1987,12 +1987,12 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>检查dbg的使用情况！宏。</t>
+          <t>检查dbg！宏的使用情况。</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>dbg！宏是一个调试工具。它不应出现在已发布的软件中，也不应提交到版本控制系统中。</t>
+          <t>dbg！宏用作调试工具。它不应出现在已发布的软件中，也不应提交到版本控制系统中。</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
@@ -2085,7 +2085,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>使用默认值检查单元结构的构造。</t>
+          <t>使用默认值检查单元struct的构造。</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -2192,12 +2192,12 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>使用默认表示形式（不带#[repr（C）]属性）声明并集时显示警告。</t>
+          <t>当使用默认表示形式（不带#[repr（C）]属性）声明union时，显示警告。</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Rust中的工会默认情况下有未指定的布局，尽管许多人认为他们在工会开始时就布局了每个字段（就像C一样）。也就是说，对于具有多个非ZST字段而没有明确指定布局的并集，无法保证字段的偏移量。这些情况可能导致不安全块中的未定义行为。</t>
+          <t>Rust中的联合默认情况下有未指定的布局，尽管许多人认为它们在union的开头布局每个字段（就像C一样）。也就是说，对于具有多个非ZST字段而没有明确指定布局的并集，无法保证字段的偏移量。这些情况可能导致不安全块中的未定义行为。</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
@@ -2600,7 +2600,7 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>拒绝在clippy.toml中配置的宏注意：即使此lint在默认情况下是警告的，但只有在clippy.toml文件中定义了宏时，它才会触发。</t>
+          <t>拒绝在clippy.toml中配置的宏注意：即使默认情况下此lint是警告，但只有在clippy.toml文件中定义了宏时才会触发。</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -2645,7 +2645,7 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>拒绝在clippy.toml中配置的方法和函数注意：即使此lint在默认情况下是警告的，但只有在clippy.toml文件中定义了方法时，它才会触发。</t>
+          <t>拒绝在clippy.toml中配置的方法和函数注意：即使默认情况下此lint是警告的，但只有在clippy.toml文件中定义了方法时，它才会触发。</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -2719,12 +2719,12 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>检查unicode脚本的使用情况，而不是lint配置明确允许的脚本。此lint不考虑Unknown和Linear_A等非文本脚本。它还忽略Common脚本类型。配置时，请确保使用支持脚本列表中的正式脚本名称别名。另请参阅：non_ascii_identits。</t>
+          <t>检查除lint配置明确允许的unicode脚本之外的其他脚本的使用情况。此linnt不考虑Unknown和Linear_A等非文本脚本。它还忽略Common脚本类型。配置时，请确保使用支持脚本列表中的正式脚本名别名。另请参阅：non_ascii_identits。</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>可能不希望在代码库中有许多不同的标识符脚本。请注意，如果您只想使用纯英语，则可能需要使用内置的non_ascii_identits lint。</t>
+          <t>可能不希望在代码库中有许多不同的标识符脚本。请注意，如果您只想使用纯英语，则可能需要使用内置的non_ascii_identitslint。</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
@@ -2750,7 +2750,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>拒绝在clippy.toml中配置的类型。注意：即使此lint在默认情况下是警告的，它也只会在clippy.toml文件中定义类型时触发。</t>
+          <t>拒绝clippy.toml中配置的类型。注意：尽管默认情况下此lint是警告，但它只会在clippy.toml文件中定义类型时触发。</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -2799,7 +2799,7 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Rustdoc支持markdown格式，_，：：和camel大小写可能表示一些应该包含在记号之间的代码也可以用于降价中的强调，这个lint试图考虑到这一点。</t>
+          <t>Rustdoc支持markdown格式，_，：：和camel大小写可能表示一些应该包含在记号之间的代码也可以用于markdown中的强调，thislint试图考虑这一点。</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
@@ -2833,7 +2833,7 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>不安全功能应记录其安全修复，以便用户能够确保他们安全使用它们。</t>
+          <t>不安全功能应记录其安全修复，以便用户能够确保他们安全使用这些功能。</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
@@ -2938,12 +2938,12 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>检查doctest中的fn main（）｛..｝</t>
+          <t>检查doctest中的fnmain（）｛..｝</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>如果将fn main（）保持为隐式，则测试可以更短（而且可能更可读）。</t>
+          <t>如果fnmain（）保持隐式，则测试可以更短（并且可能更可读）。</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
@@ -3292,7 +3292,7 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>检查没有变体的枚举。截至本文撰写之时，never_type仍然是唯一的实验性API。因此，只有在启用never_type时才会触发此lint。</t>
+          <t>检查没有变体的枚举。截至本文撰写之时，never_type仍然是唯一的实验性API。因此，只有启用了never_type，才会触发此lint。</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
@@ -3328,7 +3328,7 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>结构声明后的空括号可以省略。</t>
+          <t>可以省略struct声明后的空括号。</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
@@ -3501,7 +3501,7 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>一个典型的初学者错误是拥有mod foo；andagain mod foo｛..｝在foo.rs中。期望的是，内部mod foo｛.｝中的项通过foo：：x可用，但它们只能通过foo:：foo:：x可用。如果这是故意的，最好选择一个更具代表性的模块名称。</t>
+          <t>一个典型的初学者错误是有modfoo；andagainmodfoo｛..｝在foo.rs中。期望的是，内部modfoo{..｝中的项通过foo:：x是可用的，但它们只能通过foo:：foo:：x.使用。如果这是故意的，最好选择一个更具代表性的模块名称。</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
@@ -4197,7 +4197,7 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>检查二进制运算符右侧的一元运算符的格式。如果二进制运算符和一元运算符之间没有空格，但一元运算符和其操作数之间有空格，则它将进行lints。</t>
+          <t>检查二进制运算符右侧的一元运算符的格式。如果二进制运算符和一元运算符之间没有空格，但一元运算符及其操作数之间有空格，则为lints。</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
@@ -4232,7 +4232,7 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>检查else的格式。它判断elseis后面是否紧跟着一行换行符，或者else似乎不见了。</t>
+          <t>检查else的格式。它lints如果else后面紧跟一个换行符，或者else似乎丢失了。</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
@@ -4271,7 +4271,7 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>检查数组中是否可能缺少逗号。它表示ifan数组元素是一个二进制运算符表达式，它位于两行上。</t>
+          <t>检查数组中是否可能缺少逗号。ifan数组元素是一个二进制运算符表达式，它位于两行上。</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
@@ -4300,7 +4300,7 @@
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>检测格式！在另一个进行格式化的宏的参数中，例如format！本身，写！或println！。建议更改格式！呼叫</t>
+          <t>检测格式！在另一个进行格式化的宏的参数中，例如format！本身，write！或println！。建议更改格式！呼叫</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
@@ -4436,7 +4436,7 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>通过对self的递归调用来检查格式特征实现（例如Display），该调用使用self作为参数。这通常是通过write！宏或使用to_string（）。</t>
+          <t>使用self作为参数的递归调用来检查格式特征实现（例如Display）。这通常是通过write！宏或to_string（）间接完成的。</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
@@ -4601,7 +4601,7 @@
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>在处理FFI中的c_void原始指针时，很容易遇到用c_void指针调用from_raw的陷阱。Box:：from_law的类型签名是fn from_raw（raw:*mut T）-&gt;Box&lt;T&gt;，所以如果你传递一个*mut c_void，你会得到一个Box&lt;c_void&gt;（Rc、Arc和Weak也是如此）。为了安全起见，c_void需要与原始类型具有相同的内存布局，通常情况并非如此。</t>
+          <t>在处理FFI中的c_void原始指针时，很容易遇到用c_void指针调用from_raw的陷阱。Box:：from_law的类型签名是fnfrom_raw（raw:*mut T）-&gt;Box&lt;T&gt;，所以如果你传递*mut c_void，你会得到一个Box&lt;c_void&gt;（类似于Rc、Arc和Weak）。为了安全起见，c_void需要与原始类型具有相同的内存布局，通常情况并非如此。</t>
         </is>
       </c>
       <c r="E117" t="inlineStr">
@@ -4953,7 +4953,7 @@
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>检查所有字段都是简写的结构构造函数，并且构造函数中字段init简写的顺序与结构定义中的顺序不一致。</t>
+          <t>检查所有字段都是简写的struct构造函数，并且构造函数中字段init简写的顺序与struct定义中的顺序不一致。</t>
         </is>
       </c>
       <c r="D127" t="inlineStr">
@@ -5164,7 +5164,7 @@
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>检查结构的多个固有实现</t>
+          <t>检查struct的多个固有实现</t>
         </is>
       </c>
       <c r="D133" t="inlineStr">
@@ -5292,7 +5292,7 @@
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>检查使用字段语法初始化的元组结构。但是，如果存在基初始值设定项，它将不会lint。lint还会忽略宏中的代码。</t>
+          <t>检查是否使用字段语法初始化的元组结构。但是，如果存在基初始值设定项，则不会执行lint。lind也将忽略宏中的代码。</t>
         </is>
       </c>
       <c r="D136" t="inlineStr">
@@ -5362,7 +5362,7 @@
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>很容易意外地写入prev_instant-instant:：now（），它将始终为0nsas。instant减法饱和。prev_intant.elapsed（）也更清楚地表示意图。</t>
+          <t>很容易意外地写入prev_instant-instant:：now（），它将始终是0nsasinstant减法饱和。prev_intant.elapsed（）也更清楚地表示意图。</t>
         </is>
       </c>
       <c r="E138" t="inlineStr">
@@ -5712,7 +5712,7 @@
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>它检查async fn或async｛｝创建的Future的大小。</t>
+          <t>它检查由asyncfn或async｛｝创建的Future的大小。</t>
         </is>
       </c>
       <c r="D148" t="inlineStr">
@@ -5853,7 +5853,7 @@
       </c>
       <c r="D152" t="inlineStr">
         <is>
-          <t>两种方法都有是很好的自定义，因为对于某些数据结构，询问长度将是一项代价高昂的操作，而.is_empty（）通常可以在恒定时间内回答。此外，它曾在len_zero lint上导致误报——目前lint将忽略此类实体。</t>
+          <t>两种方法都有是很好的自定义，因为对于某些数据结构，询问长度将是一项代价高昂的操作，而.is_empty（）通常可以在恒定时间内回答。此外，它曾在len_zerolint上导致误报——目前lint将忽略此类实体。</t>
         </is>
       </c>
       <c r="E152" t="inlineStr">
@@ -6030,7 +6030,7 @@
       </c>
       <c r="D157" t="inlineStr">
         <is>
-          <t>必须对未来的工作进行调查。最初的意图很可能是等待未来，而忽略由此产生的价值。</t>
+          <t>必须对未来的工作进行调查。最初的意图很可能是wait未来，而忽略由此产生的价值。</t>
         </is>
       </c>
       <c r="E157" t="inlineStr">
@@ -6363,7 +6363,7 @@
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>如果积分或浮点常量的数字分组过大，则发出警告。</t>
+          <t>如果积分或浮点常量的数字分组太大，则发出警告。</t>
         </is>
       </c>
       <c r="D167" t="inlineStr">
@@ -6477,7 +6477,7 @@
       </c>
       <c r="D171" t="inlineStr">
         <is>
-          <t>明确肯定比如果那么恐慌更简单！。</t>
+          <t>assert！比if-then-panic！简单！。</t>
         </is>
       </c>
       <c r="E171" t="inlineStr">
@@ -6506,7 +6506,7 @@
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>它检查异步函数的手动实现。</t>
+          <t>它检查async函数的手动实现。</t>
         </is>
       </c>
       <c r="D172" t="inlineStr">
@@ -6853,7 +6853,7 @@
       </c>
       <c r="D181" t="inlineStr">
         <is>
-          <t>写入时间更短消除了人员和编译器对多路复用中溢出的担忧在运行时可能会更快，因为rust在计算字节长度时会发出特殊的无包装标志减少了涡轮捕鱼</t>
+          <t>写入时间更短消除了人员和编译器对多路复用中溢出的担忧可能在运行时更快，因为rust在计算字节长度时会发出特殊的无包装标志减少了涡轮捕鱼</t>
         </is>
       </c>
       <c r="E181" t="inlineStr">
@@ -7471,7 +7471,7 @@
       </c>
       <c r="D199" t="inlineStr">
         <is>
-          <t>Doc很好。rustc为公共成员提供了一个MISSING_DOCSallowed-by-default lint，但无法强制执行私有项的文档。这个lint解决了这个问题。</t>
+          <t>Doc很好。rustc为公共成员提供了一个MISSING_OCSallowed-by-defaultlint，但无法强制执行私有项的文档。此lint修复了此问题。</t>
         </is>
       </c>
       <c r="E199" t="inlineStr"/>
@@ -7521,12 +7521,12 @@
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>它检测导出的函数、方法、具有默认impl的trait方法或trait方法impl是否不是#[inline]。</t>
+          <t>如果导出的函数、方法、具有默认impl的trait方法或trait方法impl不是#[inline]，则为lints。</t>
         </is>
       </c>
       <c r="D201" t="inlineStr">
         <is>
-          <t>总的来说，事实并非如此。只要使用任何形式的LTO，只要有利可图，函数就可以跨脚本内联。当LTO被禁用时，非#[inline]的函数不能跨板条箱内联。某些类型的cratesmith打算使其公共API中的大多数方法能够跨crates内联，即使LTO被禁用。对于这些类型的板条箱，启用这种棉绒可能是有意义的。它允许机箱默认要求所有导出的方法都是#[inline]，然后在可能没有意义的情况下选择退出特定的方法。</t>
+          <t>总的来说，事实并非如此。只要使用任何形式的LTO，只要有利可图，函数就可以跨脚本内联。当LTO被禁用时，非#[inline]的函数不能跨板条箱内联。某些类型的cratesmith打算使其公共API中的大多数方法能够跨crates内联，即使LTO被禁用。对于这些类型的板条箱，启用这种lint可能是有意义的。它允许crate在默认情况下要求所有导出的方法都是#[inline]，然后在可能没有意义的情况下选择退出特定的方法。</t>
         </is>
       </c>
       <c r="E201" t="inlineStr">
@@ -7570,7 +7570,7 @@
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>检查所提供的方法是否被跟踪实现隐式使用。一个使用示例是包装器，其中每个方法都应该在委托给内部类型的simplementation之前执行一些操作。该lint通常应该在特定的trait impl项上启用，而不是全局启用。</t>
+          <t>检查所提供的方法是否被跟踪实现隐式使用。一个使用示例是一个包装器，其中每个方法都应该在委托给内部类型“simplementation”之前执行一些操作。该lint通常应该在特定的trait impl项上启用，而不是全局启用。</t>
         </is>
       </c>
       <c r="D202" t="inlineStr">
@@ -7769,7 +7769,7 @@
       </c>
       <c r="D207" t="inlineStr">
         <is>
-          <t>该lint与undocumented_unsaf.blocks相结合，确保每个不安全的操作都必须独立证明。与unused_unsafe相结合，该lint还确保通过重构消除不必要的不安全块。</t>
+          <t>此lint与undocumented_unsaf.blocks结合，确保每个不安全的操作都必须独立证明。与unused_unsafe结合，也确保通过重构消除不必要的不安全块。</t>
         </is>
       </c>
       <c r="E207" t="inlineStr">
@@ -8252,7 +8252,7 @@
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t>lint检查循环中出现的if语句是否在其主块或else块中包含continue语句，而省略else块可能会使代码更容易理解。</t>
+          <t>lint检查循环中出现的语句是否在其主块或else块中包含continue语句，而省略else块可能会使代码更容易理解。</t>
         </is>
       </c>
       <c r="D220" t="inlineStr">
@@ -8408,7 +8408,7 @@
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>lint检查范围语句中的文本上是否有括号。</t>
+          <t>lint检查范围语句中超级模糊的文字上的括号。</t>
         </is>
       </c>
       <c r="D223" t="inlineStr">
@@ -8526,7 +8526,7 @@
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>当所有字段都发生更改时，检查是否在更新时不必要地包含基结构。此lint不应用于标记为non_exhaustive的结构。</t>
+          <t>当所有字段都更改时，检查是否在更新时不必要地包含基struct。此lint不应用于标记为non_exhaustive的结构。</t>
         </is>
       </c>
       <c r="D226" t="inlineStr">
@@ -8640,7 +8640,7 @@
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>使用pub-fn-new（）-&gt;Self方法检查公共类型，并且不执行默认值。</t>
+          <t>使用pubfnnew（）-&gt;Self方法检查公共类型，并且不实现默认值。</t>
         </is>
       </c>
       <c r="D229" t="inlineStr">
@@ -8683,7 +8683,7 @@
       </c>
       <c r="D230" t="inlineStr">
         <is>
-          <t>这主要是一个一致性lint，尽管使用（）或[]不会在项位置给您一个分号，这可能是出乎意料的。</t>
+          <t>这主要是一种一致性lint，尽管使用（）或[]不会在项位置使用分号，这可能是出乎意料的。</t>
         </is>
       </c>
       <c r="E230" t="inlineStr">
@@ -8713,7 +8713,7 @@
       </c>
       <c r="D231" t="inlineStr">
         <is>
-          <t>const被复制到引用的任何地方，也就是说，每次引用const时，都会创建一个新的Cell或Mutemor AtomicXxxx实例，这从一开始就违背了使用这些类型的全部目的。如果需要全局变量，const最好用静态项替换，如果需要构造函数，则最好用const fn替换。</t>
+          <t>const被复制到引用的任何地方，也就是说，每次引用const时，都会创建一个新的Cell或Mutemor AtomicXxxx实例，这从一开始就违背了使用这些类型的全部目的。如果需要全局变量，const最好用静态项替换，如果需要构造函数，则最好用constfn替换。</t>
         </is>
       </c>
       <c r="E231" t="inlineStr">
@@ -8898,12 +8898,12 @@
       </c>
       <c r="C237" t="inlineStr">
         <is>
-          <t>此lint警告一个类型的Send实现，该类型包含在线程之间发送不安全的字段。它试图检测在发送到另一个线程（例如，Rc）时可能导致可靠性问题的字段，同时允许！发送类型中应存在的发送字段，例如原始指针。</t>
+          <t>此lint警告一个类型的Send实现，该类型包含在线程间发送不安全的字段。它试图检测在发送到另一个线程（例如Rc）时可能导致可靠性问题的字段，同时允许！发送类型中应存在的发送字段，例如原始指针。</t>
         </is>
       </c>
       <c r="D237" t="inlineStr">
         <is>
-          <t>将结构发送到另一个线程可以有效地发送其所有字段，而不实现Send的字段可能会导致健全性错误，例如在与创建它的线程不同的线程中访问数据时会发生争用。请参阅：关于Send和Sync的Rustonomicon Send文档</t>
+          <t>将struct发送到另一个线程可以有效地发送它的所有字段，而不实现Send的字段可能会导致健全性错误，例如在与创建它的线程不同的线程中访问数据时会发生争用。请参阅：关于Send和Sync的Rustonomicon Send文档</t>
         </is>
       </c>
       <c r="E237" t="inlineStr">
@@ -9228,7 +9228,7 @@
       </c>
       <c r="C247" t="inlineStr">
         <is>
-          <t>检查恐慌的使用情况！，未实现！，todo！，无法访问！或result类型函数中的断言。</t>
+          <t>检查恐慌的使用情况！，未实现！，todo！，reachable！或result类型函数中的断言。</t>
         </is>
       </c>
       <c r="D247" t="inlineStr">
@@ -9268,7 +9268,7 @@
       </c>
       <c r="D248" t="inlineStr">
         <is>
-          <t>惊恐将停止执行可执行文件</t>
+          <t>panic！将停止执行可执行文件</t>
         </is>
       </c>
       <c r="E248" t="inlineStr">
@@ -9431,7 +9431,7 @@
       </c>
       <c r="C254" t="inlineStr">
         <is>
-          <t>检查结构的部分字段是否为公共字段。将某个类型的所有字段设置为公共字段，或者不设置任何公共字段</t>
+          <t>检查struct的部分字段是否为公共字段。将某个类型的所有字段设为公共字段，或者不设任何字段为公共字段</t>
         </is>
       </c>
       <c r="D254" t="inlineStr">
@@ -9533,7 +9533,7 @@
       </c>
       <c r="C257" t="inlineStr">
         <is>
-          <t>检查不是应用到的类型的精确表示的模式。要满足此lint，您必须调整与匹配的表达式或模式本身，以及调整后的模式引入的绑定。为了进行匹配，您必须使用*运算符取消对表达式的引用，或者根据引用的可变性修改模式以显式匹配&amp;&lt;pattern&gt;或&amp;mut&lt;pattern&gt;。对于绑定，您需要使用相反的方法。如果您希望复制值，可以将它们保留为纯绑定，但必须使用ref mut＜variable＞或ref＜variable＜在匹配的结构中构造引用。如果您正在寻找更详细地了解所有权语义的方法，建议您查看可用的IDE选项，以突出显示代码中的类型、生命周期和引用语义。即使在各种模式匹配机制之外，可用的工具也会以通用的方式暴露这些东西。当然，这个lint仍然可以用来突出感兴趣的领域，并确保对所有权语义有很好的理解。</t>
+          <t>检查不是应用到的类型的精确表示的模式。要满足此lint，您必须调整与匹配的表达式或模式本身，以及调整后的模式引入的绑定。为了进行匹配，您必须使用*运算符取消对表达式的引用，或者根据引用的可变性修改模式以显式匹配&amp;&lt;pattern&gt;或&amp;mut&lt;pattern&gt;。对于绑定，您需要使用相反的方法。如果您希望复制值，可以将它们保留为纯绑定，但必须使用ref mut＜variable＞或ref＜variable＜在匹配的结构中构造引用。如果您正在寻找更详细地了解所有权语义的方法，建议您查看可用的IDE选项，以突出显示代码中的类型、生命周期和引用语义。即使在各种模式匹配机制之外，可用的工具也会以通用的方式暴露这些东西。当然，这个lint仍然可以用来突出感兴趣的领域，并确保很好地理解所有权语义。</t>
         </is>
       </c>
       <c r="D257" t="inlineStr">
@@ -9644,7 +9644,7 @@
       </c>
       <c r="C260" t="inlineStr">
         <is>
-          <t>此lint检查类型为&amp;String、&amp;Vec、&amp;PathBuf和Cow＜_＞的函数参数。它还建议您将.clone（）调用替换为适当的.to_owned（）/to_string（）调用。</t>
+          <t>此lint检查类型为&amp;String、&amp;Vec、&amp;PathBuf和Cow&lt;_&gt;的函数参数。它还建议您将.clone（）调用替换为适当的.to_owned（）/to_string（）调用。</t>
         </is>
       </c>
       <c r="D260" t="inlineStr">
@@ -10087,7 +10087,7 @@
       </c>
       <c r="C273" t="inlineStr">
         <is>
-          <t>此lint捕获对零长度Vec的读取。特别是在调用with_capacity的情况下，此lint警告readgets是从Vec的长度而非容量中获取字节数。</t>
+          <t>这个lint捕获对零长度Vec的读取。特别是在调用with_capacity的情况下，这个linet警告read从Vec的长度而不是容量中获取字节数。</t>
         </is>
       </c>
       <c r="D273" t="inlineStr">
@@ -10126,7 +10126,7 @@
       </c>
       <c r="C274" t="inlineStr">
         <is>
-          <t>检查只返回等待未来的异步块。</t>
+          <t>检查只在将来返回await的async块。</t>
         </is>
       </c>
       <c r="D274" t="inlineStr">
@@ -10164,7 +10164,7 @@
       </c>
       <c r="C275" t="inlineStr">
         <is>
-          <t>检查冗余克隆（）（及其亲属），该克隆克隆将被丢弃而不再使用的所有者值。</t>
+          <t>检查一个冗余克隆（）（及其亲属），该克隆克隆将被丢弃而不再使用的所有者值。</t>
         </is>
       </c>
       <c r="D275" t="inlineStr">
@@ -10276,7 +10276,7 @@
       </c>
       <c r="C278" t="inlineStr">
         <is>
-          <t>检查结构文本中可以使用shorthands的字段。</t>
+          <t>检查struct文本中可以使用shorthands的字段。</t>
         </is>
       </c>
       <c r="D278" t="inlineStr">
@@ -10308,7 +10308,7 @@
       </c>
       <c r="C279" t="inlineStr">
         <is>
-          <t>检查声明为pub（板条箱）的物品，这些物品由于在专用模块内而不可见。</t>
+          <t>检查声明为pub（crate）的项目，这些项目由于在私有模块内而不可见。</t>
         </is>
       </c>
       <c r="D279" t="inlineStr">
@@ -10705,7 +10705,7 @@
       </c>
       <c r="C291" t="inlineStr">
         <is>
-          <t>它检测一个结构是否有两个同名的方法：一个来自trait，另一个不来自trait。</t>
+          <t>如果一个struct有两个同名的方法：一个来自trait，另一个不来自trait。</t>
         </is>
       </c>
       <c r="D291" t="inlineStr">
@@ -10785,7 +10785,7 @@
       </c>
       <c r="D293" t="inlineStr">
         <is>
-          <t>为了保持一致性，最好在块内部/外部使用分号。无论哪种方式都很好，这个lint建议在块内部。看看另一种选择的分号outside_block。</t>
+          <t>为了保持一致性，最好在块内部/外部使用分号。无论哪种方式都很好，lint都建议在块内部。另一种选择是分号outside_block。</t>
         </is>
       </c>
       <c r="E293" t="inlineStr">
@@ -10819,7 +10819,7 @@
       </c>
       <c r="D294" t="inlineStr">
         <is>
-          <t>为了保持一致性，最好在块内部/外部使用分号。无论哪种方式都很好，这个lint建议在块外。看看另一种选择的分号_inside_block。</t>
+          <t>为了保持一致性，最好在块内部/外部使用分号。无论哪种方式都很好，lint建议在块外。另一种选择请查看分号_inside_block。</t>
         </is>
       </c>
       <c r="E294" t="inlineStr">
@@ -11236,7 +11236,7 @@
       </c>
       <c r="D306" t="inlineStr">
         <is>
-          <t>具有no-std兼容性的机箱可能希望确保从核心导入类型，以确保重新编译std不会导致机箱编译失败。这种皮棉也有助于板条箱迁移，使其与no-std兼容。</t>
+          <t>具有no-std兼容性的板条箱可能希望确保从核心导入类型，以确保重新编译std不会导致crate编译失败。此lint也可用于板条箱迁移，使其与no-std兼容。</t>
         </is>
       </c>
       <c r="E306" t="inlineStr">
@@ -11266,7 +11266,7 @@
       </c>
       <c r="D307" t="inlineStr">
         <is>
-          <t>具有no-std兼容性并需要alloc的机箱可能希望确保从alloc导入类型，以确保禁用std不会导致机箱编译失败。这种皮棉也适用于迁移到no-std兼容的板条箱。</t>
+          <t>具有no-std兼容性并需要alloc的机箱可能希望确保从alloc导入类型，以确保禁用std不会导致crate编译失败。这个lint也适用于crates迁移到no-std兼容。</t>
         </is>
       </c>
       <c r="E307" t="inlineStr">
@@ -11297,7 +11297,7 @@
       </c>
       <c r="D308" t="inlineStr">
         <is>
-          <t>具有no-std兼容性并可能需要alloc的机箱可能希望确保从核心导入类型，以确保禁用alloc不会导致机箱编译失败。这种短绒也适用于迁移到no-std兼容的板条箱。</t>
+          <t>具有no-std兼容性并可能需要alloc的机箱可能希望确保从核心导入类型，以确保禁用alloc不会导致crate编译失败。这个lint对于crates迁移到no_std兼容也很有用。</t>
         </is>
       </c>
       <c r="E308" t="inlineStr">
@@ -11781,7 +11781,7 @@
       </c>
       <c r="C323" t="inlineStr">
         <is>
-          <t>检查手动交换。注意，lint不会在const块中发出，因为该建议不适用。</t>
+          <t>检查手动交换。请注意，lint不会在const块中发出，因为该建议不适用。</t>
         </is>
       </c>
       <c r="D323" t="inlineStr">
@@ -11893,7 +11893,7 @@
       </c>
       <c r="D326" t="inlineStr">
         <is>
-          <t>铁锈风格指南提倡使用空格而不是制表符进行缩进。为了保持对源代码的一致看法，文档注释也不应该有制表符。此外，当作者和读者的显示设置不同时，解释包含制表符的ascii图可能会显示不正确。</t>
+          <t>rust样式指南提倡使用空格而不是制表符进行缩进。为了保持对源代码的一致性，文档注释也不应该有制表符。此外，当作者和读者的显示设置不同时，解释包含制表符的ascii图可能会不正确地显示。</t>
         </is>
       </c>
       <c r="E326" t="inlineStr">
@@ -12045,12 +12045,12 @@
       </c>
       <c r="C330" t="inlineStr">
         <is>
-          <t>当在没有repr属性的情况下声明具有尾随零大小数组的结构时，显示警告。</t>
+          <t>当声明带有尾随零大小数组的struct而没有repr属性时，显示警告。</t>
         </is>
       </c>
       <c r="D330" t="inlineStr">
         <is>
-          <t>零大小的数组在Rust本身中不是很有用，因此创建这样的结构很可能是为了传递给C代码，或者在其他对内存布局的控制很重要的情况下（例如，结合手动分配，可以轻松计算数组的偏移量）。无论哪种方式，都需要#[repr（C）]（或另一个repr属性）。</t>
+          <t>零大小的数组在Rust本身中不是很有用，所以创建这样的struct很可能是为了传递给C代码，或者在其他对内存布局的控制很重要的情况下（例如，结合手动分配，可以轻松计算数组的偏移量）。无论哪种方式，都需要#[repr（C）]（或另一个repr属性）。</t>
         </is>
       </c>
       <c r="E330" t="inlineStr">
@@ -12082,7 +12082,7 @@
       </c>
       <c r="C331" t="inlineStr">
         <is>
-          <t>该lint警告在特征范围内不必要的类型重复</t>
+          <t>此lint警告特征边界中不必要的类型重复</t>
         </is>
       </c>
       <c r="D331" t="inlineStr">
@@ -12412,7 +12412,7 @@
       </c>
       <c r="C342" t="inlineStr">
         <is>
-          <t>检查包含Box＜T＞的返回类型，其中T实现SizedLint忽略Box＜T&gt;，其中T大于unnecessary_Box_size，因为直接返回大T可能会对性能不利。</t>
+          <t>检查包含Box＜T＞的返回类型，其中T实现Sizedlint忽略Box＜T&gt;，其中T大于unnecessary_Box_size，因为直接返回大T可能会对性能不利。</t>
         </is>
       </c>
       <c r="D342" t="inlineStr">
@@ -12506,12 +12506,12 @@
       </c>
       <c r="C345" t="inlineStr">
         <is>
-          <t>通过复制基而不设置任何字段来检查结构的初始化。</t>
+          <t>通过复制基而不设置任何字段来检查struct的初始化。</t>
         </is>
       </c>
       <c r="D345" t="inlineStr">
         <is>
-          <t>可读性受到不必要的结构构建的影响。</t>
+          <t>可读性受到不必要的struct构建的影响。</t>
         </is>
       </c>
       <c r="E345" t="inlineStr">
@@ -12655,7 +12655,7 @@
       </c>
       <c r="D349" t="inlineStr">
         <is>
-          <t>没有异步代码的异步函数在心理和计算上都会产生开销。异步方法的调用方要么需要自己从异步函数调用，要么在执行器上运行，这两者都会给调用方带来运行时开销和麻烦。</t>
+          <t>没有Async代码的异步函数在心理和计算上都会产生开销。Async方法的调用方要么需要自己从assync函数调用，要么在执行器上运行，这两种情况都会给调用方带来运行时开销和麻烦。</t>
         </is>
       </c>
       <c r="E349" t="inlineStr">
@@ -12972,7 +12972,7 @@
       </c>
       <c r="D358" t="inlineStr">
         <is>
-          <t>在CamelCase中，首字母缩略词算作一个单词。有关更多信息，请参阅命名惯例。默认情况下，lint仅在全大写名称上触发。您可以使用大写首字母缩写词aggressive：true config选项在所有camel大小写名称上启用lintin</t>
+          <t>在CamelCase中，首字母缩略词算作一个单词。有关更多信息，请参阅命名惯例。默认情况下，lint仅在全大写名称上触发。您可以使用大写首字母缩略语aggressive：true config选项在所有camel大小写名称上启用linting</t>
         </is>
       </c>
       <c r="E358" t="inlineStr">
@@ -13098,7 +13098,7 @@
       </c>
       <c r="C362" t="inlineStr">
         <is>
-          <t>在创建新的Vec后立即检查对push的调用。如果使用with_capacity创建Vec，则只有在容量保持不变且推送次数大于或等于初始容量时，才会进行lint。如果Vec在初始推送序列之后扩展，并且它是默认初始化的，则至少有四次推送后，才会进行linet。这个数字将来可能会改变。</t>
+          <t>在创建新的Vec后立即检查对push的调用。如果使用with_capacity创建Vec，则只有在容量不变且推送次数大于或等于初始容量的情况下，此调用才会lint。如果Vec在初始推送序列之后扩展，并且它是默认初始化的，则至少有四次推送后，此调用才lind。这个数字将来可能会改变。</t>
         </is>
       </c>
       <c r="D362" t="inlineStr">
@@ -13195,7 +13195,7 @@
       </c>
       <c r="C365" t="inlineStr">
         <is>
-          <t>使用println时，此皮棉会发出警告！（“”）打印新行。</t>
+          <t>当您使用println时，此lint会发出警告！（“”）打印新行。</t>
         </is>
       </c>
       <c r="D365" t="inlineStr">
@@ -13225,7 +13225,7 @@
       </c>
       <c r="C366" t="inlineStr">
         <is>
-          <t>当你使用印花时，这种棉绒会发出警告！（），格式字符串以换行符结尾。</t>
+          <t>当您使用打印时，此lint会发出警告！（），格式字符串以换行符结尾。</t>
         </is>
       </c>
       <c r="D366" t="inlineStr">
@@ -13339,7 +13339,7 @@
       </c>
       <c r="D370" t="inlineStr">
         <is>
-          <t>使用文字作为println！args是低效的（c.f。，https://github.com/matthiaskrgr/rust-str-bench)和不必要的（即，只需将文本放在格式字符串中）</t>
+          <t>使用文本作为println！参数是低效的（c.f。，https://github.com/matthiaskrgr/rust-str-bench)和不必要的（即，只需将文本放在格式字符串中）</t>
         </is>
       </c>
       <c r="E370" t="inlineStr">
@@ -13396,7 +13396,7 @@
       </c>
       <c r="C372" t="inlineStr">
         <is>
-          <t>当你使用write时，这个lint会发出警告！（），格式字符串以换行结束。</t>
+          <t>当您使用write时，此lint会发出警告！（），格式字符串以换行结束。</t>
         </is>
       </c>
       <c r="D372" t="inlineStr">
@@ -13653,7 +13653,7 @@
       </c>
       <c r="C379" t="inlineStr">
         <is>
-          <t>检查是否安装了多个版本的板条箱。</t>
+          <t>检查是否安装了crate的多个版本。</t>
         </is>
       </c>
       <c r="D379" t="inlineStr">
@@ -13709,7 +13709,7 @@
       </c>
       <c r="C381" t="inlineStr">
         <is>
-          <t>检查从任何数字类型到浮点类型的强制转换，如果接收类型无法存储原始类型中的所有值而没有超出范围的错误。这种可能的舍入是意料之中的，所以这个lint在默认情况下是Allow。基本上，这会警告将任何32位或更多位的整数强制转换为f32，或将任何64位整数强制转换成f64。</t>
+          <t>检查从任何数字类型到浮点类型的强制转换，如果接收类型无法存储原始类型中的所有值而没有超出范围的错误。这种可能的四舍五入是意料之中的，所以默认情况下，这个lint是Allow。基本上，当将任何32位或更多位的整数强制转换为f32或将任何64位的整数转换为f64时，这会发出警告。</t>
         </is>
       </c>
       <c r="D381" t="inlineStr">
@@ -13736,7 +13736,7 @@
       </c>
       <c r="C382" t="inlineStr">
         <is>
-          <t>检查从有符号数字类型到无符号数字类型的强制转换。在这种情况下，负值会变成大的正值，这在实践中可能会非常令人惊讶。但是，由于强制转换按定义工作，该lint在默认情况下为“允许”。</t>
+          <t>检查从有符号数字类型到无符号数字类型的强制转换。在这种情况下，负值会变成大的正值，这在实践中可能会非常令人惊讶。但是，由于强制转换按定义工作，默认情况下此lint为Allow。</t>
         </is>
       </c>
       <c r="D382" t="inlineStr">
@@ -13768,7 +13768,7 @@
       </c>
       <c r="D383" t="inlineStr">
         <is>
-          <t>在某些问题领域，避免截断是一种很好的做法。这种棉绒可以被激活，以帮助评估额外检查可能有益的地方。</t>
+          <t>在某些问题领域，避免截断是一种很好的做法。该lint可以被激活，以帮助评估额外检查可能有益的地方。</t>
         </is>
       </c>
       <c r="E383" t="inlineStr">
@@ -14140,7 +14140,7 @@
       </c>
       <c r="C394" t="inlineStr">
         <is>
-          <t>检查是否从枚举类型强制转换为肯定会截断值的整型。</t>
+          <t>检查是否从enum类型转换为肯定会截断值的整型。</t>
         </is>
       </c>
       <c r="D394" t="inlineStr">
@@ -14213,12 +14213,12 @@
       </c>
       <c r="C396" t="inlineStr">
         <is>
-          <t>检查从枚举元组构造函数到整数的强制转换。</t>
+          <t>检查从enum元组构造函数到整数的强制转换。</t>
         </is>
       </c>
       <c r="D396" t="inlineStr">
         <is>
-          <t>强制转换很容易与将类似c的枚举值强制转换为整数混淆。</t>
+          <t>强制转换很容易与将类似c的enum值强制转换为整数混淆。</t>
         </is>
       </c>
       <c r="E396" t="inlineStr">
@@ -14502,7 +14502,7 @@
       </c>
       <c r="D405" t="inlineStr">
         <is>
-          <t>该函数几乎肯定应该被标记为不安全，因为对于一个rbitrary原始指针，没有办法确定它是否有效。通常，除非它是肯定的（如果是，请提交一个问题），否则永远不应该禁用此lint，因为它破坏了Rust的健全性保证，直接使API用户面临潜在的危险程序行为。对于内部API也是如此，因为它很容易泄漏。</t>
+          <t>该函数几乎肯定应该被标记为不安全，因为对于一个原始指针，没有办法确定它是否有效。通常，除非它肯定是肯定的（如果是，请提交一个问题），否则永远不应该禁用这个lint，因为它破坏了Rust的可靠性保证，直接使API用户面临潜在的危险程序行为。对于内部API也是如此，因为它很容易泄漏。</t>
         </is>
       </c>
       <c r="E405" t="inlineStr">
@@ -14598,7 +14598,7 @@
       </c>
       <c r="D408" t="inlineStr">
         <is>
-          <t>一点也不坏，这个lint只是显示了可以添加属性的地方。</t>
+          <t>不错，这个lint只是显示了可以添加属性的地方。</t>
         </is>
       </c>
       <c r="E408" t="inlineStr">
@@ -15038,7 +15038,7 @@
       </c>
       <c r="D420" t="inlineStr">
         <is>
-          <t>这些繁忙的循环在不做任何事情的情况下消耗CPU周期。恐慌几乎总是一个更好的主意！如果恐慌是不可能的，考虑一下环境，要么：阻塞一些东西，让线程休眠几微秒，要么暂停线程。对于std目标，这可以承受：：thread:：sleep或std:：thread：：yield_now。对于no-std目标，这样做更复杂，尤其是因为#[pacil_handler]s不能恐慌。要停止/暂停线程，您可能需要调用一些特定于目标的内在函数。示例包括：x86_64:：instructions:：hltcortex_m:：asm:：wfi</t>
+          <t>这些繁忙的循环在不做任何事情的情况下消耗CPU周期。panic！几乎总是比有一个繁忙的循环更好的主意。如果恐慌是不可能的，考虑一下环境，要么：阻塞一些东西，让线程休眠几微秒，要么暂停线程。对于std目标，这可以在：thread:：sleep或std:：thread：：yield_now下完成。对于no-std目标，这样做更复杂，尤其是因为#[panic_handler]不会恐慌。要停止/暂停线程，您可能需要调用一些特定于目标的内在函数。示例包括：x86_64:：instructions:：hltcortex_m:：asm:：wfi</t>
         </is>
       </c>
       <c r="E420" t="inlineStr">
@@ -15698,12 +15698,12 @@
       </c>
       <c r="C439" t="inlineStr">
         <is>
-          <t>使用_检查通配符枚举匹配。</t>
+          <t>使用_检查通配符enum匹配项。</t>
         </is>
       </c>
       <c r="D439" t="inlineStr">
         <is>
-          <t>库更新添加的新枚举变体可能会丢失。</t>
+          <t>库更新添加的新enum变体可能会丢失。</t>
         </is>
       </c>
       <c r="E439" t="inlineStr">
@@ -15738,12 +15738,12 @@
       </c>
       <c r="C440" t="inlineStr">
         <is>
-          <t>检查单个变体的通配符枚举匹配项。</t>
+          <t>检查单个变体的通配符enum匹配项。</t>
         </is>
       </c>
       <c r="D440" t="inlineStr">
         <is>
-          <t>库更新添加的新枚举变体可能会丢失。</t>
+          <t>库更新添加的新enum变体可能会丢失。</t>
         </is>
       </c>
       <c r="E440" t="inlineStr">
@@ -15818,7 +15818,7 @@
       </c>
       <c r="C442" t="inlineStr">
         <is>
-          <t>检查用于销毁单个变量枚举元组结构的匹配项，其中let就足够了。</t>
+          <t>检查用于销毁单个变量枚举元组struct的匹配项，其中let就足够了。</t>
         </is>
       </c>
       <c r="D442" t="inlineStr">
@@ -15896,12 +15896,12 @@
       </c>
       <c r="C444" t="inlineStr">
         <is>
-          <t>检查是否存在不必要的“..”当所有字段都显式匹配时，结构上的模式绑定。</t>
+          <t>检查是否存在不必要的“..”当所有字段都显式匹配时，struct上的模式绑定。</t>
         </is>
       </c>
       <c r="D444" t="inlineStr">
         <is>
-          <t>正确性和可读性。这就像在显式匹配所有枚举变体后使用通配符模式一样。</t>
+          <t>正确性和可读性。这就像在显式匹配所有enum变体之后有一个通配符模式。</t>
         </is>
       </c>
       <c r="E444" t="inlineStr">
@@ -16115,7 +16115,7 @@
       </c>
       <c r="C449" t="inlineStr">
         <is>
-          <t>在不添加任何分支的情况下，查找模式可能“折叠”在一起的嵌套匹配或if let表达式。请注意，此lint并不是用于查找所有可以合并嵌套匹配模式的情况，而是仅用于合并最有可能使代码更可读的情况。</t>
+          <t>在不添加任何分支的情况下，查找模式可能“折叠”在一起的嵌套匹配或if let表达式。请注意，此lint并不是要查找所有可以合并嵌套匹配模式的情况，而是仅用于合并最有可能使代码更具可读性的情况。</t>
         </is>
       </c>
       <c r="D449" t="inlineStr">
@@ -16578,7 +16578,7 @@
       </c>
       <c r="D461" t="inlineStr">
         <is>
-          <t>最好处理None或Err的情况，或者至少调用.expect（_）并返回更有用的消息。尽管如此，对于许多快速且肮脏的代码，unwrap是一个不错的选择，这就是为什么这个lint默认为Allow.result.unwrap（）会让线程对Err值感到恐慌。通常，你想实现更复杂的错误处理，并用？操作员。即使你想对错误感到恐慌，也不是所有的错误都能在显示中实现好消息。因此，查看它们可能显示的位置可能是有益的。激活这个棉绒就可以做到这一点。</t>
+          <t>最好处理None或Err的情况，或者至少调用.expect（_）并返回更有用的消息。尽管如此，对于许多快速且肮脏的代码，unwrap是一个不错的选择，这就是为什么这个lint默认为Allow.result.unwrap（）会让线程对Err值感到恐慌。通常，你想实现更复杂的错误处理，并用向上传播错误？操作员。即使你想对错误感到恐慌，也不是所有的错误都能在显示中实现好消息。因此，查看它们可能显示的位置可能是有益的。激活此lint即可执行此操作。</t>
         </is>
       </c>
       <c r="E461" t="inlineStr">
@@ -16615,7 +16615,7 @@
       </c>
       <c r="D462" t="inlineStr">
         <is>
-          <t>通常最好处理None或Err的情况。不过，对于许多快速且脏的代码，expect是一个不错的选择，这就是为什么lint默认为Allow的原因。result.expect（）会让线程在Errvalues上死机。通常，您希望实现更复杂的错误处理，并使用向上传播错误？操作人员</t>
+          <t>通常最好处理None或Err的情况。不过，对于许多快速且肮脏的代码，expect是一个不错的选择，这就是为什么默认情况下lint为Allow。result.expect（）会让线程在Errvalues上死机。通常，您希望实现更复杂的错误处理，并使用向上传播错误？操作人员</t>
         </is>
       </c>
       <c r="E462" t="inlineStr">
@@ -16679,7 +16679,7 @@
       </c>
       <c r="C464" t="inlineStr">
         <is>
-          <t>检查具有特定名称前缀或后缀的方法，并且不遵守关于如何获取self的标准约定。实际规则为：|Prefix |Postfix |self-take|self-type||-------|--------------------------------------------||as_|none|&amp;self或&amp;mut-self|any|from_|none|none|any||into_|none|self|any||is_|none|&amp;mut-self或&amp;self或none|any|to_|_mut |&amp;mut-self|any|to_|not_mut |self|Copy||to_| not_mut |&amp;self|notCopy|注意：Clippy不会触发在：特征定义中带有to_前缀的方法trait是否为Copy。当采用&amp;self时，实现Traits。方法签名由trait控制，并且通常实现trait的所有类型都需要&amp;self（例如，请参阅std:：string:：ToString trait）。如果需要&amp;selve和&amp;mut self，Clippy允许Pin＜&amp;self＞和Pin＜&amp;mut self＞。请在此处查找更多信息：https://rust-lang.github.io/api-guidelines/naming.html#ad-hoc-conversions-follow-as-to-into-conventions-c-conv</t>
+          <t>检查具有特定名称前缀或后缀的方法，并且不遵守关于如何获取self的标准约定。实际规则为：|Prefix|Postfix|self-take|self-type||--------------------------------------------|------------------------------||as_|none|&amp;self或&amp;mut self|any||from_|none|any|into_|none|self|any|Copy||to_|not_mut|&amp;self|notCopy|注意：Clippy在：Traits定义中不触发带有to_前缀的方法。Clippy无法判断实现trait的类型是否为Copy。Traits实现，当使用&amp;self时。方法签名由trait控制，并且通常实现trait的所有类型都需要&amp;self（例如，请参见std:：string:：ToString trait）。如果需要&amp;selve和&amp;mut self，Clippy允许Pin＜&amp;self＞和Pin＜&amp;mut self＞。请在此处查找更多信息：https://rust-lang.github.io/api-guidelines/naming.html#ad-hoc-conversions-follow-as-to-into-conventions-c-conv</t>
         </is>
       </c>
       <c r="D464" t="inlineStr">
@@ -17728,7 +17728,7 @@
       </c>
       <c r="D495" t="inlineStr">
         <is>
-          <t>使用x.last（）更容易阅读，并且具有相同的结果。注意，使用x[x.len（）-1]在语义上与x.last。</t>
+          <t>使用x.last（）更容易阅读，并且具有相同的结果。请注意，使用x[x.len（）-1]在语义上与x.last。</t>
         </is>
       </c>
       <c r="E495" t="inlineStr">
@@ -18351,7 +18351,7 @@
       </c>
       <c r="C514" t="inlineStr">
         <is>
-          <t>作为or_fun_call的对应项，此lint在Option和Result上查找不必要的求值闭包。当在示例代码中得到急切的求值结果时，此linnt建议更改以下函数：unwrap_or_else到unwrap_orand_then到andor_other到orget_or_insert_with到get_or_inserterk_or_elsen到ok_orthen到then_some（对于msrv&gt;=1.62.0）</t>
+          <t>作为or_fun_call的对应项，此lint在Option和Result上查找不必要的求值闭包。当在简单代码中得到急切的求值结果时，此_lint建议更改以下函数：unwrap_or_else到unwrap_orand_then到andor_olset到orget_or_insert_with到get_or_inserterk_or_els到ok_orthen到then_some（对于msrv&gt;=1.62.0）</t>
         </is>
       </c>
       <c r="D514" t="inlineStr">
@@ -19284,7 +19284,7 @@
       </c>
       <c r="C542" t="inlineStr">
         <is>
-          <t>在Iterator或Option上检查map（|x|x.clone（））orderreference闭包对Copy类型的使用情况，并建议改用cloned（）或copied（）</t>
+          <t>在Iterator或Option上检查map（|x|x.clone（））ordereferencing闭包对Copy类型的使用情况，并建议改用cloned（）或copied（）</t>
         </is>
       </c>
       <c r="D542" t="inlineStr">
@@ -19323,7 +19323,7 @@
       </c>
       <c r="D543" t="inlineStr">
         <is>
-          <t>此map_err丢弃原始错误，而不允许枚举包含并报告错误原因</t>
+          <t>此map_err丢弃原始错误，而不允许enum包含并报告错误原因</t>
         </is>
       </c>
       <c r="E543" t="inlineStr">
@@ -19551,7 +19551,7 @@
       </c>
       <c r="C548" t="inlineStr">
         <is>
-          <t>检查重复（1）的用法，并为每种类型建议以下方法。。to_string（）for str.clone（）for string.to_vec（）for sliceLint将计算常量表达式和值作为.reeat（..）的参数，并在它们等于1时发出消息。（在锈夹子#7306中的相关讨论）</t>
+          <t>检查重复（1）的用法，并为每种类型建议以下方法。。to_string（）for str.clone（）for string。to_vec（）for slicelint将计算常量表达式和值作为.reeat（..）的参数，并在它们等于1时发出消息。（在锈夹子#7306中的相关讨论）</t>
         </is>
       </c>
       <c r="D548" t="inlineStr">
@@ -20510,7 +20510,7 @@
       </c>
       <c r="C576" t="inlineStr">
         <is>
-          <t>检查比较中是否存在不兼容的位掩码。可以从下表中确定用于检测类型为_&lt;bit_op&gt;m&lt;cmp_op&gt;c的表达式（其中&lt;bit_op&gt;是｛&amp;，|｝之一，&lt;cmp_oop&gt;是｛！=，&gt;=，&gt;，！=，&gt;&gt;｝之一）的公式：|Comparison|bit-op|示例|始终为|formula ||---------------|---------------|---------------|===或！=|&amp;|x&amp;2==3|false|c&amp;m！=c||&lt;或&gt;=|&amp;|x&amp;2&lt;3|true|m&lt;c||&gt;或&lt;=|&amp;| x&amp;1&gt;1|false|m&lt;=c||==或！=|\||x\|1==0|false|c\|m！=c||&lt;或&gt;=|\|x\|1&lt;1|false|m&gt;=c||&lt;=或&gt;||x\|1&gt;0|true|m&gt;c|</t>
+          <t>检查比较中是否存在不兼容的位掩码。可以从下表中确定用于检测类型为_&lt;bit_op&gt;m&lt;cmp_op&gt;c的表达式（其中&lt;bit_op&gt;是｛&amp;，|｝之一，&lt;cmp_oop&gt;是｛！=，&gt;=，&gt;，！=，&gt;&gt;｝之一）的公式：|比较|位操作|示例|始终为|公式||--------------|--------------|--------------------------------------------|===或！=|&amp;|x&amp;2==3|false|c&amp;m！=c||&lt;或&gt;=|&amp;|x&amp;2&lt;3|true|m&lt;c||&gt;或&lt;=|&amp;| x&amp;1&gt;1|false|m&lt;=c||==或！=|\||x\|1==0|false|c\|m！=c||&lt;或&gt;=|\|x\|1&lt;1|false|m&gt;=c||&lt;=或&gt;||x\|1&gt;0|true|m&gt;c|</t>
         </is>
       </c>
       <c r="D576" t="inlineStr">
@@ -21045,7 +21045,7 @@
       </c>
       <c r="D593" t="inlineStr">
         <is>
-          <t>位运算符不支持短路，因此可能会阻碍代码性能。此外，布尔逻辑“屏蔽”为位逻辑不会被unnecessary_fold等lint捕获</t>
+          <t>逐位运算符不支持短路，因此可能会阻碍代码性能。此外，布尔逻辑“屏蔽”为逐位逻辑不会被lints捕获，如unnecessary_fold</t>
         </is>
       </c>
       <c r="E593" t="inlineStr">
@@ -21747,7 +21747,7 @@
       </c>
       <c r="D615" t="inlineStr">
         <is>
-          <t>选项&lt;_&gt;表示一个可选值。Option＜Option＜_＞表示一个可选值，该值本身封装了一个可选。这在逻辑上与可选值相同，但有一个不必要的额外包装级别。如果您的案例中Some（Some（_））、Some（None）和None是不同的案例，请考虑使用自定义枚举，每个案例都有明确的名称。</t>
+          <t>选项&lt;_&gt;表示一个可选值。Option＜Option＜_＞表示一个可选值，该值本身封装了一个可选。这在逻辑上与可选值相同，但有一个不必要的额外包装级别。如果您的案例中Some（Some（_））、Some（None）和None是不同的案例，请考虑使用自定义enum，每个案例都有明确的名称。</t>
         </is>
       </c>
       <c r="E615" t="inlineStr">
@@ -22069,7 +22069,7 @@
       </c>
       <c r="C625" t="inlineStr">
         <is>
-          <t>array_into_iter lint检测在数组上调用into_ter。</t>
+          <t>array_into_iterlint检测在数组上调用into_ter。</t>
         </is>
       </c>
       <c r="D625" t="inlineStr">
@@ -22096,7 +22096,7 @@
       </c>
       <c r="C626" t="inlineStr">
         <is>
-          <t>while_true lint检测while为true｛｝。</t>
+          <t>while_truelint检测到while-true｛｝。</t>
         </is>
       </c>
       <c r="D626" t="inlineStr">
@@ -22123,12 +22123,12 @@
       </c>
       <c r="C627" t="inlineStr">
         <is>
-          <t>box_pointers lints使用box类型。</t>
+          <t>box_pointerslints使用box类型。</t>
         </is>
       </c>
       <c r="D627" t="inlineStr">
         <is>
-          <t>这种皮棉大多是历史性的，并不是特别有用。Box＜T＞曾经被内置到该语言中，也是进行堆分配的唯一方法。今天的Rust可以调用其他分配器等。</t>
+          <t>这个lint主要是历史性的，并不是特别有用。Box＜T＞曾经被内置到该语言中，也是进行堆分配的唯一方法。今天的Rust可以调用其他分配器等。</t>
         </is>
       </c>
       <c r="E627" t="inlineStr">
@@ -22152,7 +22152,7 @@
       </c>
       <c r="C628" t="inlineStr">
         <is>
-          <t>non_shorthand_field_patterns lint在模式中使用Struct｛x:x｝而不是Struct{x｝进行检测。</t>
+          <t>non_shorthand_field_patternslint检测到在模式中使用Struct｛x:x｝而不是Struct{x｝。</t>
         </is>
       </c>
       <c r="D628" t="inlineStr">
@@ -22190,12 +22190,12 @@
       </c>
       <c r="C629" t="inlineStr">
         <is>
-          <t>unsafecode lint捕获不安全代码的使用。</t>
+          <t>unsafecodelint捕获不安全代码的使用。</t>
         </is>
       </c>
       <c r="D629" t="inlineStr">
         <is>
-          <t>这种棉绒旨在限制不安全的使用，这可能会使正确使用变得困难。</t>
+          <t>此lint旨在限制不安全的使用，这可能会使正确使用变得困难。</t>
         </is>
       </c>
       <c r="E629" t="inlineStr">
@@ -22220,12 +22220,12 @@
       </c>
       <c r="C630" t="inlineStr">
         <is>
-          <t>missing_docs lint检测到公共项目缺少文档。</t>
+          <t>missing_docslint检测到公共项目缺少文档。</t>
         </is>
       </c>
       <c r="D630" t="inlineStr">
         <is>
-          <t>此lint旨在确保库具有良好的文档。没有文档的项目可能很难让用户理解如何正确使用。此lint默认为“允许”，因为它可能会发出噪音，并且并非所有项目都希望强制所有内容都要文档化。</t>
+          <t>此lint旨在确保库具有良好的文档。没有文档的项目可能很难让用户理解如何正确使用。默认情况下，此linet是“允许”的，因为它可能很嘈杂，并且并非所有项目都希望强制所有内容都有文档。</t>
         </is>
       </c>
       <c r="E630" t="inlineStr">
@@ -22247,12 +22247,12 @@
       </c>
       <c r="C631" t="inlineStr">
         <is>
-          <t>missing_copy_implementations lint检测公共类型可能放弃的copy实现。</t>
+          <t>missing_copy_implementationslint检测到公共类型可能放弃的copy实现。</t>
         </is>
       </c>
       <c r="D631" t="inlineStr">
         <is>
-          <t>历史上（在1.0之前），如果可能的话，类型会自动标记为Copy。这一点已经改变，因此它需要一个明确的选择加入来实现复制特性。作为此更改的一部分，如果可复制类型没有标记为Copy，则添加了一个lint以提醒。此lint默认为“允许”，因为此代码还不错；通常会专门编写这样的新类型，这样Copy类型就不再是Copy了。复制类型可能会导致意外复制大数据，从而影响性能。</t>
+          <t>历史上（在1.0之前），如果可能的话，类型会自动标记为Copy。这一点已经改变，因此它需要一个明确的选择加入来实现复制特性。作为此更改的一部分，如果可复制类型未标记为Copy，则添加了一个lint以发出警报。默认情况下，此linnt为“允许”，因为此代码还不错；通常会专门编写这样的新类型，这样Copy类型就不再是Copy了。复制类型可能会导致意外复制大数据，从而影响性能。</t>
         </is>
       </c>
       <c r="E631" t="inlineStr">
@@ -22305,12 +22305,12 @@
       </c>
       <c r="C633" t="inlineStr">
         <is>
-          <t>anonymous_parameters lint检测训练定义中的匿名参数。</t>
+          <t>匿名参数lint检测训练定义中的匿名参数。</t>
         </is>
       </c>
       <c r="D633" t="inlineStr">
         <is>
-          <t>这种语法大多是历史上的意外，可以通过添加_模式或描述性标识符来轻松解决：trait Foo｛fn Foo（_:usize）；｝这种语法现在在2018版中是一个严重错误。在2015版中，此lint默认为“警告”。此Lint使带有--edition标志的货物修复工具能够自动将旧代码从2015版转换到2018版。该工具将运行此lint并自动应用编译器建议的修复程序（即向每个参数添加_）。这提供了一种完全自动化的方式来为新版本更新旧代码。有关更多详细信息，请参阅第41686期。</t>
+          <t>这种语法大多是历史上的意外，可以通过添加_模式或描述性标识符来轻松解决：trait Foo｛fnFoo（_:usize）；｝这种语法现在在2018版中是一个严重错误。在2015版中，默认情况下，此lint为“警告”。此Lint使带有--edition标志的carge修复工具能够自动将旧代码从2015版转换到2018版。该工具将运行此lint并自动应用编译器建议的修复程序（即向每个参数添加_）。这提供了一种完全自动化的方式来为新版本更新旧代码。有关更多详细信息，请参阅第41686期。</t>
         </is>
       </c>
       <c r="E633" t="inlineStr">
@@ -22336,7 +22336,7 @@
       </c>
       <c r="C634" t="inlineStr">
         <is>
-          <t>no_mangle_const_items lint检测具有no_mangle属性的任何常量项。</t>
+          <t>no_mangle_const_itemslint检测具有no_mangle属性的任何常量项。</t>
         </is>
       </c>
       <c r="D634" t="inlineStr">
@@ -22363,7 +22363,7 @@
       </c>
       <c r="C635" t="inlineStr">
         <is>
-          <t>no_mangle_generic_items lint检测必须混淆的泛型项。</t>
+          <t>no_mangle_generic_itemslint检测必须混淆的泛型项。</t>
         </is>
       </c>
       <c r="D635" t="inlineStr">
@@ -22391,7 +22391,7 @@
       </c>
       <c r="C636" t="inlineStr">
         <is>
-          <t>mutable_transmutes lint捕获从&amp;T转换为&amp;mut T的过程，因为这是未定义的行为。</t>
+          <t>mutable_transmuteslint捕获了从&amp;T到&amp;mut T的转换，因为这是未定义的行为。</t>
         </is>
       </c>
       <c r="D636" t="inlineStr">
@@ -22437,7 +22437,7 @@
       </c>
       <c r="C638" t="inlineStr">
         <is>
-          <t>当在异步函数、方法或闭包上使用#[track_caller]属性，而没有启用相应的不稳定功能标志时，unsted_async_fn_track_caller lint会发出警告。</t>
+          <t>当#[track_caller]属性用于async函数、方法或闭包时，unsted_async_fn_track_callerlint会发出警告，而不会启用相应的不稳定功能标志。</t>
         </is>
       </c>
       <c r="D638" t="inlineStr">
@@ -22464,12 +22464,12 @@
       </c>
       <c r="C639" t="inlineStr">
         <is>
-          <t>无法从机箱根目录访问pub项目的unreachable_pub lint触发器。</t>
+          <t>无法从crate根访问的pub项目的unreachable_publint触发器。</t>
         </is>
       </c>
       <c r="D639" t="inlineStr">
         <is>
-          <t>如果商品实际上不是从板条箱中公开出口的，那么裸露的酒吧可见性可能会产生误导。建议使用pub（板条箱）可见性，这更清楚地表达了物品只在自己的板条箱中可见的意图。该lint默认为“允许”，因为它会触发大量现有的Rust代码，并且有一些误报。最终，它希望在默认情况下成为警告。</t>
+          <t>如果商品实际上不是从板条箱中公开出口的，那么裸露的酒吧可见性可能会产生误导。建议使用pub（板条箱）可见性，这更清楚地表达了物品只在自己的板条箱中可见的意图。默认情况下，这个lint是“允许”的，因为它会触发大量现有的Rust代码，并且有一些误报。最终，它希望在默认情况下成为警告。</t>
         </is>
       </c>
       <c r="E639" t="inlineStr">
@@ -22494,7 +22494,7 @@
       </c>
       <c r="C640" t="inlineStr">
         <is>
-          <t>type_alias_bounds lint检测类型别名中的边界。</t>
+          <t>type_alias_boundslint检测类型别名中的边界。</t>
         </is>
       </c>
       <c r="D640" t="inlineStr">
@@ -22520,7 +22520,7 @@
       </c>
       <c r="C641" t="inlineStr">
         <is>
-          <t>平凡边界lint检测不依赖于任何类型参数的特征边界。</t>
+          <t>trivial_boundslint检测不依赖于任何类型参数的特征边界。</t>
         </is>
       </c>
       <c r="D641" t="inlineStr">
@@ -22547,7 +22547,7 @@
       </c>
       <c r="C642" t="inlineStr">
         <is>
-          <t>ellipsis_inclusive_range_patterns lint检测到。。。rangepattern，已弃用。</t>
+          <t>ellipsis_inclusive_range_patternslint检测。。。rangepattern，已弃用。</t>
         </is>
       </c>
       <c r="D642" t="inlineStr">
@@ -22577,12 +22577,12 @@
       </c>
       <c r="C643" t="inlineStr">
         <is>
-          <t>unnameable_test_items lint检测#[test]函数，这些函数无法由测试线束运行，因为它们位于不可命名的位置。</t>
+          <t>unnameable_test_itemslint检测#[test]函数，这些函数无法由测试线束运行，因为它们位于不可命名的位置。</t>
         </is>
       </c>
       <c r="D643" t="inlineStr">
         <is>
-          <t>为了让测试线束运行测试，测试函数必须位于可以从机箱根访问的位置。这通常意味着它必须在模块中定义，而不是在其他任何地方，例如在另一个函数中。编译器以前允许这样做而没有错误，因此添加了一个lint作为没有使用测试的警告。这是否应该被允许还没有决定，请参阅RFC 2471和问题#36629。</t>
+          <t>为了让测试线束运行测试，测试函数必须位于可以从crate根访问的位置。这通常意味着它必须在模块中定义，而不是在其他任何位置定义，例如在另一个函数中。编译器以前允许这样做而没有出现错误，因此添加了lint作为没有使用测试的警告。这是否应该被允许还没有决定，请参阅RFC 2471和问题#36629。</t>
         </is>
       </c>
       <c r="E643" t="inlineStr">
@@ -22609,12 +22609,12 @@
       </c>
       <c r="C644" t="inlineStr">
         <is>
-          <t>keyword_idents lint检测用作标识符的版本关键字。</t>
+          <t>关键字word_identslint检测用作标识符的版本关键字。</t>
         </is>
       </c>
       <c r="D644" t="inlineStr">
         <is>
-          <t>Rust版本允许语言在不破坏向后兼容性的情况下进行发展。这个lint捕获使用新关键字的代码，这些关键字被添加到用作标识符的语言中（如可用名称、函数名称等）。如果你在不更新代码的情况下将编译器切换到新版本，那么如果你使用新关键字作为标识符，它将无法编译。你可以手动将标识符更改为非关键字，或者使用araw标识符，例如r#dyn，转换到新版本。这个lint自动解决了问题。默认情况下它是“允许”的，因为代码在旧版本中完全有效。带有--edition标志的货物修复工具将把这个lint切换到“warn”，并自动应用编译器建议的修复（它将使用原始标识符）。这提供了一种为新版本更新旧代码的完全自动化的方式。</t>
+          <t>Rust版本允许语言在不破坏向后兼容性的情况下进行发展。此lint捕获使用新关键字的代码，这些关键字将添加到用作标识符的语言中（如可用名称、函数名称等）。如果您在不更新代码的情况下将编译器切换到新版本，则如果您使用新关键字作为标识符，则它将无法编译。您可以手动将标识符更改为非关键字，或使用新标识符，例如r#dyn，转换到新版本。这lint自动解决了问题。默认情况下它是“允许”的，因为代码在旧版本中完全有效。带有--edition标志的carge修复工具将把这个lint切换到“警告”，并自动应用编译器建议的修复（它将使用原始标识符）。这提供了一种为新版本更新旧代码的完全自动化的方式。</t>
         </is>
       </c>
       <c r="E644" t="inlineStr">
@@ -22637,7 +22637,7 @@
       </c>
       <c r="C645" t="inlineStr">
         <is>
-          <t>不完整_功能lint检测使用功能属性启用的不稳定功能，这些功能在某些或所有情况下可能无法正常工作。</t>
+          <t>不完整功能lint检测到使用功能属性启用的不稳定功能，这些功能在某些或所有情况下可能无法正常工作。</t>
         </is>
       </c>
       <c r="D645" t="inlineStr">
@@ -22663,12 +22663,12 @@
       </c>
       <c r="C646" t="inlineStr">
         <is>
-          <t>invalid_value lint检测创建的值无效，例如null引用。</t>
+          <t>invalid_valuelint检测创建的值无效，例如null引用。</t>
         </is>
       </c>
       <c r="D646" t="inlineStr">
         <is>
-          <t>在某些情况下，编译器可以检测到代码创建了一个无效值，这应该避免。特别是，此lint将检查是否使用了可能导致未定义行为的mem:：zered、mem:：uninitialized、mem：：transmite和MaybeUninit:：assume_init。lint应该提供额外的信息来说明问题所在以及可能的解决方案。</t>
+          <t>在某些情况下，编译器可以检测到代码正在创建一个无效值，这应该避免。特别是，此lint将检查是否不正确使用了可能导致未定义行为的mem:：zered、mem:：uninitialized、mem：：transmite和MaybeUninit:：assume_init。lint应该提供额外的信息来说明问题所在以及可能的解决方案。</t>
         </is>
       </c>
       <c r="E646" t="inlineStr">
@@ -22692,12 +22692,12 @@
       </c>
       <c r="C647" t="inlineStr">
         <is>
-          <t>当使用相同名称但不同类型声明外部fn时，clashing_extern_declarations lint会检测到。</t>
+          <t>clashing_extern_declarationslint检测何时使用相同名称但不同类型声明了外部fn。</t>
         </is>
       </c>
       <c r="D647" t="inlineStr">
         <is>
-          <t>由于同一名称的两个符号在链接时无法解析为两个不同的函数，并且一个函数不可能具有两种类型，因此几乎可以肯定，使用冲突的外部声明是错误的。检查以确保外部定义是正确和等效的，并可能考虑将它们统一在一个位置。此lint不会在板条箱之间运行，因为一个项目可能具有依赖项，它们都依赖于相同的外部函数，但以不同的（但有效的）方式解密。例如，它们既可以为一个或多个参数声明不透明类型（这将结束更新类型），也可以使用在定义extern fn的语言中有效转换的类型。在这些情况下，编译器不会说冲突声明是不正确的。</t>
+          <t>由于同一名称的两个符号在链接时无法解析为两个不同的函数，并且一个函数不可能具有两种类型，因此几乎可以肯定，使用冲突的外部声明是错误的。检查以确保外部定义是正确和等效的，并可能考虑将它们统一在一个位置。此lint不会在crates之间运行，因为项目可能具有依赖项，它们都依赖于相同的外部函数，但以不同的（但有效的）方式解密。例如，它们既可以为一个或多个参数声明不透明类型（这将结束更新类型），也可以使用在定义externfn的语言中有效转换的类型。在这些情况下，编译器不会说冲突声明是不正确的。</t>
         </is>
       </c>
       <c r="E647" t="inlineStr">
@@ -22725,7 +22725,7 @@
       </c>
       <c r="C648" t="inlineStr">
         <is>
-          <t>deref_nullptr lint检测何时取消引用空指针，这会导致未定义的行为。</t>
+          <t>deref_nullptrlint检测何时取消引用空指针，这会导致未定义的行为。</t>
         </is>
       </c>
       <c r="D648" t="inlineStr">
@@ -22757,7 +22757,7 @@
       </c>
       <c r="C649" t="inlineStr">
         <is>
-          <t>named_asm_labels lint检测到在线asm中使用了命名标签！宏。</t>
+          <t>named_asm_labelslint检测到在线asm中使用了命名标签！宏。</t>
         </is>
       </c>
       <c r="D649" t="inlineStr">
@@ -22789,12 +22789,12 @@
       </c>
       <c r="C650" t="inlineStr">
         <is>
-          <t>special_module_name lint检测具有特殊意义的文件的模块声明。</t>
+          <t>special_module_namelint检测具有特殊含义的文件的模块声明。</t>
         </is>
       </c>
       <c r="D650" t="inlineStr">
         <is>
-          <t>Cargo将lib.rs和main.rs识别为alibrary或二进制机箱的根，因此除非配置正确，否则将它们声明为模块将导致机箱编译错误。要从同一机箱内的二进制目标访问库，使用your_crate_name:：作为路径，而不是lib:：//bar/src/lib.rsfn run（）｛//…｝//bar/src/main.rsfn main（）｛bar:：run（）；｝二进制目标不能用作库，因此不允许将declarginone作为模块。</t>
+          <t>Cargo将lib.rs和main.rs识别为alibrary或二进制机箱的根，因此除非进行了正确配置，否则将它们声明为模块将导致crate的编译错误。要从同一机箱内的二进制目标访问库，使用your_crate_name:：作为路径，而不是lib:：//bar/src/lib.rsfn run（）｛//…｝//bar/src/main.rsfn main（）｛bar:：run（）；｝二进制目标不能用作库，因此不允许将declarginone作为模块。</t>
         </is>
       </c>
       <c r="E650" t="inlineStr">
@@ -22818,7 +22818,7 @@
       </c>
       <c r="C651" t="inlineStr">
         <is>
-          <t>每当使用dyn supertrait类型为output的deref实现时，就会输出deref_into_dyn_suptrait lint。当trait_upcasting功能稳定时，这些实现将变为阴影。deref函数将不再被隐式调用，因此可能会发生行为更改。</t>
+          <t>只要使用dyn supertrait类型为output的deref实现，就会输出deref_into_dyn_suptraitlint。当trait_upcasting功能稳定时，这些实现将变为阴影。deref函数将不再被隐式调用，因此可能会发生行为更改。</t>
         </is>
       </c>
       <c r="D651" t="inlineStr">
@@ -22858,7 +22858,7 @@
       </c>
       <c r="C652" t="inlineStr">
         <is>
-          <t>dropping_references lint检查对std：：mem：：drop的调用是否带有一个所属值的referenceinstead。</t>
+          <t>dropping_referenceslint检查对std:：mem:：drop的调用是否具有所属值的referenceinstead。</t>
         </is>
       </c>
       <c r="D652" t="inlineStr">
@@ -22889,7 +22889,7 @@
       </c>
       <c r="C653" t="inlineStr">
         <is>
-          <t>forgeting_references lint检查对std：：mem：：forget的调用是否带有一个所属值的referenceinstead。</t>
+          <t>forgetting_referenceslint检查对std：：mem：：forget的调用是否带有所属值的referenceinstead。</t>
         </is>
       </c>
       <c r="D653" t="inlineStr">
@@ -22916,7 +22916,7 @@
       </c>
       <c r="C654" t="inlineStr">
         <is>
-          <t>dropping_copy_types lint检查对std:：mem:：drop的调用是否具有派生copy特性的值。</t>
+          <t>dropping_copy_typeslint检查对std:：mem:：drop的调用是否具有派生copy特性的值。</t>
         </is>
       </c>
       <c r="D654" t="inlineStr">
@@ -22944,7 +22944,7 @@
       </c>
       <c r="C655" t="inlineStr">
         <is>
-          <t>forgeting_copy_types lint检查对std:：mem:：forget的调用，该调用的值派生copy特性。</t>
+          <t>forgetting_copy_typeslint使用派生copy特性的值来检查对std:：mem:：forget的调用。</t>
         </is>
       </c>
       <c r="D655" t="inlineStr">
@@ -22972,12 +22972,12 @@
       </c>
       <c r="C656" t="inlineStr">
         <is>
-          <t>enum_intrinsics_non_enums-lint检测对需要枚举（core:：mem:：differential，core:：mem:：variant_count）但使用非枚举类型调用的intrinsic函数的调用。</t>
+          <t>enum_intrinsics_non_enumslint检测对需要enum（core:：mem:：differential，core:：mem:：variant_count）但使用非枚举类型调用的intrinsic函数的调用。</t>
         </is>
       </c>
       <c r="D656" t="inlineStr">
         <is>
-          <t>为了接受任何枚举，mem:：differential和mem:：variant_count函数在类型T上是泛型的。这使得T在技术上可以是非枚举，在这种情况下返回值是未指定的。此lint可以防止这些函数的错误使用。</t>
+          <t>为了接受任何枚举，mem:：differential和mem:：variant_count函数在类型T上是泛型的。这使得T在技术上可以是非枚举，在这种情况下返回值是未指定的。这lint防止了这些函数的错误使用。</t>
         </is>
       </c>
       <c r="E656" t="inlineStr">
@@ -22999,7 +22999,7 @@
       </c>
       <c r="C657" t="inlineStr">
         <is>
-          <t>for_loops_over_fallibles lint检查Option或Result值上的循环。</t>
+          <t>for_loops_over_fallibleslint检查Option或Result值上的循环。</t>
         </is>
       </c>
       <c r="D657" t="inlineStr">
@@ -23026,12 +23026,12 @@
       </c>
       <c r="C658" t="inlineStr">
         <is>
-          <t>text_direction_codepoint_in_litrial lint检测Unicode代码点，这些代码点以与内存表示不一致的方式更改屏幕上文本的视觉表示。</t>
+          <t>text_direction_codepoint_in_litriallint检测Unicode代码点，这些代码点以与内存表示不一致的方式更改屏幕上文本的视觉表示。</t>
         </is>
       </c>
       <c r="D658" t="inlineStr">
         <is>
-          <t>unicode字符\u 202A｝、\u 202B｝、/u 202D｝、\u 202E｝、\ u 2066｝、\\u 2067｝、\\ u 2068｝、%u 202C｝和\u 2069｝使屏幕上的文本流在支持这些代码点的软件上改变了方向。这使得文本“abc”在屏幕上显示为“cba”。通过利用支持这些功能的软件，人们可以编写专门编写的文字，使周围的代码看起来像是在执行一个动作，而实际上它正在执行另一个动作。正因为如此，我们主动抵制他们的出现，以避免意外。</t>
+          <t>unicode字符\u 202A｝、\u 202B｝、/u 202D｝、\u 202E｝、\ u 2066｝、\\u 2067｝、\\ u 2068｝、%u 202C｝和\u 2069｝使屏幕上的文本流在支持这些代码点的软件上改变了方向。这使得文本“abc”在屏幕上显示为“cba”。通过利用支持这些功能的软件，人们可以编写专门编写的文字，使周围的代码看起来像是在执行一个动作，而实际上它正在执行另一个动作。正因为如此，我们主动lint反对他们的存在，以避免意外。</t>
         </is>
       </c>
       <c r="E658" t="inlineStr">
@@ -23055,7 +23055,7 @@
       </c>
       <c r="C659" t="inlineStr">
         <is>
-          <t>let_underscore_drop-lint检查那些不将具有非平凡drop实现的表达式绑定到任何内容的语句，从而导致表达式立即被丢弃，而不是在作用域结束时。</t>
+          <t>let_underscore_droplint检查那些没有将具有非平凡drop实现的表达式绑定到任何内容的语句，从而导致该表达式立即被丢弃，而不是在作用域结束时。</t>
         </is>
       </c>
       <c r="D659" t="inlineStr">
@@ -23095,7 +23095,7 @@
       </c>
       <c r="C660" t="inlineStr">
         <is>
-          <t>let_underscore_lock lint检查那些没有将互斥锁绑定到任何东西的语句，导致锁在作用域结束时立即释放，这通常是不正确的。</t>
+          <t>let_underscore_locklint检查不将互斥锁绑定到任何东西的语句，导致锁立即释放，而不是在作用域结束时释放，这通常是不正确的。</t>
         </is>
       </c>
       <c r="D660" t="inlineStr">
@@ -23131,7 +23131,7 @@
       </c>
       <c r="C661" t="inlineStr">
         <is>
-          <t>map_unit_fn lint检查Iterator:：map是否接收到返回（）的可调用项。</t>
+          <t>map_unit_fnlint检查Iterator:：map是否接收到返回（）的可调用项。</t>
         </is>
       </c>
       <c r="D661" t="inlineStr">
@@ -23166,7 +23166,7 @@
       </c>
       <c r="C662" t="inlineStr">
         <is>
-          <t>temporary_cstring_as_ptr lint检测是否获取临时cstring的内部指针。</t>
+          <t>temporary_cstring_as_ptrlint检测是否获取临时cstring的内部指针。</t>
         </is>
       </c>
       <c r="D662" t="inlineStr">
@@ -23194,12 +23194,12 @@
       </c>
       <c r="C663" t="inlineStr">
         <is>
-          <t>multiple_superstrait_upplast lint检测对象安全特性何时具有多个超级特性。</t>
+          <t>multiple_superstrait_upplastlint检测对象安全特征何时具有多个超级特征。</t>
         </is>
       </c>
       <c r="D663" t="inlineStr">
         <is>
-          <t>为了支持具有多个超特性的上行，我们需要存储多个vtable，这可能会导致额外的空间开销，即使没有代码实际使用上行。这个lint允许用户识别何时发生这种情况，并决定额外的开销是否合理。</t>
+          <t>为了支持具有多个超特性的上行，我们需要存储多个vtable，这可能会导致额外的空间开销，即使没有代码实际使用上行。这lint允许用户识别此类场景何时发生，并决定额外的开销是否合理。</t>
         </is>
       </c>
       <c r="E663" t="inlineStr">
@@ -23223,7 +23223,7 @@
       </c>
       <c r="C664" t="inlineStr">
         <is>
-          <t>non_camel_case_types lint检测没有camel大小写名称的类型、变体、特征和类型参数。</t>
+          <t>non_camel_case_typeslint检测没有camel大小写名称的类型、变体、特征和类型参数。</t>
         </is>
       </c>
       <c r="D664" t="inlineStr">
@@ -23249,7 +23249,7 @@
       </c>
       <c r="C665" t="inlineStr">
         <is>
-          <t>non_snake_case lint检测没有snake大小写名称的变量、方法、函数、生存期参数和模块。</t>
+          <t>non_snake_caselint检测没有snake大小写名称的变量、方法、函数、生存期参数和模块。</t>
         </is>
       </c>
       <c r="D665" t="inlineStr">
@@ -23275,7 +23275,7 @@
       </c>
       <c r="C666" t="inlineStr">
         <is>
-          <t>non_upper_case_globals lint检测没有大写标识符的静态项。</t>
+          <t>non_upper_case_globalslint检测没有大写标识符的静态项。</t>
         </is>
       </c>
       <c r="D666" t="inlineStr">
@@ -23301,12 +23301,12 @@
       </c>
       <c r="C667" t="inlineStr">
         <is>
-          <t>non_ascii_identits lint检测非ascii标识符。</t>
+          <t>non_ascii_identitslint检测非ascii标识符。</t>
         </is>
       </c>
       <c r="D667" t="inlineStr">
         <is>
-          <t>此lint允许希望保留仅使用ASCII字符的限制的项目将此lint切换为“禁止”（例如，为了便于协作或出于安全原因）。有关更多详细信息，请参阅RFC 2457。</t>
+          <t>此lint允许希望保留仅使用ASCII字符的限制的项目将此linet切换为“禁止”（例如，为了便于协作或出于安全原因）。有关更多详细信息，请参阅RFC 2457。</t>
         </is>
       </c>
       <c r="E667" t="inlineStr">
@@ -23331,12 +23331,12 @@
       </c>
       <c r="C668" t="inlineStr">
         <is>
-          <t>uncommon_cdepoints lint在标识符中检测到不常见的Unicode代码点。</t>
+          <t>uncommon_cdepointslint在标识符中检测到不常见的Unicode代码点。</t>
         </is>
       </c>
       <c r="D668" t="inlineStr">
         <is>
-          <t>该lint警告不要使用不常用的字符，和可能导致视觉混乱。此lint是由包含不属于Unicode®技术标准#39 Unicode安全机制第3.1节标识符的通用安全配置文件所述的“允许”代码点集的代码点的标识符触发的。请注意，不常见代码点集可能会随时间变化。请注意，如果你“禁止”这个lint，那么现有的代码将来可能会失败。</t>
+          <t>此lint警告不要使用不常用的字符，并且可能导致视觉混乱。此lint是由包含不属于Unicode®技术标准#39 Unicode安全机制第3.1节标识符的通用安全配置文件所述的“允许”代码点集的代码点的标识符触发的。请注意，不常见代码点集可能会随时间变化。请注意，如果你“禁止”这个lint，那么现有的代码将来可能会失败。</t>
         </is>
       </c>
       <c r="E668" t="inlineStr">
@@ -23358,12 +23358,12 @@
       </c>
       <c r="C669" t="inlineStr">
         <is>
-          <t>confusable_idents lint检测标识符之间视觉上可混淆的对。</t>
+          <t>可混淆的标识符lint检测标识符之间视觉上可混淆的对。</t>
         </is>
       </c>
       <c r="D669" t="inlineStr">
         <is>
-          <t>当不同的标识符在视觉上可能相似时，此lint会发出警告，这可能会导致混淆。可混淆检测算法基于Unicode®技术标准#39 Unicode安全机制第4节可混淆检测。对于每个不同的标识符X，执行函数骨架（X）。如果在同一个机箱中存在两个不同的标识符Xan和Y，其中skeleton（X）=skeleton。</t>
+          <t>当不同的标识符可能在视觉上看起来相似时，会发出警告，这可能会导致混淆。可混淆检测算法基于Unicode®技术标准#39 Unicode安全机制第4节可混淆检测。对于每个不同的标识符X，执行函数骨架（X）。如果在同一个crate中存在两个不同的标识符Xan和Y，其中skeleton（X）=skeleton。</t>
         </is>
       </c>
       <c r="E669" t="inlineStr">
@@ -23387,12 +23387,12 @@
       </c>
       <c r="C670" t="inlineStr">
         <is>
-          <t>mixed_script_confusables lint检测不同脚本之间标识符中视觉上可混淆的字符。</t>
+          <t>mixed_script_confusableslint检测不同脚本之间标识符中视觉上可混淆的字符。</t>
         </is>
       </c>
       <c r="D670" t="inlineStr">
         <is>
-          <t>当不同脚本之间的字符看起来可能相似时，此lint会发出警告，这可能会导致混淆。如果板条箱在同一脚本中包含具有不可混淆字符的其他标识符，则不会发出此lint。例如，如果上面给出的例子有另一个带有片假名字符的标识符（例如letカタカナ = 123；），那么这表明你有意使用片假名，它不会对此发出警告。注意，易混淆的字符集可能会随着时间的推移而变化。注意，如果你“禁止”这个lint，现有的代码将来可能会失败。</t>
+          <t>当不同脚本之间的字符看起来可能相似时，此lint会发出警告，这可能会导致混淆。如果crate在同一脚本中包含具有不可混淆字符的其他标识符，则不会发出此linet。例如，如果上面给出的例子有另一个带有片假名字符的标识符（例如letカタカナ = 123；），那么这表明你有意使用片假名，它不会对此发出警告。注意，易混淆的字符集可能会随着时间的推移而变化。注意，如果你“禁止”这个lint，那么现有的代码将来可能会失败。</t>
         </is>
       </c>
       <c r="E670" t="inlineStr">
@@ -23414,7 +23414,7 @@
       </c>
       <c r="C671" t="inlineStr">
         <is>
-          <t>non_fmt_panics lint检测到死机！（..）调用，其中第一个参数不是格式化字符串。</t>
+          <t>non_fmt_panicslint检测到死机！（..）调用，其中第一个参数不是格式化字符串。</t>
         </is>
       </c>
       <c r="D671" t="inlineStr">
@@ -23441,12 +23441,12 @@
       </c>
       <c r="C672" t="inlineStr">
         <is>
-          <t>noop_method_call lint检测对noop方法的特定调用，将其作为调用&lt;&amp;T as Clone&gt;：：Clone，其中T:！克隆</t>
+          <t>noop_method_calllint检测对noop方法的特定调用，将其作为调用&lt;&amp;T as Clone&gt;：：Clone，其中T:！克隆</t>
         </is>
       </c>
       <c r="D672" t="inlineStr">
         <is>
-          <t>有些方法调用是noop，这意味着它们什么都不做。通常，这样的方法是一揽子实现的结果，这些实现碰巧创建了一些方法调用，但最终什么都不做。例如，克隆在所有&amp;T上都实现了，但在一个&amp;T上调用克隆，其中T没有实现克隆，实际上什么都不做，因为引用是复制的。此lint检测到这些呼叫并向用户发出警告。</t>
+          <t>有些方法调用是noop，这意味着它们什么都不做。通常，这样的方法是一揽子实现的结果，这些实现碰巧创建了一些方法调用，但最终什么都不做。例如，克隆在所有&amp;T上都实现了，但在一个&amp;T上调用克隆，其中T没有实现克隆，实际上什么都不做，因为引用是复制的。此lint检测到这些调用并向用户发出警告。</t>
         </is>
       </c>
       <c r="E672" t="inlineStr">
@@ -23500,12 +23500,12 @@
       </c>
       <c r="C674" t="inlineStr">
         <is>
-          <t>opaque_hidden_inferred_bound lint检测关联类型边界中的nestedimpl Trait通常未被写入以满足关联类型的边界的情况。</t>
+          <t>opaque_hidden_inferred_boundlint检测关联类型边界中的nestedimpl Trait通常未被写入以满足关联类型的边界的情况。</t>
         </is>
       </c>
       <c r="D674" t="inlineStr">
         <is>
-          <t>这个功能在#97346中被删除，但后来在#99860中被回滚，因为它导致了倒退。我们计划将其作为一个硬错误重新引入，但同时，这个lint可以警告并建议修复任何依赖此行为的用例。</t>
+          <t>该功能在#97346中被删除，但随后在#99860中被回滚，因为它导致了倒退。我们计划将其作为一个硬错误重新引入，但同时，该lint用于警告并建议修复依赖该行为的任何用例。</t>
         </is>
       </c>
       <c r="E674" t="inlineStr">
@@ -23545,7 +23545,7 @@
       </c>
       <c r="C675" t="inlineStr">
         <is>
-          <t>redundant_name分号lint检测不必要的trailing分号。</t>
+          <t>冗余分号lint检测不必要的跟踪分号。</t>
         </is>
       </c>
       <c r="D675" t="inlineStr">
@@ -23571,7 +23571,7 @@
       </c>
       <c r="C676" t="inlineStr">
         <is>
-          <t>drop_bounds lint使用std:：ops:：drop-asbounds检查泛型。</t>
+          <t>drop_boundslint检查std:：ops:：drop-asbounds的泛型。</t>
         </is>
       </c>
       <c r="D676" t="inlineStr">
@@ -23597,7 +23597,7 @@
       </c>
       <c r="C677" t="inlineStr">
         <is>
-          <t>dyn_drop lint使用std:：ops:：drop检查trait对象。</t>
+          <t>dyn_droplint使用std:：ops:：drop检查trait对象。</t>
         </is>
       </c>
       <c r="D677" t="inlineStr">
@@ -23623,7 +23623,7 @@
       </c>
       <c r="C678" t="inlineStr">
         <is>
-          <t>unused_comparisons lint检测由于所涉及类型的限制而变得无用的比较。</t>
+          <t>unused_comparisonslint检测由于所涉及类型的限制而变得无用的比较。</t>
         </is>
       </c>
       <c r="D678" t="inlineStr">
@@ -23651,7 +23651,7 @@
       </c>
       <c r="C679" t="inlineStr">
         <is>
-          <t>overlowing_literals lint检测到其类型的文字超出范围。</t>
+          <t>overrowing_literalslint检测到文本超出了其类型的范围。</t>
         </is>
       </c>
       <c r="D679" t="inlineStr">
@@ -23677,12 +23677,12 @@
       </c>
       <c r="C680" t="inlineStr">
         <is>
-          <t>variant_size_differences lint检测具有广泛变化的变量大小的枚举。</t>
+          <t>variant_size_differenceslint检测具有广泛变化的变量大小的枚举。</t>
         </is>
       </c>
       <c r="D680" t="inlineStr">
         <is>
-          <t>将一个变体添加到比其他变体大得多的枚举中可能是错误的，这会使所有变体所需的总体大小膨胀。这可能会影响性能和内存使用率。如果一个变量比第二大变量大3倍以上，就会触发这种情况。可以考虑将大变量的内容放在堆上（例如，levia Box），以保持枚举本身的整体大小。默认情况下，这个lint是“允许”的，因为它可能有噪声，并且可能不会产生实际问题。有关这方面的决策应以分析和基准测试为指导。</t>
+          <t>将一个变体添加到比其他变体大得多的enum中可能是错误的，这会使所有变体所需的总体大小膨胀。这可能会影响性能和内存使用率。如果一个变体比第二大变体大3倍以上，就会触发这种情况。考虑将大变体的内容放在堆上（例如，Levia Box），以降低enum本身的整体大小。默认情况下，这个lint是“允许”的，因为它可能有噪声，并且可能不会产生实际问题。有关这方面的决策应以分析和基准测试为指导。</t>
         </is>
       </c>
       <c r="E680" t="inlineStr">
@@ -23707,12 +23707,12 @@
       </c>
       <c r="C681" t="inlineStr">
         <is>
-          <t>improver_types lint检测到在foreignmodule中不正确使用类型。</t>
+          <t>improver_typeslint检测到在foreignmodule中不正确使用类型。</t>
         </is>
       </c>
       <c r="D681" t="inlineStr">
         <is>
-          <t>编译器有几个检查来验证外部块中使用的类型是否安全，并遵循某些规则以确保与外部接口的适当兼容性。当检测到定义中可能存在错误时，就会发出此lint。lint通常应该提供问题的描述，并可能提供如何解决问题的提示。</t>
+          <t>编译器有几个检查来验证外部块中使用的类型是否安全，并遵循某些规则以确保与外部接口的适当兼容性。当它检测到定义中可能存在错误时，就会发出此lint。lint通常应该提供问题的描述，并可能提供如何解决问题的提示。</t>
         </is>
       </c>
       <c r="E681" t="inlineStr">
@@ -23735,12 +23735,12 @@
       </c>
       <c r="C682" t="inlineStr">
         <is>
-          <t>improver_types_definitions lint检测到外部函数定义的错误使用。</t>
+          <t>improver_types_definitionslint检测到外部函数定义的使用不正确。</t>
         </is>
       </c>
       <c r="D682" t="inlineStr">
         <is>
-          <t>外部函数中可能指定了许多与给定ABI不兼容的参数和返回类型。Thislint是一个警告，不应使用这些类型。lint通常应该提供问题的描述，并可能提示如何解决问题。</t>
+          <t>外部函数中可能指定了许多与给定ABI不兼容的参数和返回类型。Thislint是一个警告，不应使用这些类型。lint通常应该提供该问题的描述，并可能提示如何解决该问题。</t>
         </is>
       </c>
       <c r="E682" t="inlineStr">
@@ -23762,7 +23762,7 @@
       </c>
       <c r="C683" t="inlineStr">
         <is>
-          <t>invalid_atomic_ordering lint检测将ordering传递给不支持该排序的原子操作。</t>
+          <t>invalid_atomic_orderinglint检测将ordering传递给不支持该排序的原子操作。</t>
         </is>
       </c>
       <c r="D683" t="inlineStr">
@@ -23791,7 +23791,7 @@
       </c>
       <c r="C684" t="inlineStr">
         <is>
-          <t>unused_must_use lint检测标记为#[must_use]的类型的未使用结果。</t>
+          <t>unused_must_uselint检测标记为#[must_use]的类型的未使用结果。</t>
         </is>
       </c>
       <c r="D684" t="inlineStr">
@@ -23822,12 +23822,12 @@
       </c>
       <c r="C685" t="inlineStr">
         <is>
-          <t>unused_results lint检查语句中表达式的未使用结果。</t>
+          <t>unused_resultslint检查语句中表达式的未使用结果。</t>
         </is>
       </c>
       <c r="D685" t="inlineStr">
         <is>
-          <t>忽略函数的返回值可能表示错误。如果几乎可以确定应该使用结果，建议使用must_use属性对函数进行注释。如果不使用这样的返回值，将触发unused_must_userint，默认情况下会发出警告。unused_results lint本质上是相同的，但会触发所有返回值。默认情况下，这个lint是“允许”的，因为它可能有噪音，而且可能不是真正的问题。例如，调用VecorHashMap的remove方法会返回上一个值，您可能不关心这个值。使用这个lint需要显式忽略或丢弃这些值。</t>
+          <t>忽略函数的返回值可能表示错误。如果几乎可以确定应该使用结果，建议使用must_use属性对函数进行注释。如果不使用这样的返回值，将触发unused_must_userint，默认情况下会发出警告。unused_resultslint本质上是相同的，但会触发所有返回值。默认情况下，这个linnt是“允许”的，因为它可能有噪音，可能不会产生实际问题。例如，调用Vecor HashMap的remove方法会返回上一个值，您可能不关心这个值。使用这个lint需要显式忽略或丢弃这些值。</t>
         </is>
       </c>
       <c r="E685" t="inlineStr">
@@ -23852,7 +23852,7 @@
       </c>
       <c r="C686" t="inlineStr">
         <is>
-          <t>path_statements lint检测到无效的路径语句。</t>
+          <t>path_statementslint检测到无效的路径语句。</t>
         </is>
       </c>
       <c r="D686" t="inlineStr">
@@ -23879,7 +23879,7 @@
       </c>
       <c r="C687" t="inlineStr">
         <is>
-          <t>unused_rens lint检测if、match、while，并用括号返回；他们不需要它们。</t>
+          <t>unused_renslint检测if、match、while，并用括号返回；他们不需要它们。</t>
         </is>
       </c>
       <c r="D687" t="inlineStr">
@@ -23905,7 +23905,7 @@
       </c>
       <c r="C688" t="inlineStr">
         <is>
-          <t>unused_bracing lint检测表达式周围不必要的大括号。</t>
+          <t>unused_raceslint检测表达式周围不必要的大括号。</t>
         </is>
       </c>
       <c r="D688" t="inlineStr">
@@ -23933,12 +23933,12 @@
       </c>
       <c r="C689" t="inlineStr">
         <is>
-          <t>unused_import_braces lint在所移植的项目周围捕获不必要的大括号。</t>
+          <t>unused_import_braceslint捕获了一个移植项目周围不必要的大括号。</t>
         </is>
       </c>
       <c r="D689" t="inlineStr">
         <is>
-          <t>如果只有一个项目，那么删除大括号（例如，使用test:：a）。这个lint默认为“允许”，因为它只是强制执行astylistic选项。</t>
+          <t>如果只有一个项目，那么删除大括号（例如，使用test:：a）。默认情况下，这个lint是“允许”的，因为它只是强制执行astylistic选项。</t>
         </is>
       </c>
       <c r="E689" t="inlineStr">
@@ -23964,7 +23964,7 @@
       </c>
       <c r="C690" t="inlineStr">
         <is>
-          <t>unused_allocation lint检测可以消除的不必要的分配。</t>
+          <t>unused_allocationlint检测可以消除的不必要的分配。</t>
         </is>
       </c>
       <c r="D690" t="inlineStr">
@@ -23992,12 +23992,12 @@
       </c>
       <c r="C691" t="inlineStr">
         <is>
-          <t>forbidden_lint_groups lint检测应用于lint组的边界冲突。由于编译器中的一个错误，这些过去都被完全忽略了。它们现在生成一个警告。</t>
+          <t>forbidden_lint_groupslint检测应用于lint组的orbid的冲突。由于编译器中的一个错误，这些过去都被完全忽略了。它们现在生成一个警告。</t>
         </is>
       </c>
       <c r="D691" t="inlineStr">
         <is>
-          <t>由于编译器的错误，对lint组应用禁止显然没有效果。这个错误现在已经修复，但我们没有强制禁止，而是发布这个未来的兼容性警告，以避免破坏现有的板条箱。</t>
+          <t>由于编译器错误，对lint组广泛应用禁止没有任何效果。这个错误现在已经修复，但我们没有强制禁止，而是发布这个未来的兼容性警告，以避免破坏现有的板条箱。</t>
         </is>
       </c>
       <c r="E691" t="inlineStr">
@@ -24020,12 +24020,12 @@
       </c>
       <c r="C692" t="inlineStr">
         <is>
-          <t>ill_formed_attribute_input lint检测以前在实践中接受和使用的不正确的attributeinputs。</t>
+          <t>ill_formed_attribute_inputlint检测以前在实践中接受和使用的格式错误的attributeinputs。</t>
         </is>
       </c>
       <c r="D692" t="inlineStr">
         <is>
-          <t>以前，许多内置属性的输入没有经过验证，并且接受了无意义的属性输入。经过验证后，确定一些现有项目使用了这些无效表格。这是一个未来不兼容的皮棉，将其转变为未来的一个硬错误。有关更多详细信息，请参阅第57571期。有关属性的有效输入，请查看属性引用。</t>
+          <t>以前，许多内置属性的输入没有经过验证，并且接受了无意义的属性输入。经过验证后，确定一些现有项目使用了这些无效表格。这是一个未来不兼容的lint，将其转变为未来的一个硬错误。有关更多详细信息，请参阅第57571期。有关属性的有效输入，请查看属性引用。</t>
         </is>
       </c>
       <c r="E692" t="inlineStr">
@@ -24047,12 +24047,12 @@
       </c>
       <c r="C693" t="inlineStr">
         <is>
-          <t>conflicting_rer_hits lint检测具有冲突提示的repr属性。</t>
+          <t>conflicting_rer_hitslint检测具有冲突提示的repr属性。</t>
         </is>
       </c>
       <c r="D693" t="inlineStr">
         <is>
-          <t>编译器过去错误地接受了这些相互冲突的表示。这是一个未来不兼容的lint，以便在未来将其转换为一个hard错误。有关更多详细信息，请参阅问题#68585。若要更正此问题，请删除其中一个冲突提示。</t>
+          <t>编译器过去错误地接受了这些相互冲突的表示。这是一个未来不兼容的lint，以便在未来将其转换为一个严重错误。有关更多详细信息，请参阅问题#68585。若要更正此问题，请删除其中一个冲突提示。</t>
         </is>
       </c>
       <c r="E693" t="inlineStr">
@@ -24076,12 +24076,12 @@
       </c>
       <c r="C694" t="inlineStr">
         <is>
-          <t>meta_variable_misuse lint检测宏定义中可能存在的元变量误用。</t>
+          <t>meta_variable_misuselint检测宏定义中可能存在的元变量误用。</t>
         </is>
       </c>
       <c r="D694" t="inlineStr">
         <is>
-          <t>macro_rules宏有很多不同的定义方式。这些错误中的许多以前只有在宏被扩展或根本没有被扩展时才被检测到。此lint是在定义宏时尝试发现其中一些问题。此lint默认为“允许”，因为它可能存在误报和其他问题。有关更多详细信息，请参阅第61053期。</t>
+          <t>macro_rules宏有很多不同的定义方式。这些错误中的许多以前只有在宏被扩展或根本没有被扩展时才被检测到。此lint是在定义宏时尝试发现其中一些问题。此linet默认为“允许”，因为它可能存在误报和其他问题。有关更多详细信息，请参阅第61053期。</t>
         </is>
       </c>
       <c r="E694" t="inlineStr">
@@ -24109,12 +24109,12 @@
       </c>
       <c r="C695" t="inlineStr">
         <is>
-          <t>incomplete_include lint检测到使用了include！具有包含多个表达式的文件的宏。</t>
+          <t>incomplete_includelint检测include的使用！具有包含多个表达式的文件的宏。</t>
         </is>
       </c>
       <c r="D695" t="inlineStr">
         <is>
-          <t>包括！宏当前仅用于包含单个表达式或多个项。从历史上看，它会忽略第一个表达式之后的任何内容，但这可能会造成混淆。在上面的例子中，println！表达式在分号之前结束，使分号成为被忽略的“额外”信息。也许更令人惊讶的是，如果包含的文件有多个print语句，那么后面的语句将被忽略！一种解决方法是将内容放在大括号中以创建块表达式。还要考虑其他选择，比如使用函数来封装表达式，或者使用proc-macros。这是一个lint错误，而不是一个硬错误，因为发现现有项目遇到了这个错误。需要谨慎的是，这只是暂时的问题。include的未来语义！宏观经济也不确定，见第35560号问题。</t>
+          <t>包括！宏当前仅用于包含单个表达式或多个项。从历史上看，它会忽略第一个表达式之后的任何内容，但这可能会造成混淆。在上面的示例中，println！表达式正好在分号之前结束，从而使分号成为被忽略的“额外”信息。也许更令人惊讶的是，如果包含的文件有多个print语句，那么后面的语句将被忽略！一种解决方法是将内容放在大括号中以创建块表达式。还要考虑其他选择，比如使用函数封装表达式，或者使用proc-macros。这是一个lint错误，而不是一个硬错误，因为发现现有项目遇到了这个错误。需要谨慎的是，目前这是一个lint。include的未来语义！宏观经济也不确定，见第35560号问题。</t>
         </is>
       </c>
       <c r="E695" t="inlineStr">
@@ -24173,12 +24173,12 @@
       </c>
       <c r="C697" t="inlineStr">
         <is>
-          <t>uncconditional_palace lint检测到一个将在运行时导致apanic的操作。</t>
+          <t>unconditional_apaniclint检测到一个将在运行时导致故障的操作。</t>
         </is>
       </c>
       <c r="D697" t="inlineStr">
         <is>
-          <t>这个lint检测到很可能不正确的代码，因为它总是会死机，比如除以零和越界数组处理。如果这是一个bug，请考虑调整您的代码，或者使用anic！或无法访问！宏，以防恐慌。</t>
+          <t>这个lint检测到很可能不正确的代码，因为它总是死机，比如除以零和越界数组处理。如果这是一个bug，请考虑调整您的代码，或者使用anic！或者reachable！宏，以防出现恐慌。</t>
         </is>
       </c>
       <c r="E697" t="inlineStr">
@@ -24200,7 +24200,7 @@
       </c>
       <c r="C698" t="inlineStr">
         <is>
-          <t>unused_imports lint检测从未使用过的导入。</t>
+          <t>unused_importslint检测从未使用过的导入。</t>
         </is>
       </c>
       <c r="D698" t="inlineStr">
@@ -24226,12 +24226,12 @@
       </c>
       <c r="C699" t="inlineStr">
         <is>
-          <t>must_not_suspend lint保护不应该在挂起点（.await）之间保留的值</t>
+          <t>must_not_suspendlint保护不应该在挂起点（.await）之间保留的值</t>
         </is>
       </c>
       <c r="D699" t="inlineStr">
         <is>
-          <t>must_not_suspend lint检测标记有#[must_not_suspend]属性的值，该属性在挂起点之间保持。“suspend”点通常是asyncfunction中的.await。此属性可用于标记在suspend中语义不正确的值（如某些类型的计时器）、具有异步替代项的值以及经常导致async-fn返回的futures的发送性问题的值（例如MutexGuard）</t>
+          <t>must_not_suspendlint检测标记有#[must_not_suspend]属性的值，该属性在挂起点之间保持。“suspend”点通常是async函数中的.await。此属性可用于标记在suspend中语义不正确的值（如某些类型的计时器）、具有async替代项的值，以及经常导致asyncfn返回期货的发送性问题的值（例如MutexGuard）</t>
         </is>
       </c>
       <c r="E699" t="inlineStr">
@@ -24260,12 +24260,12 @@
       </c>
       <c r="C700" t="inlineStr">
         <is>
-          <t>未使用的_extern_crates皮棉可防止从未使用过的外部板条箱物品。</t>
+          <t>未使用的_extern_crateslint可防止从未使用过的外部crate项目。</t>
         </is>
       </c>
       <c r="D700" t="inlineStr">
         <is>
-          <t>未使用的外部板条箱物品没有任何影响，应予以移除。请注意，在某些情况下，为了确保给定的板条箱被链接的副作用，即使没有直接引用，也需要指定外部板条箱。lint可以通过将crate别名为下划线来静音，例如_之类的xtern crate foo。还要注意的是，在2018年的版本中，它不再是惯用的外部板条箱，因为外部板条箱现在自动添加到范围中。默认情况下，这个皮棉是“允许”的，因为它可能会发出噪音，并产生假阳性。如果要从项目中删除依赖项，建议将其从构建配置（如Cargo.toml）中删除，以确保不会留下过时的构建条目。</t>
+          <t>未使用的外部crate物品没有任何效果，应予以移除。请注意，在某些情况下，为了确保给定的crate被链接的副作用，即使没有直接引用，也需要指定外部crates。lint可以通过将crate别名为下划线来静音，例如xterncratesfoo为_。还要注意的是，在2018年的版本中，它不再是惯用的externcrates，因为extern_crates现在自动添加到scope中。默认情况下，这个lint是“允许”的，因为它可能会发出噪音，并产生假阳性。如果要从项目中删除依赖项，建议将其从构建配置（如Cargo.toml）中删除，以确保不会留下过时的构建条目。</t>
         </is>
       </c>
       <c r="E700" t="inlineStr">
@@ -24288,12 +24288,12 @@
       </c>
       <c r="C701" t="inlineStr">
         <is>
-          <t>unused_rate_dependences lint检测从未使用过的机箱依赖项。</t>
+          <t>unused_rate_dependenceslint检测从未使用过的crate依赖项。</t>
         </is>
       </c>
       <c r="D701" t="inlineStr">
         <is>
-          <t>删除使用依赖项的代码后，通常还需要从生成配置中删除依赖项。但是，有时可能会错过这一步骤，从而导致生成不再使用的依赖项，从而浪费时间。此lint可以检测从未使用过的依赖项（更具体地说，任何通过use、extern crate或任何路径引用的带有--extern命令行标志的依赖项）。此lint默认为“允许”，因为它可以根据构建系统的配置方式提供假阳性。例如，当使用Cargo时，一个“包裹”由多个板条箱组成（例如不合格品和二进制），但依赖关系是为整个包裹定义的。如果有一个依赖项只在二进制中使用，而在库中没有使用，那么lint将在库中错误地发出。</t>
+          <t>删除使用依赖项的代码后，通常还需要从生成配置中删除依赖项。但是，有时可能会错过这一步骤，从而导致生成不再使用的依赖项，从而浪费时间。这个lint可以检测从未使用过的依赖项（更具体地说，任何通过use、extern crate或任何路径引用的带有--extern命令行标志的依赖项）。默认情况下，这个linet是“允许”的，因为它可以根据构建系统的配置方式提供误报。例如，当使用Cargo时，一个“包裹”由多个crates（如不在场和二进制）组成，但依赖关系是为整个包裹定义的。如果有一个依赖项只在二进制文件中使用，而在库中没有使用，那么lint将在库中被错误地发出。</t>
         </is>
       </c>
       <c r="E701" t="inlineStr">
@@ -24322,12 +24322,12 @@
       </c>
       <c r="C702" t="inlineStr">
         <is>
-          <t>unused_qualifications lint检测不必要的限定名称。</t>
+          <t>unused_qualificationslint检测不必要的限定名称。</t>
         </is>
       </c>
       <c r="D702" t="inlineStr">
         <is>
-          <t>如果来自另一个模块的项目已经进入范围，那么在这种情况下就不需要对其进行限定。你可以直接调用bar（），不需要foo:：。这个lint在默认情况下是“允许”的，因为它有点迂腐，并不表示实际的问题，而是一种风格选择，并且在重构或移动代码时可能会很吵。</t>
+          <t>如果来自另一个模块的项目已经进入范围，那么在这种情况下就不需要对其进行限定。您可以直接调用bar（），而不使用foo:：。默认情况下，这个lint是“允许”的，因为它有点迂腐，并不表示实际的问题，而是一种风格选择，并且在重构或移动代码时可能会很吵。</t>
         </is>
       </c>
       <c r="E702" t="inlineStr">
@@ -24355,12 +24355,12 @@
       </c>
       <c r="C703" t="inlineStr">
         <is>
-          <t>unknown_lints lint检测到无法识别的lint属性。</t>
+          <t>unknown_lintslint检测到无法识别的linnt属性。</t>
         </is>
       </c>
       <c r="D703" t="inlineStr">
         <is>
-          <t>指定不存在的皮棉通常是错误的。检查拼写，并检查lint列表中的正确名称。如果您使用的是旧版本的编译器，而lint仅在新版本中可用，则使用Alsoconsider。</t>
+          <t>指定不存在的lint通常是错误的。检查拼写，并在lint列表中查找正确的名称。如果您使用的是旧版本的编译器，而lint仅在新版本中可用，则使用Alsoconsider。</t>
         </is>
       </c>
       <c r="E703" t="inlineStr">
@@ -24381,12 +24381,12 @@
       </c>
       <c r="C704" t="inlineStr">
         <is>
-          <t>未完成的lint_expectations lint检测到尚未完成的lint触发预期。</t>
+          <t>未实现的lint_expectationslint检测到尚未实现的触发器预期。</t>
         </is>
       </c>
       <c r="D704" t="inlineStr">
         <is>
-          <t>预计标记的代码会发出一个lint。此预期尚未实现。如果这是预期行为，则可以删除expect属性，否则应调查不再发出预期lint的原因。在极少数情况下，预期可能会在与所示代码段中显示的位置不同的位置发出。在大多数情况下，#[expect]属性在添加到外部作用域时起作用。在一个板条箱级别上只能预期几个短绒。RFC 2383的一部分。54503号中正在跟踪进度</t>
+          <t>预计标记的代码会发出一个lint。此预期尚未实现。如果这是预期行为，则可以删除expect属性，否则应调查不再发出预期lint的原因。在极少数情况下，预期可能会在与所示代码段中显示的位置不同的位置发出。在大多数情况下，#[expect]属性在添加到外部作用域时起作用。几个lint只能在crate级别上预期。RFC 2383的一部分。54503号中正在跟踪进度</t>
         </is>
       </c>
       <c r="E704" t="inlineStr">
@@ -24410,7 +24410,7 @@
       </c>
       <c r="C705" t="inlineStr">
         <is>
-          <t>unused_variables lint检测未以任何方式使用的变量。</t>
+          <t>unused_variableslint检测未以任何方式使用的变量。</t>
         </is>
       </c>
       <c r="D705" t="inlineStr">
@@ -24436,7 +24436,7 @@
       </c>
       <c r="C706" t="inlineStr">
         <is>
-          <t>unused_assignments lint检测永远不会读取的分配。</t>
+          <t>unused_assignmentslint检测到永远不会读取的分配。</t>
         </is>
       </c>
       <c r="D706" t="inlineStr">
@@ -24463,7 +24463,7 @@
       </c>
       <c r="C707" t="inlineStr">
         <is>
-          <t>dead_code lint检测未使用、未过期的项目。</t>
+          <t>dead_codelint检测未使用、未过期的项目。</t>
         </is>
       </c>
       <c r="D707" t="inlineStr">
@@ -24489,7 +24489,7 @@
       </c>
       <c r="C708" t="inlineStr">
         <is>
-          <t>unused_attributes lint检测编译器未使用的属性。</t>
+          <t>unused_attributeslint检测编译器未使用的属性。</t>
         </is>
       </c>
       <c r="D708" t="inlineStr">
@@ -24515,12 +24515,12 @@
       </c>
       <c r="C709" t="inlineStr">
         <is>
-          <t>unused_tuple_struct_fields lint检测从未读取的元组结构的字段。</t>
+          <t>unused_tuple_struct_fieldslint检测从未读取的元组结构的字段。</t>
         </is>
       </c>
       <c r="D709" t="inlineStr">
         <is>
-          <t>从不在任何地方读取的元组结构字段可能指示错误或未完成的代码。若要使此警告静音，请考虑移动未使用的字段，或者，若要保留保留字段的编号，请将未使用字段更改为单位类型。</t>
+          <t>从不在任何地方读取的元组struct字段可能指示错误或未完成的代码。若要使此警告静音，请考虑移动未使用的字段，或者，若要保留保留字段的编号，请将未使用字段更改为单位类型。</t>
         </is>
       </c>
       <c r="E709" t="inlineStr">
@@ -24544,7 +24544,7 @@
       </c>
       <c r="C710" t="inlineStr">
         <is>
-          <t>unreachable_code lint检测不可访问的代码路径。</t>
+          <t>unreachable_codelint检测不可访问的代码路径。</t>
         </is>
       </c>
       <c r="D710" t="inlineStr">
@@ -24571,7 +24571,7 @@
       </c>
       <c r="C711" t="inlineStr">
         <is>
-          <t>unreachable_patterns lint检测不可访问的模式。</t>
+          <t>无法访问的_patternslint检测无法访问的模式。</t>
         </is>
       </c>
       <c r="D711" t="inlineStr">
@@ -24601,7 +24601,7 @@
       </c>
       <c r="C712" t="inlineStr">
         <is>
-          <t>overlaping_range_endpoints lint检测在其端点上具有重叠范围模式的匹配臂。</t>
+          <t>overlaping_range_endpointslint检测在其端点上具有重叠范围模式的比赛臂。</t>
         </is>
       </c>
       <c r="D712" t="inlineStr">
@@ -24631,12 +24631,12 @@
       </c>
       <c r="C713" t="inlineStr">
         <is>
-          <t>bindings_with_variant_name lint检测与匹配变体之一具有相同名称的模式绑定。</t>
+          <t>bindings_with_variant_namelint检测与匹配变体之一具有相同名称的模式绑定。</t>
         </is>
       </c>
       <c r="D713" t="inlineStr">
         <is>
-          <t>将枚举变体名称指定为标识符模式通常是错误的。在上面的例子中，匹配arms指定了一个变量名来将x值绑定到。第二个armis被忽略，因为第一个armis匹配所有值。可能的意图是arm打算在枚举变体上匹配。两种可能的解决方案是：使用路径模式指定枚举变体，例如enum:：Foo。将枚举变体绑定到本地范围，例如添加use enum:；到上面示例中foo函数的开头。</t>
+          <t>将enum变体名称指定为标识符模式通常是错误的。在上面的例子中，匹配arms指定了一个变量名来将x值绑定到。第二个armis被忽略，因为第一个armis匹配所有值。可能的意图是arm打算在enum变体上匹配。两种可能的解决方案是：使用路径模式指定enum变体，例如enum:：Foo。将enu姆变体绑定到本地作用域中，例如添加use enum：：*；到上面示例中foo函数的开头。</t>
         </is>
       </c>
       <c r="E713" t="inlineStr">
@@ -24666,7 +24666,7 @@
       </c>
       <c r="C714" t="inlineStr">
         <is>
-          <t>unused_macros-lint检测未使用的宏。请注意，此lint与unused_acros_rules lint不同，后者检查从未与其他使用的宏匹配的单个规则，因此永远不会展开。</t>
+          <t>unused_macroslint检测未使用的宏。请注意，此linnt与unused_acro_rules lint不同，后者检查从未与其他使用的宏匹配的单个规则，因此从未展开。</t>
         </is>
       </c>
       <c r="D714" t="inlineStr">
@@ -24696,7 +24696,7 @@
       </c>
       <c r="C715" t="inlineStr">
         <is>
-          <t>未使用的_macro_rules lint检测未使用的宏规则。请注意，lint与未使用的.macros lint不同，后者在从未调用整个宏的情况下会激发，而此lint则会激发宏中未使用的单个规则。只有在未使用的/macros不会激发时，nused_macro_rules才会激发。</t>
+          <t>unused_macro_ruleslint检测未使用的宏规则。请注意，linnt与未使用的macro-lint不同，后者在从未调用整个宏的情况下会激发，而此lint则为未使用的、以其他方式使用的宏的单个未使用规则激发。只有在未使用的_macros不会激发时，才会激发nused_macro_rules。</t>
         </is>
       </c>
       <c r="D715" t="inlineStr">
@@ -24734,7 +24734,7 @@
       </c>
       <c r="D716" t="inlineStr">
         <is>
-          <t>警告lint有点特别；通过更改其级别，您可以将每一个会产生警告的警告更改为您想要的任何值。因此，您永远不会直接在代码中触发此lint。</t>
+          <t>警告lint有点特别；通过更改其级别，您可以将每一个会产生警告的警告更改为您想要的任何值。因此，您永远不会在代码中直接触发这个lint。</t>
         </is>
       </c>
       <c r="E716" t="inlineStr">
@@ -24756,7 +24756,7 @@
       </c>
       <c r="C717" t="inlineStr">
         <is>
-          <t>unused_features lint检测未使用或未知的功能，发现这些功能会增加级别的功能属性。注意：此lint当前不起作用，有关详细信息，请参阅问题#44232。</t>
+          <t>unused_featureslint检测到未使用或未知的功能，这些功能已在高级功能属性中找到。注意：此lint当前不起作用，有关详细信息，请参阅问题#44232。</t>
         </is>
       </c>
       <c r="D717" t="inlineStr"/>
@@ -24774,7 +24774,7 @@
       </c>
       <c r="C718" t="inlineStr">
         <is>
-          <t>stable_features lint检测一个已稳定的特征属性。</t>
+          <t>stable_featureslint检测一个已稳定的特征属性。</t>
         </is>
       </c>
       <c r="D718" t="inlineStr">
@@ -24801,7 +24801,7 @@
       </c>
       <c r="C719" t="inlineStr">
         <is>
-          <t>unknown_crate_types lint检测到在crate_type属性中发现的未知板条箱类型。</t>
+          <t>unknown_crate_typeslint检测到在crate_type属性中发现的未知crate类型。</t>
         </is>
       </c>
       <c r="D719" t="inlineStr">
@@ -24828,12 +24828,12 @@
       </c>
       <c r="C720" t="inlineStr">
         <is>
-          <t>trivil_casts lint检测可以用强制替换的琐碎强制，强制可能需要一个临时变量。</t>
+          <t>trivil_castslint检测可以用强制替换的琐碎类型转换，强制可能需要一个临时变量。</t>
         </is>
       </c>
       <c r="D720" t="inlineStr">
         <is>
-          <t>琐碎的强制转换是将e强制转换为T，其中e的类型为U，U的类型为T。通常可以推断出，这种类型的强制转换通常是不必要的。默认情况下，这个lint是“允许”的，因为在某些情况下，例如使用FFI接口或复杂类型别名时，它会正确触发，或者在更难清楚地表达意图的情况下。这可能会在未来引起人们的注意，可能会有一个明确的强制语法，为解决当前问题提供了一种方便的方法。有关历史上下文，请参阅RFC 401（强制）、RFC 803（类型归属）和RFC 3307（删除类型归属）。</t>
+          <t>琐碎的强制转换是将e强制转换为T，其中e的类型为U，U的类型为T。通常可以推断出，这种类型的强制转换通常是不必要的。默认情况下，这个lint是“允许”的，因为在某些情况下，例如使用FFI接口或复杂的类型别名，它会正确触发，或者在更难清楚地表达意图的情况下。这可能会在未来引起人们的注意，可能会有一个明确的强制语法，为解决当前问题提供了一种方便的方法。有关历史上下文，请参阅RFC 401（强制）、RFC 803（类型归属）和RFC 3307（删除类型归属）。</t>
         </is>
       </c>
       <c r="E720" t="inlineStr">
@@ -24856,12 +24856,12 @@
       </c>
       <c r="C721" t="inlineStr">
         <is>
-          <t>trivial_numeric_casts lint检测可以删除的类型的琐碎数字类型转换。</t>
+          <t>trivial_numeric_castslint检测可以删除的类型的琐碎数字类型转换。</t>
         </is>
       </c>
       <c r="D721" t="inlineStr">
         <is>
-          <t>琐碎的数字强制转换是将一个数字类型强制转换为相同的数字类型。这种类型的强制转换通常是不必要的。默认情况下，此lint是“允许”的，因为在某些情况下，例如使用FFI接口或复杂类型别名时，它会正确触发，或者在更难清楚地表达意图的情况下。这可能会在未来引起人们的注意，可能会有一个明确的强制语法，为解决当前问题提供了一种方便的方法。有关历史上下文，请参阅RFC 401（强制）、RFC 803（类型归属）和RFC 3307（删除类型归属）。</t>
+          <t>琐碎的数字强制转换是将一个数字类型强制转换为相同的数字类型。这种类型的强制转换通常是不必要的。默认情况下，这个lint是“允许”的，因为在某些情况下，例如使用FFI接口或复杂类型别名时，它会正确触发，或者在更难清晰表达意图的情况下。这可能会在未来引起人们的注意，可能会有一个明确的强制语法，为解决当前问题提供了一种方便的方法。有关历史上下文，请参阅RFC 401（强制）、RFC 803（类型归属）和RFC 3307（删除类型归属）。</t>
         </is>
       </c>
       <c r="E721" t="inlineStr">
@@ -24883,12 +24883,12 @@
       </c>
       <c r="C722" t="inlineStr">
         <is>
-          <t>private_in_public lint检测未被旧实现捕获的公共接口中的私有项。</t>
+          <t>private_in_publiclint检测公共接口中未被旧实现捕获的私有项。</t>
         </is>
       </c>
       <c r="D722" t="inlineStr">
         <is>
-          <t>可见性规则旨在防止在公共接口中暴露私有项。这是一个未来不兼容的lint，它将在未来转变为一个硬错误。有关更多详细信息，请参阅第34537期。</t>
+          <t>可见性规则旨在防止在公共接口中暴露私有项。这是一个未来不兼容的lint，将其转换为未来的硬错误。有关更多详细信息，请参阅第34537期。</t>
         </is>
       </c>
       <c r="E722" t="inlineStr">
@@ -24917,7 +24917,7 @@
       </c>
       <c r="C723" t="inlineStr">
         <is>
-          <t>invalid_aligent lint在常量求值期间检测未对齐指针的取消引用。</t>
+          <t>invalid_alignmentlint在常量求值期间检测未对齐指针的取消引用。</t>
         </is>
       </c>
       <c r="D723" t="inlineStr">
@@ -24950,7 +24950,7 @@
       </c>
       <c r="C724" t="inlineStr">
         <is>
-          <t>exported_private_dependencies lint检测在公共接口中公开的私有依赖关系。</t>
+          <t>exported_private_dependencieslint检测在公共接口中公开的私有依赖关系。</t>
         </is>
       </c>
       <c r="D724" t="inlineStr">
@@ -24986,12 +24986,12 @@
       </c>
       <c r="C725" t="inlineStr">
         <is>
-          <t>pub_use_of_private_extern_crate lint检测到重新导出专用外部机箱的特定情况。</t>
+          <t>pub_use_of_private_extern_cratelint检测到重新导出专用外部机箱的特定情况。</t>
         </is>
       </c>
       <c r="D725" t="inlineStr">
         <is>
-          <t>公共用途声明不应用于公开再出口aprivate外部板条箱。应该使用pub-externate。这在历史上是允许的，但根据可见性规则，这不是预期的行为。这是一个不可兼容的未来，将其转变为未来的一个硬错误。有关更多详细信息，请参阅第34537期。</t>
+          <t>公共用途声明不应用于公开再出口aprivate外部板条箱。应该使用pub-externcrate。这在历史上是允许的，但根据可见性规则，这不是预期的行为。这是一个不可兼容的未来，将其转变为未来的一个硬错误。有关更多详细信息，请参阅第34537期。</t>
         </is>
       </c>
       <c r="E725" t="inlineStr">
@@ -25013,12 +25013,12 @@
       </c>
       <c r="C726" t="inlineStr">
         <is>
-          <t>invalid_type_param_default lint检测到类型参数defaultserront在无效位置被允许。</t>
+          <t>invalid_type_param_defaultlint检测到类型参数defaultserront在无效位置被允许。</t>
         </is>
       </c>
       <c r="D726" t="inlineStr">
         <is>
-          <t>默认类型参数只在某些情况下被允许，但从历史上看，编译器在任何地方都允许它们。这是一个未来不兼容的lint，将来会将其转换为硬错误。有关更多详细信息，请参阅第36887期。</t>
+          <t>默认类型参数只在某些情况下被允许，但从历史上看，编译器在任何地方都允许它们。这是未来不兼容的lint，将来会将其转换为硬错误。有关更多详细信息，请参阅第36887期。</t>
         </is>
       </c>
       <c r="E726" t="inlineStr">
@@ -25039,12 +25039,12 @@
       </c>
       <c r="C727" t="inlineStr">
         <is>
-          <t>renamed_and_removed_lints lint检测已重命名或删除的lints。</t>
+          <t>renamed_and_removed_lintslint检测已重命名或删除的lints。</t>
         </is>
       </c>
       <c r="D727" t="inlineStr">
         <is>
-          <t>要解决此问题，请删除皮棉或使用新名称。这有助于避免对不再有效的lint产生混淆，并有助于保持重命名的lint的一致性。</t>
+          <t>要解决此问题，请删除lint或使用新名称。这有助于避免对已失效的lints的混淆，并有助于保持重命名的lints的一致性。</t>
         </is>
       </c>
       <c r="E727" t="inlineStr">
@@ -25065,12 +25065,12 @@
       </c>
       <c r="C728" t="inlineStr">
         <is>
-          <t>const_item_mutation lint检测对组成项进行变异的尝试。</t>
+          <t>const_item_mutationlint检测对组成项进行变异的尝试。</t>
         </is>
       </c>
       <c r="D728" t="inlineStr">
         <is>
-          <t>试图直接变异const项几乎总是一个错误。上面的例子中发生的情况是，const的临时副本发生了变异，但原始const没有。每次按名称引用const（如上例中的FOO）时，该值的一个单独副本都会在该位置内联。此lint检查是否直接写入字段（FOO.field=some_value）或数组项（FOO[0]=val），或获取const项的可变引用（&amp;mut FOO），包括通过anautoderef（FOO.some_mut_self_method（））。根据您试图实现的内容，有各种替代方案：首先，始终重新考虑使用可变全局变量，因为它们很难正确使用，并且会使代码更难使用或理解。如果您试图对全局变量执行一次性初始化：如果值可以在编译时计算，考虑使用const兼容的值（请参阅Constant Evaluation）。对于更复杂的单次初始化情况，请考虑使用第三方机箱，如lazy_static或once_cell。如果您使用的是夜间通道，请考虑标准库中的newlazy模块。如果您真的需要一个可变的全局，它有多种选项：简单的数据类型可以直接定义，并与解剖类型一起突变。更复杂的类型可以放在同步原语中，如Mutex，可以用上面列出的选项之一初始化。可变静态是一种低级原语，需要不安全。通常，应该避免这种情况，而不是像上面列出的更高级别的类型。</t>
+          <t>试图直接变异const项几乎总是一个错误。上面的例子中发生的情况是，const的临时副本发生了变异，但原始const没有。每次按名称引用const（如上例中的FOO）时，该值的一个单独副本都会在该位置内联。此lint检查是否直接写入字段（FOO.field=some_value）或数组项（FOO[0]=val），或对const项进行可变引用（&amp;mut FOO），包括通过anautoderef（FOO.some_mut_self_method（））。根据您试图实现的内容，有各种替代方案：首先，始终重新考虑使用可变全局变量，因为它们很难正确使用，并且会使代码更难使用或理解。如果您试图对全局变量执行一次性初始化：如果值可以在编译时计算，考虑使用const兼容的值（请参阅Constant Evaluation）。对于更复杂的单次初始化情况，请考虑使用第三方机箱，如lazy_static或once_cell。如果您使用的是夜间通道，请考虑标准库中的newlazy模块。如果您真的需要一个可变的全局，它有多种选项：简单的数据类型可以直接定义，并与解剖类型一起突变。更复杂的类型可以放在同步原语中，如Mutex，可以用上面列出的选项之一初始化。可变静态是一种低级原语，需要不安全。通常，应该避免这种情况，而不是像上面列出的更高级别的类型。</t>
         </is>
       </c>
       <c r="E728" t="inlineStr">
@@ -25096,12 +25096,12 @@
       </c>
       <c r="C729" t="inlineStr">
         <is>
-          <t>patterns_in_fns_without_body lint将mut标识符模式检测为没有主体的函数中的参数。</t>
+          <t>patterns_in_fns_without_bodylint将mut标识符模式检测为无正文函数中的参数。</t>
         </is>
       </c>
       <c r="D729" t="inlineStr">
         <is>
-          <t>要解决此问题，请从特征定义中的参数中删除mut；它可以在实现中使用。也就是说，以下内容是可以的：trait trait{fn foo（arg:u8）；//删除了i32的impl trait{fn foo。无正文函数中的参数名称只能是_或用于文档目的的标识符（只有类型是相关的）。以前版本的编译器错误地允许使用out关键字的标识符模式，但这是不允许的。这是一个未来不兼容的lint，将其转换为未来的硬错误。有关更多详细信息，请参阅第35203期。</t>
+          <t>要解决此问题，请从特征定义中的参数中删除mut；它可以在实现中使用。也就是说，以下内容是可以的：trait trait｛fnfoo（arg:u8）；//删除了此处的“mut”｝impl针对i32的trait{fnfoo（mut-arg:u8。无正文函数中的参数名称只能是_或用于文档目的的标识符（只有类型是相关的）。以前版本的编译器错误地允许使用out关键字的标识符模式，但这是不允许的。这是一个未来不兼容的lint，将其转换为未来的硬错误。有关更多详细信息，请参阅第35203期。</t>
         </is>
       </c>
       <c r="E729" t="inlineStr">
@@ -25124,7 +25124,7 @@
       </c>
       <c r="C730" t="inlineStr">
         <is>
-          <t>当amacro_rules中出现未使用的模式时，会发出missing_fragment_specifier lint！宏定义有一个元变量（例如$e），后面没有片段说明符（例如：expr）。可以通过删除macro_rules中未使用的模式来修复此警告！宏定义。</t>
+          <t>当amacro_rules中出现未使用的模式时，会发出missing_fragment_specifierlint！宏定义有一个元变量（例如$e），后面没有片段说明符（例如：expr）。可以通过删除macro_rules中未使用的模式来修复此警告！宏定义。</t>
         </is>
       </c>
       <c r="D730" t="inlineStr">
@@ -25156,7 +25156,7 @@
       </c>
       <c r="C731" t="inlineStr">
         <is>
-          <t>late_bound_lifetime_arguments lint检测具有后期绑定生存期参数的路径段中的通用生存期参数。</t>
+          <t>late_bound_lifetime_argumentslint检测具有后期绑定生存期参数的路径段中的通用生存期参数。</t>
         </is>
       </c>
       <c r="D731" t="inlineStr">
@@ -25188,12 +25188,12 @@
       </c>
       <c r="C732" t="inlineStr">
         <is>
-          <t>order_dependent_ttrait_objects lint检测到一个特征一致性违反，这将允许为涉及标记特征的同一动态特征对象创建两个特征impl。</t>
+          <t>order_dependent_ttrait_objectslint检测到一个特征一致性违反，该违反将允许为涉及标记特征的同一动态特征对象创建两个特征impl。</t>
         </is>
       </c>
       <c r="D732" t="inlineStr">
         <is>
-          <t>以前的一个错误导致编译器将具有不同标识符的特征（如Send+Sync和Sync+Send）解释为不同的类型，而它们本应被相同对待。这允许代码在出现一致性错误时定义单独的特征实现。这是一个未来不兼容的lint，以便在未来将其转换为一个hard错误。有关更多详细信息，请参阅第56484期。</t>
+          <t>以前的一个错误导致编译器将具有不同标识符的特征（如Send+Sync和Sync+Send）解释为不同的类型，而它们本应被相同对待。这允许代码在出现一致性错误时定义单独的特征实现。这是一个未来不兼容的lint，以便在未来将其转换为一个严重错误。有关更多详细信息，请参阅第56484期。</t>
         </is>
       </c>
       <c r="E732" t="inlineStr">
@@ -25216,12 +25216,12 @@
       </c>
       <c r="C733" t="inlineStr">
         <is>
-          <t>coherence_leak_check lint检测到只有旧的泄漏检查代码才能区分的特征的冲突实现。</t>
+          <t>coherence_leak_checklint检测一个只有旧的泄漏检查代码才能区分的特征的冲突实现。</t>
         </is>
       </c>
       <c r="D733" t="inlineStr">
         <is>
-          <t>在过去，编译器会接受相同函数的特征实现，这些函数的不同之处仅在于存在生存期绑定。由于借用检查器实现中的更改修复了几个错误，因此不再允许这样做。然而，由于这影响了代码的性别，这是一个未来不兼容的lint，将其转换为未来的一个硬错误。依赖于此模式的代码应该引入“新类型”，如structFoo（用于&lt;'a&gt;fn（&amp;'au8））。有关更多详细信息，请参阅第56105期。</t>
+          <t>在过去，编译器会接受相同函数的特征实现，这些函数的不同之处仅在于存在生存期绑定。由于借用检查器实现中的更改修复了几个错误，因此不再允许这样做。然而，由于这种影响性别的代码，这是一个未来不兼容的lint，以在未来将其转换为一个硬错误。依赖于这种模式的代码应该引入“新类型”，如structFoo（用于&lt;'a&gt;fn（&amp;'au8））。有关更多详细信息，请参阅第56105期。</t>
         </is>
       </c>
       <c r="E733" t="inlineStr">
@@ -25244,7 +25244,7 @@
       </c>
       <c r="C734" t="inlineStr">
         <is>
-          <t>不推荐使用的lint检测不推荐使用项目的情况。</t>
+          <t>弃用的lint检测到使用了弃用的项。</t>
         </is>
       </c>
       <c r="D734" t="inlineStr">
@@ -25274,7 +25274,7 @@
       </c>
       <c r="C735" t="inlineStr">
         <is>
-          <t>unused_unsafe lint检测到不必要地使用了不安全的块。</t>
+          <t>unused_unsafelint检测不必要地使用不安全块。</t>
         </is>
       </c>
       <c r="D735" t="inlineStr">
@@ -25300,7 +25300,7 @@
       </c>
       <c r="C736" t="inlineStr">
         <is>
-          <t>unused_mut-lint检测不需要可变的mut变量。</t>
+          <t>unused_mutlint检测不需要可变的mut变量。</t>
         </is>
       </c>
       <c r="D736" t="inlineStr">
@@ -25326,7 +25326,7 @@
       </c>
       <c r="C737" t="inlineStr">
         <is>
-          <t>非条件递归lint检测不调用自身就无法返回的函数。</t>
+          <t>无条件递归lint检测不调用自身就无法返回的函数。</t>
         </is>
       </c>
       <c r="D737" t="inlineStr">
@@ -25354,12 +25354,12 @@
       </c>
       <c r="C738" t="inlineStr">
         <is>
-          <t>single_use_lifetimes lint检测只使用一次的寿命。</t>
+          <t>single_use_lifetimeslint检测只使用一次的寿命。</t>
         </is>
       </c>
       <c r="D738" t="inlineStr">
         <is>
-          <t>在函数或impl中指定类似“a”的显式生存期只能用于将两件事链接在一起。否则，你应该只使用'_来表示生存期与任何东西都没有关联，或者如果可能的话，完全取消生存期。这个lint默认为“允许”，因为它是在首次引入'_和取消的生存期时引入的，而这个lint太吵了。此外，它还产生了一些已知的假阳性。有关历史上下文，请参阅RFC 2115，有关更多详细信息，请参阅#44752。</t>
+          <t>在函数或impl中指定类似“a”的显式生存期只能用于将两件事链接在一起。否则，您应该只使用'_来表示生存期与任何东西都没有关联，或者如果可能的话，完全取消生存期。默认情况下，这个lint是“允许”的，因为它是在首次引入'_和取消的生存期时引入的，而这个lint太吵了。此外，它还产生了一些已知的假阳性。有关历史上下文，请参阅RFC 2115，有关更多详细信息，请参阅#44752。</t>
         </is>
       </c>
       <c r="E738" t="inlineStr">
@@ -25381,7 +25381,7 @@
       </c>
       <c r="C739" t="inlineStr">
         <is>
-          <t>unused_lifetimes lint检测从未使用过的寿命参数。</t>
+          <t>unused_lifetimeslint检测从未使用过的寿命参数。</t>
         </is>
       </c>
       <c r="D739" t="inlineStr">
@@ -25408,12 +25408,12 @@
       </c>
       <c r="C740" t="inlineStr">
         <is>
-          <t>tyvar_behind_raw_pointer lint检测指向引用变量的原始指针。</t>
+          <t>tyvar_behind_raw_pointerlint检测指向引用变量的原始指针。</t>
         </is>
       </c>
       <c r="D740" t="inlineStr">
         <is>
-          <t>这种推理以前是允许的，但由于未来任意自我类型的竞争对手，这可能会引入歧义。为了解决这个问题，请使用显式类型，而不是依赖类型推理。这是一个未来不兼容的lint，可以在2018年版本中将其转换为硬错误。有关更多详细信息，请参阅第46906期。这在2018版中是一个严重错误，在2015版中默认为“警告”。</t>
+          <t>这种推理以前是允许的，但由于未来任意自我类型的竞争对手，这可能会引入歧义。为了解决这个问题，请使用显式类型，而不是依赖类型推理。这是一个未来不兼容的lint，可以在2018版中将其转换为硬错误。有关更多详细信息，请参阅第46906期。这在2018版中是一个严重错误，在2015版中默认为“警告”。</t>
         </is>
       </c>
       <c r="E740" t="inlineStr">
@@ -25437,12 +25437,12 @@
       </c>
       <c r="C741" t="inlineStr">
         <is>
-          <t>elided_lifetimes_in_paths lint检测hiddenlifetime参数的使用情况。</t>
+          <t>elided_lifetimes_in_pathslint检测hiddenlifetime参数的使用。</t>
         </is>
       </c>
       <c r="D741" t="inlineStr">
         <is>
-          <t>被排除的寿命参数可能会使人们很难在一个节点上看到借款的发生。此lint确保始终显式声明lifetimeparameters，即使它是“_placeholder lifetime”。此lint默认为“允许”，因为它存在一些已知问题，并且可能需要对旧代码进行重大转换。</t>
+          <t>被排除的寿命参数可能会使人们很难在一个节点上看到借款的发生。此lint确保始终显式声明lifetimeparameters，即使它是'_placeholder lifetime'。此linet默认为“允许”，因为它存在一些已知问题，并且可能需要对旧代码进行重大转换。</t>
         </is>
       </c>
       <c r="E741" t="inlineStr">
@@ -25469,7 +25469,7 @@
       </c>
       <c r="C742" t="inlineStr">
         <is>
-          <t>bare_trait_objects lint建议对traitobjects使用dyn trait。</t>
+          <t>bare_trait_objectslint建议对traitobjects使用dyn trait。</t>
         </is>
       </c>
       <c r="D742" t="inlineStr">
@@ -25497,12 +25497,12 @@
       </c>
       <c r="C743" t="inlineStr">
         <is>
-          <t>absolute_paths_not_starting_with_crate lint检测以模块名称而非机箱、自身或外部机箱名称开头的完全限定路径</t>
+          <t>absolute_paths_not_starting_with_cratelint检测以模块名称而非crate、self或externcrate名称开头的完全限定路径</t>
         </is>
       </c>
       <c r="D743" t="inlineStr">
         <is>
-          <t>Rust版本允许语言在不破坏向后兼容性的情况下进行发展。这个lint捕获了2015年版本风格中使用绝对值的代码。在2015年的版本中，absolutepaths（以：开头的）指的是板条箱根或外部板条箱。在2018年的版本中，它被更改为仅指外部板条箱。应该使用路径前缀crate:：来引用来自crate根目录的项。如果您在不更新代码的情况下将编译器从2015版切换到2018版，那么如果使用旧式路径，它将无法编译。您可以手动更改路径以使用crate:：前缀转换到2018版本。此lint自动解决了问题。默认情况下它是“允许”的，因为该代码在2015版本中完全有效。带有--edition标志的货物修复工具会将此lint切换为“warn”，并自动应用编译器建议的修复。这提供了一种完全自动化的方式来将旧代码更新到2018版。</t>
+          <t>Rust版本允许语言在不破坏向后兼容性的情况下进行发展。这个lint捕获了2015版风格中使用绝对值的代码。在2015年的版本中，absolutepaths（以：开头的）指的是crate根或外部板条箱。在2018年的版本中，它被更改为仅指外部板条箱。应该使用路径前缀crate:：来引用crate根目录中的项。如果您在不更新代码的情况下将编译器从2015版切换到2018版，那么如果使用旧式路径，它将无法编译。您可以手动更改路径以使用crate:：前缀转换到2018版本。这lint自动解决了问题。默认情况下它是“允许”的，因为该代码在2015版本中完全有效。带有--edition标志的carge修复工具会将此lint切换为“警告”，并自动应用编译器建议的修复。这提供了一种完全自动化的方式来将旧代码更新到2018版。</t>
         </is>
       </c>
       <c r="E743" t="inlineStr">
@@ -25529,12 +25529,12 @@
       </c>
       <c r="C744" t="inlineStr">
         <is>
-          <t>illegal_floating_point_literal_pattern lint检测模式中使用的浮点文字。</t>
+          <t>illegal_floating_point_literal_patternlint检测模式中使用的浮点文字。</t>
         </is>
       </c>
       <c r="D744" t="inlineStr">
         <is>
-          <t>以前版本的编译器接受模式中的浮点文字，但后来确定这是一个错误。与“结构相等”相比，比较浮点值的要求在模式中可能不明确。通常，您可以使用火柴保护来解决此问题，例如：#let x=42.0；match x｛y if y==5.0=&gt;｛｝_=&gt;｛}｝这是一个未来不兼容的lint，将来会将其转换为硬错误。有关更多详细信息，请参阅第41620期。</t>
+          <t>以前版本的编译器接受模式中的浮点文字，但后来确定这是一个错误。与“结构相等”相比，比较浮点值的要求在模式中可能不明确。通常，您可以使用火柴保护来解决此问题，例如：#let x=42.0；match x｛y if y==5.0=&gt;｛｝_=&gt;｛}｝这是一个未来不兼容的lint，将来将其转换为硬错误。有关更多详细信息，请参阅第41620期。</t>
         </is>
       </c>
       <c r="E744" t="inlineStr">
@@ -25591,12 +25591,12 @@
       </c>
       <c r="C746" t="inlineStr">
         <is>
-          <t>无可辩驳的_let_patterns lint在if let、while let和if let guards中检测无可辩驳模式。</t>
+          <t>无可辩驳的let模式lint检测if let、while let和if let guards中的无可辩驳模式。</t>
         </is>
       </c>
       <c r="D746" t="inlineStr">
         <is>
-          <t>通常没有理由在anif-let或while let语句中使用无可辩驳的模式，因为该模式总是能够成功匹配。let或loop语句就足够了。然而，当使用宏生成代码时，在宏不知道模式是否可拒绝的情况下，禁止无可辩驳的模式将需要尴尬的解决方案。这个lint允许小程序接受这个表单，同时警告正常代码中可能存在的错误。有关更多详细信息，请参阅RFC 2086。</t>
+          <t>通常没有理由在anif-let或while let语句中使用无可辩驳的模式，因为该模式总是能够成功匹配。let或loop语句就足够了。然而，当使用宏生成代码时，在宏不知道模式是否可拒绝的情况下，禁止无可辩驳的模式将需要尴尬的解决方案。这lint允许小程序接受此表单，同时警告正常代码中可能存在的错误。有关更多详细信息，请参阅RFC 2086。</t>
         </is>
       </c>
       <c r="E746" t="inlineStr">
@@ -25619,7 +25619,7 @@
       </c>
       <c r="C747" t="inlineStr">
         <is>
-          <t>unused_labels lint检测从未使用过的标签。</t>
+          <t>unused_labelslint检测从未使用过的标签。</t>
         </is>
       </c>
       <c r="D747" t="inlineStr">
@@ -25645,7 +25645,7 @@
       </c>
       <c r="C748" t="inlineStr">
         <is>
-          <t>whire_clauses_object_safety lint检测其中子句的对象安全性。</t>
+          <t>whire_clauses_object_safetylint检测其中子句的对象安全性。</t>
         </is>
       </c>
       <c r="D748" t="inlineStr">
@@ -25676,12 +25676,12 @@
       </c>
       <c r="C749" t="inlineStr">
         <is>
-          <t>proc_macro_derive_resolution_fallback lint使用父模块中不可访问的名称检测proc宏派生。</t>
+          <t>proc_macro_derive_resolution_ffalllint使用父模块中不可访问的名称检测proc宏派生。</t>
         </is>
       </c>
       <c r="D749" t="inlineStr">
         <is>
-          <t>如果proc宏生成了一个模块，编译器会意外地允许该模块中的项引用机箱根中的项，而不导入它们。这是一个未来不兼容的lint，将其转换为未来的一个硬错误。有关详细信息，请参阅第50504期。</t>
+          <t>如果proc宏生成了一个模块，编译器会意外地允许该模块中的项引用crate根中的项，而不导入它们。这是一个未来不兼容的lint，将其转换为未来的硬错误。有关详细信息，请参阅第50504期。</t>
         </is>
       </c>
       <c r="E749" t="inlineStr">
@@ -25727,12 +25727,12 @@
       </c>
       <c r="C750" t="inlineStr">
         <is>
-          <t>macro_use_extern_crate lint检测macro_use属性的使用。</t>
+          <t>macro_use_extern_cratelint检测macro_use属性的使用。</t>
         </is>
       </c>
       <c r="D750" t="inlineStr">
         <is>
-          <t>[extern crate]项上的macro_use属性导致该外部板条箱中的宏被带到速率的前奏中，从而使宏无处不在。作为【2018年版】中简化依赖关系处理的努力的一部分，外部机箱的使用正在逐步取消。要将外部cratesi中的宏放入作用域，建议使用use导入。此lint默认为“允许”，因为这是一种尚未解决的风格选择，请参阅问题#52043以了解更多信息。</t>
+          <t>[extern crate]项上的macro_use属性导致该外部crate中的宏被带到速率的前奏中，从而使宏无处不在。作为2018年版中简化依赖关系处理的努力的一部分，外部crate的使用正在逐步取消。要将外部cratesi中的宏引入作用域，建议使用use import。默认情况下，此lint为“允许”，因为这是一种尚未解决的风格选择，有关详细信息，请参阅问题#52043。</t>
         </is>
       </c>
       <c r="E750" t="inlineStr">
@@ -25770,7 +25770,7 @@
       </c>
       <c r="C751" t="inlineStr">
         <is>
-          <t>macro_expanded_macro_exports_accessed_by_absolute_paths lint检测到当前板条箱中的宏扩展宏_export宏，该宏无法由绝对路径引用。</t>
+          <t>macro_expanded_macro_exports_accessed_by_absolute_paths lint检测到当前crat中的宏扩展macro_export宏，该宏不能被绝对路径引用。</t>
         </is>
       </c>
       <c r="D751" t="inlineStr">
@@ -25807,12 +25807,12 @@
       </c>
       <c r="C752" t="inlineStr">
         <is>
-          <t>explicit_outlives_requirements lint检测可以推断的不必要的生存时间界限。</t>
+          <t>explicit_outlives_requirementslint检测可以推断的不必要的生存时间界限。</t>
         </is>
       </c>
       <c r="D752" t="inlineStr">
         <is>
-          <t>如果一个结构包含引用，如&amp;‘a T，则compiler要求T的寿命超过生存期‘a。这在历史上要求写一个明确的生命周期来表明这一要求。然而，这可能过于明确，导致混乱和不必要的复杂性。如果未指定绑定，语言已更改为自动推断绑定。具体地说，如果该结构包含对具有lifetime'x的T的直接或间接引用，那么它将推断出T:'x是一个需求。该lint默认为“允许”，因为对于已经具有这些需求的现有代码来说，它可能是有噪声的。这是一种风格上的选择，因为明确地说明界限仍然有效。它也有一些可能引起混淆的误报。请参阅RFC 2093了解更多详细信息。</t>
+          <t>如果struct包含引用，如&amp;'a T，则compiler要求T超过生存期'a。这在历史上要求写一个明确的生命周期来表明这一要求。然而，这可能过于明确，导致混乱和不必要的复杂性。如果未指定绑定，语言已更改为自动推断绑定。具体地说，如果结构包含对具有lifetime'x的T的直接或间接引用，那么它将推断出T:'x是一个要求。默认情况下，这个lint是“允许”的，因为对于已经具有这些要求的现有代码来说，它可能是有噪声的。这是一种风格上的选择，因为明确地说明界限仍然有效。它也有一些可能引起混淆的误报。请参阅RFC 2093了解更多详细信息。</t>
         </is>
       </c>
       <c r="E752" t="inlineStr">
@@ -25841,7 +25841,7 @@
       </c>
       <c r="C753" t="inlineStr">
         <is>
-          <t>indirect_structural_match lint检测手动实现PartialEq和Eq的模式中的常量。</t>
+          <t>indirect_structural_matchlint检测手动实现PartialEq和Eq的模式中的常量。</t>
         </is>
       </c>
       <c r="D753" t="inlineStr">
@@ -25879,7 +25879,7 @@
       </c>
       <c r="C754" t="inlineStr">
         <is>
-          <t>depleted_in_future lint是rustc内部的，用户代码不应该使用它。这个lint只在标准库中启用。它可以在将来的版本中使用#[approved]和一个since字段。这允许在未来的版本中将某些内容标记为不推荐使用，然后此lint将确保该项不再在标准库中使用。有关更多详细信息，请参阅稳定性文档。</t>
+          <t>depleted_in_futurelint是rustc内部的，用户代码不应使用它。此lint仅在标准库中启用。它可以在将来的版本的since字段中使用#[已弃用]。这允许在未来的版本中将某些内容标记为已弃用，然后此lint将确保该项不再在标准库中使用。有关更多详细信息，请参阅稳定性文档。</t>
         </is>
       </c>
       <c r="D754" t="inlineStr"/>
@@ -25897,12 +25897,12 @@
       </c>
       <c r="C755" t="inlineStr">
         <is>
-          <t>pointer_structural_match lint检测在编译器版本和优化级别中不能依赖其行为的模式中使用的指针。</t>
+          <t>pointer_structural_matchlint检测模式中使用的指针，这些模式的行为在编译器版本和优化级别之间是不可依赖的。</t>
         </is>
       </c>
       <c r="D755" t="inlineStr">
         <is>
-          <t>Rust的早期版本允许在模式中使用函数指针和宽原始指针。虽然这些指针在许多情况下都如用户所期望的那样工作，但由于优化，指针可能“不等于它们自己”，或者指向不同函数的指针在运行时间比较相等。这是因为LLVM优化可以在函数体相同的情况下消除重复，从而使指向这些函数的指针指向相同的位置。此外，如果函数被实例化在不同的板条箱中，并且没有通过LTO再次消除重复，则它们可能会被复制。</t>
+          <t>Rust的早期版本允许在模式中使用函数指针和宽原始指针。虽然这些指针在许多情况下都如用户所期望的那样工作，但由于优化，指针可能“不等于它们自己”，或者指向不同函数的指针在运行时间比较相等。这是因为LLVM优化可以在函数体相同的情况下消除重复，从而使指向这些函数的指针指向相同的位置。此外，如果函数在不同的crates中实例化，并且没有通过LTO再次消除重复，则它们可能会重复。</t>
         </is>
       </c>
       <c r="E755" t="inlineStr">
@@ -25931,7 +25931,7 @@
       </c>
       <c r="C756" t="inlineStr">
         <is>
-          <t>非平凡的structural_match lint检测模式中使用的常量，这些常量的类型不是结构匹配的，并且其初始值设定项主体实际使用的值不是结构匹配。因此，如果常量仅为None，则Option＜NotStructuralMatch＞是可以的。</t>
+          <t>非平凡_结构化_匹配lint检测模式中使用的常量，这些常量的类型与结构不匹配，初始值设定项主体实际使用的值与结构不一致。因此，如果常量仅为None，则Option＜NotStructuralMatch＞是可以的。</t>
         </is>
       </c>
       <c r="D756" t="inlineStr">
@@ -25965,12 +25965,12 @@
       </c>
       <c r="C757" t="inlineStr">
         <is>
-          <t>模糊_关联项lint检测关联项和枚举变量之间的模糊性。</t>
+          <t>模糊_关联项lint检测关联项和enum变体之间的模糊性。</t>
         </is>
       </c>
       <c r="D757" t="inlineStr">
         <is>
-          <t>Rust的早期版本不允许通过类型别名访问枚举变量。当添加此功能时（请参阅RFC 2338），这引入了一些情况，在这些情况下，类型所指的内容可能不明确。要解决这种不明确的问题，您应该使用一个限定路径来明确说明要使用的类型。例如，在上面的例子中，函数可以写为fn f（）-&gt;&lt;Self as Tr&gt;：：V｛0｝来指定引用关联的类型。这是一个未来不兼容的lint，可以在未来将其转换为硬错误。有关更多详细信息，请参阅第57644期。</t>
+          <t>Rust的早期版本不允许通过类型别名访问enumvariantsthrough。当添加此功能时（请参阅RFC 2338），这引入了一些情况，在这些情况下，类型所指的内容可能不明确。要解决这种不明确的问题，您应该使用一个限定路径来明确说明要使用的类型。例如，在上面的例子中，函数可以写为fnf（）-&gt;&lt;Self as Tr&gt;：：V｛0｝来指定引用关联的类型。这是一个未来不兼容的lint，可以在未来将其转换为硬错误。有关更多详细信息，请参阅第57644期。</t>
         </is>
       </c>
       <c r="E757" t="inlineStr">
@@ -26003,12 +26003,12 @@
       </c>
       <c r="C758" t="inlineStr">
         <is>
-          <t>soft_unstable lint检测到在stable上无意中允许的不稳定功能。</t>
+          <t>soft_unstablelint检测到在stable上无意允许的不稳定功能。</t>
         </is>
       </c>
       <c r="D758" t="inlineStr">
         <is>
-          <t>意外地允许在稳定发布通道上指定bench属性。如果把它变成一个严重的错误，可能会破坏一些项目。当使用--cap lints时，此lint允许这些项目继续正确构建，但在其他情况下会发出一个错误信号，即不应在稳定通道上使用#[Beet]。这是一个未来不兼容的皮棉，将其转变为未来的一个硬错误。有关更多详细信息，请参阅第64266期。</t>
+          <t>意外地允许在稳定发布通道上指定bench属性。如果把它变成一个严重的错误，可能会破坏一些项目。当使用--cap lints时，此lint允许这些项目继续正确构建，但在其他情况下会发出一个错误信号，即不应在稳定通道上使用#[bent]。这是一个未来不兼容的lint，将其转换为未来的硬错误。有关更多详细信息，请参阅第64266期。</t>
         </is>
       </c>
       <c r="E758" t="inlineStr">
@@ -26034,7 +26034,7 @@
       </c>
       <c r="C759" t="inlineStr">
         <is>
-          <t>inline_no_sanitive lint检测#[inline（always）]和#[no_sanitize（…）]的不兼容使用。</t>
+          <t>inline_no_sanizelint检测#[inline（always）]和#[no_sanize（…）]的不兼容使用。</t>
         </is>
       </c>
       <c r="D759" t="inlineStr">
@@ -26066,12 +26066,12 @@
       </c>
       <c r="C760" t="inlineStr">
         <is>
-          <t>asm_sub_register lint仅使用寄存器的子集来检测内联asm输入。</t>
+          <t>asm_sub_registerlint仅使用寄存器的子集来检测内联asm输入。</t>
         </is>
       </c>
       <c r="D760" t="inlineStr">
         <is>
-          <t>某些体系结构上的寄存器可以使用不同的名称来引用寄存器的子集。默认情况下，编译器将使用完整寄存器大小的名称。若要显式使用寄存器的子集，可以通过在模板操作数上使用修饰符指定何时使用子寄存器来覆盖默认值。如果您传入的值的数据类型小于默认寄存器大小，则会发出此lint，以提醒您可能使用了不正确的宽度。要解决此问题，请将建议的修饰符添加到模板中，或将值强制转换为正确的大小。有关详细信息，请参阅参考中的注册模板修饰符。</t>
+          <t>某些体系结构上的寄存器可以使用不同的名称来引用寄存器的子集。默认情况下，编译器将使用完整寄存器大小的名称。若要显式使用寄存器的子集，可以通过在模板操作数上使用修饰符指定何时使用子寄存器来覆盖默认值。如果您传入的值的数据类型小于默认寄存器大小，则会出现此lint，以提醒您可能使用了不正确的宽度。要解决此问题，请将建议的修饰符添加到模板中，或将值强制转换为正确的大小。有关详细信息，请参阅参考中的注册模板修饰符。</t>
         </is>
       </c>
       <c r="E760" t="inlineStr">
@@ -26109,7 +26109,7 @@
       </c>
       <c r="C761" t="inlineStr">
         <is>
-          <t>bad_asm_style lint检测.intel_syntax和.att_syntay指令的使用。</t>
+          <t>bad_asm_stylelint检测.intel_syntax和.att_syntay指令的使用。</t>
         </is>
       </c>
       <c r="D761" t="inlineStr">
@@ -26153,12 +26153,12 @@
       </c>
       <c r="C762" t="inlineStr">
         <is>
-          <t>unsaf.op_in_unsaf_fn lint在没有显式不安全块的情况下检测不安全函数中的不安全操作。</t>
+          <t>unsaf.op_in_unsaf_fnlint在没有显式不安全块的情况下检测不安全函数中的不安全操作。</t>
         </is>
       </c>
       <c r="D762" t="inlineStr">
         <is>
-          <t>目前，不安全fn允许在其体内进行任何不安全的操作。然而，这可能会增加代码的表面积，需要仔细检查代码的正确行为。不安全块提供了一种方便的方法，可以明确代码的哪些部分正在执行不安全操作。将来，希望对其进行更改，以便在没有不安全块的情况下，无法在不安全的fn中执行不安全操作。解决此问题的方法是将不安全代码包装在不安全块中。此lint默认为“允许”，因为这将影响大量现有代码，并且提高严重性的确切计划尚待考虑。有关更多详细信息，请参阅RFC#2585和问题#71668。</t>
+          <t>目前，不安全的fn允许在其体内进行任何不安全的操作。然而，这可能会增加代码的表面积，需要仔细检查代码的正确行为。不安全块提供了一种方便的方法，可以明确代码的哪些部分正在执行不安全操作。将来，希望对其进行更改，以便在没有不安全块的情况下，无法在不安全的fn中执行不安全操作。解决此问题的方法是将不安全代码包装在不安全块中。默认情况下，此lint为“允许”，因为这将影响大量现有代码，并且提高严重性的确切计划尚待考虑。有关更多详细信息，请参阅RFC#2585和问题#71668。</t>
         </is>
       </c>
       <c r="E762" t="inlineStr">
@@ -26184,12 +26184,12 @@
       </c>
       <c r="C763" t="inlineStr">
         <is>
-          <t>cenum_impl_drop_cast lint检测实现drop的字段lessnum的强制转换。</t>
+          <t>cenum_impl_drop_castlint检测实现drop的字段lessnum的强制转换。</t>
         </is>
       </c>
       <c r="D763" t="inlineStr">
         <is>
-          <t>将不实现Copy的无字段枚举强制转换为一个枚举将在不调用drop的情况下移动该值。如果预期应该调用drop，这可能会导致意外行为。自动调用drop将与其他移动操作不一致。由于这两种行为都不明确或一致，因此决定不再允许这种性质的强制转换。这是一个未来不兼容的lint，可以在未来将其转换为硬错误。有关更多详细信息，请参阅第73333期。</t>
+          <t>将不实现Copy的无字段enum强制转换为一个整数将在不调用drop的情况下移动该值。如果预期应该调用drop，这可能会导致意外行为。自动调用drop将与其他移动操作不一致。由于这两种行为都不明确或一致，因此决定不再允许这种性质的强制转换。这是未来不兼容的lint，将其转换为未来的硬错误。有关更多详细信息，请参阅第73333期。</t>
         </is>
       </c>
       <c r="E763" t="inlineStr">
@@ -26222,12 +26222,12 @@
       </c>
       <c r="C764" t="inlineStr">
         <is>
-          <t>fuzzy_provenance_cast lint检测整数和指针之间的强制转换。</t>
+          <t>fuzzy_provenance_castlint检测整数和指针之间的强制转换。</t>
         </is>
       </c>
       <c r="D764" t="inlineStr">
         <is>
-          <t>这个lint是严格出处工作的一部分，请参阅问题#95228。将整数投射到指针被认为是糟糕的风格，因为指针除了包含地址之外，还包含出处，指示允许指针读取/写入的内存。将一个没有出处的整数转换为指针需要编译器指定（猜测）出处。编译器分配“所有公开的有效”（有关此“公开”的更多信息，请参阅ptr:：from_exposed_addr的文档）。这会惩罚优化器，不太适合动态分析/动态程序验证（例如Miri或CHERIplatforms）。最好使用ptr:：with_addr来指定您想要的程序。如果由于代码依赖于暴露的出处而无法使用此函数，则存在转义hatchptr:：from_exposed_addr。</t>
+          <t>这lint是严格出处工作的一部分，请参阅问题#95228。将整数投射到指针被认为是不好的风格，因为指针除了包含地址之外，还包含出处，指示允许指针读取/写入的内存。将一个没有出处的整数转换为指针需要编译器指定（猜测）出处。编译器分配“所有公开的有效”（有关此“公开”的更多信息，请参阅ptr:：from_exposed_addr的文档）。这会惩罚优化器，不太适合动态分析/动态程序验证（例如Miri或CHERIplatforms）。最好使用ptr:：with_addr来指定您想要的程序。如果由于代码依赖于暴露的出处而无法使用此函数，则存在转义hatchptr:：from_exposed_addr。</t>
         </is>
       </c>
       <c r="E764" t="inlineStr">
@@ -26252,12 +26252,12 @@
       </c>
       <c r="C765" t="inlineStr">
         <is>
-          <t>loss_provenance_casts lint检测指针和整数之间的强制转换。</t>
+          <t>loss_provenance_castlint检测指针和整数之间的强制转换。</t>
         </is>
       </c>
       <c r="D765" t="inlineStr">
         <is>
-          <t>此lint是严格出处工作的一部分，请参阅问题#95228。将指针投射到整数是一种有损操作，因为除了地址之外，指针可能与特定的地址相关联。这些信息被优化器用于动态分析/动态程序验证（例如Miri或CHERI平台）。由于这种转换是有损耗的，因此使用tr:：addr方法被认为是一种好的方式，它具有类似的效果，但不会“暴露”指针出处。这提高了优化潜力。有关公开指针出处的更多信息，请参阅ptr:：addr和ptr:：expose_addr的文档。如果您的代码不能遵守严格的出处，并且需要公开出处，那么有ptr:∶expose_add作为转义填充，它在明确语义的同时保留了as usinize强制转换的行为。</t>
+          <t>这lint是严格出处工作的一部分，请参阅问题#95228。将指针投射到整数是一种有损操作，因为除了地址之外，指针可能与特定的移动相关联。这些信息被优化器用于动态分析/动态程序验证（例如Miri或CHERI平台）。由于这种转换是有损耗的，因此使用tr:：addr方法被认为是一种好的方式，它具有类似的效果，但不会“暴露”指针出处。这提高了优化潜力。有关公开指针出处的更多信息，请参阅ptr:：addr和ptr:：expose_addr的文档。如果您的代码不能遵守严格的出处，并且需要公开出处，那么有ptr:∶expose_add作为转义填充，它在明确语义的同时保留了as usinize强制转换的行为。</t>
         </is>
       </c>
       <c r="E765" t="inlineStr">
@@ -26283,7 +26283,7 @@
       </c>
       <c r="C766" t="inlineStr">
         <is>
-          <t>const_evaluatable_unchecked lint检测类型中使用的泛型常量。</t>
+          <t>const_evaluatable_uncheckedlint检测类型中使用的泛型常量。</t>
         </is>
       </c>
       <c r="D766" t="inlineStr">
@@ -26318,12 +26318,12 @@
       </c>
       <c r="C767" t="inlineStr">
         <is>
-          <t>function_item_references lint检测使用fmt:：Pointer格式化或已转换的函数引用。</t>
+          <t>function_item_referenceslint检测使用fmt:：Pointer格式化或已转换的函数引用。</t>
         </is>
       </c>
       <c r="D767" t="inlineStr">
         <is>
-          <t>引用一个函数可能会被误认为是获取该函数的一种方法。这可能会在将引用格式化为指针或转换时产生意外结果。当函数引用格式化为指示器、作为fmt:：pointer绑定的参数传递或转换时，会发出此lint。</t>
+          <t>引用一个函数可能会被误认为是获取该函数的一种方法。将引用格式化为指针或转换时，这可能会产生意外结果。当函数引用格式化为指示器、作为fmt:：pointer绑定的参数传递或转换时会出现此lint。</t>
         </is>
       </c>
       <c r="E767" t="inlineStr">
@@ -26347,7 +26347,7 @@
       </c>
       <c r="C768" t="inlineStr">
         <is>
-          <t>未占用静态lint检测未占用静态。</t>
+          <t>无人静态lint检测无人静态。</t>
         </is>
       </c>
       <c r="D768" t="inlineStr">
@@ -26376,7 +26376,7 @@
       </c>
       <c r="C769" t="inlineStr">
         <is>
-          <t>useless_deprecated lint检测无效的弃用属性。</t>
+          <t>useless_deprecatedlint检测无效的弃用属性。</t>
         </is>
       </c>
       <c r="D769" t="inlineStr">
@@ -26408,7 +26408,7 @@
       </c>
       <c r="C770" t="inlineStr">
         <is>
-          <t>undefined_naked_function_abi lint检测不指定abi或指定Rust abi的裸函数定义。</t>
+          <t>undefined_naked_function_abilint检测不指定abi或指定Rust abi的裸函数定义。</t>
         </is>
       </c>
       <c r="D770" t="inlineStr">
@@ -26443,7 +26443,7 @@
       </c>
       <c r="C771" t="inlineStr">
         <is>
-          <t>invalid_unstable_trait_impl lint检测未使用的#[不稳定]属性。</t>
+          <t>invalidate_unstable_trait_impllint检测未使用的#[不稳定]属性。</t>
         </is>
       </c>
       <c r="D771" t="inlineStr">
@@ -26474,12 +26474,12 @@
       </c>
       <c r="C772" t="inlineStr">
         <is>
-          <t>当在表达式位置调用宏时，分号_in_expressions_from_macros lint在宏体中检测到尾随分号。这是以前接受的，但正在逐步取消。</t>
+          <t>当在表达式位置调用宏时，分号_in_expressions_from_macroslint在宏体中检测到尾随分号。这是以前接受的，但正在逐步取消。</t>
         </is>
       </c>
       <c r="D772" t="inlineStr">
         <is>
-          <t>以前，当在表达式位置调用宏时，Rust忽略了宏体中的尾部分号。然而，这使得语言中对分号的处理不一致，并可能在某些情况下导致意外的运行时行为（例如，如果宏作者期望删除值）。这是一个未来不兼容的lint，可以在将来将其转换为一个硬错误。有关更多详细信息，请参阅第79813期。</t>
+          <t>以前，当在表达式位置调用宏时，Rust忽略了宏体中的尾部分号。然而，这使得语言中对分号的处理不一致，并可能在某些情况下导致意外的运行时行为（例如，如果宏作者期望删除值）。这是未来不兼容的lint，可以在未来将其转换为硬错误。有关更多详细信息，请参阅第79813期。</t>
         </is>
       </c>
       <c r="E772" t="inlineStr">
@@ -26509,7 +26509,7 @@
       </c>
       <c r="C773" t="inlineStr">
         <is>
-          <t>legacy_derive_helpers lint检测在引入之前使用的派生助手属性。</t>
+          <t>legacy_derive_helperslint检测在引入之前使用的派生助手属性。</t>
         </is>
       </c>
       <c r="D773" t="inlineStr">
@@ -26546,12 +26546,12 @@
       </c>
       <c r="C774" t="inlineStr">
         <is>
-          <t>large_assignments lint检测何时移动大型对象。</t>
+          <t>large_assignmentslint检测大型对象何时移动。</t>
         </is>
       </c>
       <c r="D774" t="inlineStr">
         <is>
-          <t>当在纯赋值或函数参数中使用大型类型时，惯用代码可能效率低下。理想情况下，适当的优化可以解决此问题，但此类优化只能以尽最大努力的方式进行。此lint将在所有大型移动的站点上触发，从而允许用户在代码中解决这些问题。</t>
+          <t>当在纯赋值或函数参数中使用大类型时，惯用代码可能效率低下。理想情况下，适当的优化可以解决此问题，但此类优化只能以尽最大努力的方式进行。这lint将在所有大移动的站点上触发，从而允许用户在代码中解决它们。</t>
         </is>
       </c>
       <c r="E774" t="inlineStr">
@@ -26578,12 +26578,12 @@
       </c>
       <c r="C775" t="inlineStr">
         <is>
-          <t>depleted_cfg_attr_crate_type_name lint检测#！[cfg_attr（…，crate_type=“…”）]和#！[cfg_attr（…，crate_name=“…”）]属性在源代码中有条件地指定板条箱类型和名称。</t>
+          <t>depleted_cfg_attr_crate_type_namelint检测#！[cfg_attr（…，crate_type=“…”）]和#！[cfg_attr（…，crate_name=“…”）]属性在源代码中有条件地指定crate类型和名称。</t>
         </is>
       </c>
       <c r="D775" t="inlineStr">
         <is>
-          <t>#！[crate_type]和#！[板条箱名称]属性需要在编译器中进行破解，才能在宏扩展后更改使用的板条箱类型和板条箱名称。这两个属性都不能与Cargo结合使用，因为它在命令行上显式传递--crate type和--crate name。这些值必须与源代码中使用的值匹配，以防止出现错误。若要修复警告，请在运行grustc时在命令行中使用--crate类型，而不是#！[cfg_attr（…，crate_type=“…”）]和--机箱名称，而不是#！[cfg_attr（…，crate_name=“…”）]。</t>
+          <t>#！[crate_type]和#！[crate_name]属性需要在编译器中进行破解，才能在宏扩展后更改所使用的crate类型和crat名称。这两个属性都不能与Cargo结合使用，因为它在命令行上显式传递--crate type和--crate name。这些值必须与源代码中使用的值匹配，以防止出现错误。若要修复警告，请在运行grustc时在命令行中使用--crate类型，而不是#！[cfg_attr（…，crate_type=“…”）]和--机箱名称，而不是#！[cfg_attr（…，crate_name=“…”）]。</t>
         </is>
       </c>
       <c r="E775" t="inlineStr">
@@ -26604,12 +26604,12 @@
       </c>
       <c r="C776" t="inlineStr">
         <is>
-          <t>意外的_cfgs lint检测到意外的条件编译条件。</t>
+          <t>意外的_cfgslint检测到意外的条件编译条件。</t>
         </is>
       </c>
       <c r="D776" t="inlineStr">
         <is>
-          <t>只有当--check cfg='names（…）'选项已传递给编译器时，此lint才处于活动状态，并在使用未知条件名称或值时触发。已知条件包括传入的名称或值--check cfg、--cfg，以及一些众所周知的编译器中内置的名称和值。</t>
+          <t>此lint仅在将--check cfg='names（…）'选项传递给编译器时才处于活动状态，并在使用未知条件名称或值时触发。已知条件包括传入的名称或值--check cfg、--cfg，以及一些众所周知的编译器中内置的名称和值。</t>
         </is>
       </c>
       <c r="E776" t="inlineStr">
@@ -26645,7 +26645,7 @@
       </c>
       <c r="D777" t="inlineStr">
         <is>
-          <t>以前，Rust接受包含外部私有零大小类型的字段，尽管在该私有类型中添加非零大小字段不应该是一个突破性的更改。这是一个未来不兼容的lint，将其转换为未来的一个硬错误。有关更多详细信息，请参阅第78586期。</t>
+          <t>以前，Rust接受包含外部私有零大小类型的字段，尽管在该私有类型中添加非零大小字段不应该是一个突破性的更改。这是未来不兼容的lint，将其转换为未来的一个硬错误。有关更多详细信息，请参阅第78586期。</t>
         </is>
       </c>
       <c r="E777" t="inlineStr">
@@ -26684,12 +26684,12 @@
       </c>
       <c r="C778" t="inlineStr">
         <is>
-          <t>unstatible_syntax_pre_expansion lint检测到在属性扩展期间丢弃的unstatiblesyntax的使用。</t>
+          <t>unstatible_syntax_pre_expansionlint检测到在属性扩展期间丢弃的unstatiblesyntax的使用。</t>
         </is>
       </c>
       <c r="D778" t="inlineStr">
         <is>
-          <t>活动属性（如#[cfg]或过程宏属性）的输入必须是有效语法。以前，编译器只有在解析#[cfg]门并扩展过程宏之后才允许使用不稳定的语法功能。为了避免依赖不稳定的句法，请将不稳定语法的使用移到编译器不解析语法的位置，例如函数式宏。##！[deniy（unstatible_syntax_pre_expansion）]macro_rules！identity｛（$（$tokens:tt）*）=&gt;｛$（$tokens）*｝#[cfg（FALSE）]identity！｛macro foo（）｛｝｝这是一个未来不兼容的lint，将其转换为未来的硬错误。有关更多详细信息，请参阅第65860期。</t>
+          <t>活动属性（如#[cfg]或过程宏属性）的输入必须是有效语法。以前，编译器只有在解析#[cfg]门并扩展过程宏之后才允许使用不稳定的语法功能。为了避免依赖不稳定的句法，请将不稳定语法的使用移到编译器不解析语法的位置，例如函数式宏。##！[deniy（unstatible_syntax_pre_expansion）]macro_rules！identity｛（$（$tokens:tt）*）=&gt;｛$（$tokens）*｝#[cfg（FALSE）]identity！｛macro foo（）｛｝｝这是一个未来不兼容的lint，可以在未来将其转换为一个硬错误。有关更多详细信息，请参阅第65860期。</t>
         </is>
       </c>
       <c r="E778" t="inlineStr">
@@ -26711,12 +26711,12 @@
       </c>
       <c r="C779" t="inlineStr">
         <is>
-          <t>模糊_glob_reexports lint检测通过globscollide重新导出名称的情况。下游用户试图使用从多个globswire重新导出的相同名称，将收到一条警告，指出重新定义了相同的名称。</t>
+          <t>模糊_glob_reexportslint检测名称通过globscollide重新导出的情况。下游用户试图使用从多个globswire重新导出的相同名称，将收到一条警告，指出重新定义了相同的名称。</t>
         </is>
       </c>
       <c r="D779" t="inlineStr">
         <is>
-          <t>这是以前接受的，但它可能会无声地破坏机箱的下游用户代码。例如，如果在将bar:：X添加到导出之前重新导出了foo:：*和bar:：*，则下游用户可以毫无问题地使用This_rate:：X。但是，添加bar:：X会导致下游板条箱中的编译错误，因为X在this_rate的同一命名空间中被多次定义。</t>
+          <t>这是以前接受的，但它可能会无声地破坏机箱的下游用户代码。例如，如果在将bar:：X添加到导出之前重新导出了foo:：*和bar:：*，则下游用户可以毫无问题地使用This_rate:：X。但是，添加bar:：X会导致下游crates中的编译错误，因为X在this_rate的同一命名空间中被多次定义。</t>
         </is>
       </c>
       <c r="E779" t="inlineStr">
@@ -26747,7 +26747,7 @@
       </c>
       <c r="C780" t="inlineStr">
         <is>
-          <t>unused_doc_comments lint检测rustdoc未使用的文档注释。</t>
+          <t>unused_doc_commentslint检测rustdoc未使用的文档注释。</t>
         </is>
       </c>
       <c r="D780" t="inlineStr">
@@ -26774,7 +26774,7 @@
       </c>
       <c r="C781" t="inlineStr">
         <is>
-          <t>rust_2021_incomptible_closure_captures lint检测在rust 2021中未完全捕获的变量，因此它们的字段的Drop顺序在rust 2018和2021之间可能不同。它还可以检测变量何时实现了类似Send的特性，但它的一个字段没有，并且该字段由闭包捕获并且在假设所述字段实现与根变量相同的特性的情况下使用。</t>
+          <t>rust_2021_incomptible_closure_captureslint检测在rust 2021中未完全捕获的变量，因此它们的字段的Drop顺序在rust 2018和2021之间可能不同。它还可以检测变量何时实现了类似Send的特性，但它的一个字段没有，并且该字段由闭包捕获并且在假设所述字段实现与根变量相同的特性的情况下使用。</t>
         </is>
       </c>
       <c r="D781" t="inlineStr">
@@ -26810,7 +26810,7 @@
       </c>
       <c r="C782" t="inlineStr">
         <is>
-          <t>missing_abi lint检测从外部声明中省略abi的情况。</t>
+          <t>missing_abilint检测从外部声明中省略abi的情况。</t>
         </is>
       </c>
       <c r="D782" t="inlineStr">
@@ -26837,12 +26837,12 @@
       </c>
       <c r="C783" t="inlineStr">
         <is>
-          <t>invalid_doc_attributes lint检测#[doc（…）]何时被使用。</t>
+          <t>invalid_doc_attributeslint检测#[doc（…）]何时被使用。</t>
         </is>
       </c>
       <c r="D783" t="inlineStr">
         <is>
-          <t>以前，没有验证#[doc（..）]属性的错误用法。通常，这些应该被视为硬错误而拒绝，但引入这种lint是为了避免破坏包括它们在内的任何现有速率。这是一种[未来不兼容]lint，可以在未来将其转变为硬错误。有关更多详细信息，请参阅第82730期。</t>
+          <t>以前，没有验证#[doc（..）]属性的错误用法。通常，这些应该作为硬错误被拒绝，但引入lint是为了避免破坏包括它们在内的任何现有速率。这是一个[future-incompatible]lint来将其转换为将来的硬错误。有关更多详细信息，请参阅第82730期。</t>
         </is>
       </c>
       <c r="E783" t="inlineStr">
@@ -26866,12 +26866,12 @@
       </c>
       <c r="C784" t="inlineStr">
         <is>
-          <t>proc_macro_back_compat lint检测某些proc宏crate的旧版本的使用，这些旧版本在编译器中有硬编码的解决方案。</t>
+          <t>proc_macro_back_compatlint检测某些proc宏crate的旧版本的使用，这些旧版本在编译器中具有硬编码的解决方案。</t>
         </is>
       </c>
       <c r="D784" t="inlineStr">
         <is>
-          <t>最终，编译器中存在的向后兼容性黑客将被删除，导致某些crate的旧版本停止编译。这是一个未来不兼容的lint，以简化向错误的转换。有关更多详细信息，请参阅问题#83125。</t>
+          <t>最终，编译器中存在的向后兼容性黑客将被删除，导致某些crates的旧版本停止编译。这是一个未来不兼容的lint，以简化向错误的转换。有关更多详细信息，请参阅问题#83125。</t>
         </is>
       </c>
       <c r="E784" t="inlineStr">
@@ -26906,7 +26906,7 @@
       </c>
       <c r="C785" t="inlineStr">
         <is>
-          <t>rust_2012_incompatible_or_patterns lint检测旧版本或模式的使用情况。</t>
+          <t>rust_2012_incompatible_or_patternslint检测旧版本或模式的使用情况。</t>
         </is>
       </c>
       <c r="D785" t="inlineStr">
@@ -26946,7 +26946,7 @@
       </c>
       <c r="C786" t="inlineStr">
         <is>
-          <t>rust_2021_prelude_collisions lint检测到trait方法的使用，这些方法与未来版本中添加到前奏中的trait不明确。</t>
+          <t>rust_2021_prelude_collisionslint检测到特征方法的使用，这些方法与未来版本中添加到前奏中的特征不明确。</t>
         </is>
       </c>
       <c r="D786" t="inlineStr">
@@ -26987,12 +26987,12 @@
       </c>
       <c r="C787" t="inlineStr">
         <is>
-          <t>rust_2012_prefixes_compatible_syntax-lint检测到的标识符将在rust 2021中被解析为aprefix。</t>
+          <t>rust_2021 _prefixes_compatible_syntaxlint检测到将在rust 2021中解析为aprefix的标识符。</t>
         </is>
       </c>
       <c r="D787" t="inlineStr">
         <is>
-          <t>在Rust 2015和2018中，z“嘿”是两个标记：标识符z后面跟着字符串“嘿”。在Rust 2021中，z被认为是“嘿”的前缀。这个lint建议在z和“嘿”标记之间添加空白，以在Rust 2021。</t>
+          <t>在Rust 2015和2018中，z“嘿”是两个标记：标识符z后面跟着字符串“嘿”。在Rust 2021中，z被认为是“嘿”的前缀。这lint建议在z和“嘿”标记之间添加空格，以在Rust 2021。</t>
         </is>
       </c>
       <c r="E787" t="inlineStr">
@@ -27017,7 +27017,7 @@
       </c>
       <c r="C788" t="inlineStr">
         <is>
-          <t>只要在目标上使用了请求的目标无法有效支持的stsdcall、fastcall、thiscall、vectorcall调用约定（或其undundvariant），就会输出unsupported_calling_conventions lint。例如，stdcall对x86_64或更明显的powerpcode没有多大意义，因为从未为这些目标指定过这种调用约定。从历史上看，MSVC工具链在x86以外的目标上已经回到了常规的C调用约定，但Rust并没有真正看到在更多目标上引入类似的黑客攻击的类似需求。</t>
+          <t>只要在目标上使用了请求的目标无法有效支持的stsdcall、fastcall、thiscall、vectorcall调用约定（或其undundvariation），就会输出unsupported_calling_conventionslint。例如，stdcall对x86_64或更明显的powerpcode没有多大意义，因为从未为这些目标指定过这种调用约定。从历史上看，MSVC工具链在x86以外的目标上已经回到了常规的C调用约定，但Rust并没有真正看到在更多目标上引入类似的黑客攻击的类似需求。</t>
         </is>
       </c>
       <c r="D788" t="inlineStr">
@@ -27054,7 +27054,7 @@
       </c>
       <c r="C789" t="inlineStr">
         <is>
-          <t>break_with_label_and_loop lint检测标记的break表达式，并将未标记的循环作为其值表达式。</t>
+          <t>break_with_label_and_looplint检测标记的break表达式，其中一个未标记的循环作为其值表达式。</t>
         </is>
       </c>
       <c r="D789" t="inlineStr">
@@ -27082,7 +27082,7 @@
       </c>
       <c r="C790" t="inlineStr">
         <is>
-          <t>non_exhaustive_omitted_patters lint检测#[non_exhaustive]结构或枚举的模式中的通配符（_或..）何时可访问。</t>
+          <t>non_exhaustive_omitted_patteringslint检测#[non_exhausive]struct或enum的模式中的通配符（_或..）何时可访问。</t>
         </is>
       </c>
       <c r="D790" t="inlineStr">
@@ -27134,7 +27134,7 @@
       </c>
       <c r="C791" t="inlineStr">
         <is>
-          <t>text_direction_codepoint_in_comment lint检测注释中的Unicode代码点，这些代码点以与内存上的文本表示不一致的方式更改屏幕上文本的视觉表示。</t>
+          <t>text_direction_codepoint_in_commentlint检测注释中的Unicode代码点，这些代码点以与内存上的文本表示不一致的方式更改屏幕上文本的视觉表示。</t>
         </is>
       </c>
       <c r="D791" t="inlineStr">
@@ -27163,7 +27163,7 @@
       </c>
       <c r="C792" t="inlineStr">
         <is>
-          <t>duplicate_macro_attributes lint检测类似#[test]的内置宏属性何时在项目上重复。此lint可能在bench、cfg_eval、testand test_case上触发。</t>
+          <t>duplicate_macro_attributeslint检测类似#[test]的内置宏属性何时在项上重复。此lint可能在bench、cfg_eval、testand test_case上触发。</t>
         </is>
       </c>
       <c r="D792" t="inlineStr">
@@ -27199,7 +27199,7 @@
       </c>
       <c r="C793" t="inlineStr">
         <is>
-          <t>可疑的auto_trait_impls lint检查自动特征的潜在错误实现。</t>
+          <t>可疑的auto_trait_implslint检查自动特征的潜在错误实现。</t>
         </is>
       </c>
       <c r="D793" t="inlineStr">
@@ -27226,7 +27226,7 @@
       </c>
       <c r="C794" t="inlineStr">
         <is>
-          <t>depleted_where_clause_location lint检测equals前面的where子句何时为关联类型。</t>
+          <t>depleted_where_clause_locationlint检测前面的where子句何时等于关联类型。</t>
         </is>
       </c>
       <c r="D794" t="inlineStr">
@@ -27257,7 +27257,7 @@
       </c>
       <c r="C795" t="inlineStr">
         <is>
-          <t>test_unstable_lint lint测试不稳定的lint，并且是永久不稳定的。</t>
+          <t>test_unstable_lintlint测试不稳定lints并且是永久不稳定的。</t>
         </is>
       </c>
       <c r="D795" t="inlineStr">
@@ -27283,12 +27283,12 @@
       </c>
       <c r="C796" t="inlineStr">
         <is>
-          <t>ffi_unwind_calls lint检测对具有C展开或其他ffi展开ABI的外部函数或函数指针的调用。</t>
+          <t>ffi_unwind_callslint检测对具有C展开或其他ffi展开ABI的外部函数或函数指针的调用。</t>
         </is>
       </c>
       <c r="D796" t="inlineStr">
         <is>
-          <t>对于包含此类调用的板条箱，如果它们是用-C panic=unlock编译的，则生成的库无法与用-C panic=abort编译的板条箱链接。因此，对于那些希望拥有这种能力的陨石坑来说，有必要避免这样的呼吁。</t>
+          <t>对于包含此类调用的crates，如果它们是用-C panic=unvent编译的，则生成的库无法与用-C panic=abort编译的clates链接。因此，对于那些希望拥有这种能力的陨石坑来说，有必要避免这样的呼吁。</t>
         </is>
       </c>
       <c r="E796" t="inlineStr">
@@ -27317,7 +27317,7 @@
       </c>
       <c r="C797" t="inlineStr">
         <is>
-          <t>named_arguments_used_positionally lint检测命名参数仅在格式字符串中位置使用的情况。这种用法是有效的，但可能非常令人困惑。</t>
+          <t>named_arguments_used_positionallylint检测命名参数仅在格式化字符串中位置使用的情况。这种用法是有效的，但可能非常令人困惑。</t>
         </is>
       </c>
       <c r="D797" t="inlineStr">
@@ -27349,7 +27349,7 @@
       </c>
       <c r="C798" t="inlineStr">
         <is>
-          <t>implied_bounds_entailment lint检测impl方法的参数比其实现的trait方法的参数具有更强的隐含边界的情况。</t>
+          <t>implied_bounds_entailmentlint检测impl方法的参数比其实现的trait方法的参数具有更强的隐含边界的情况。</t>
         </is>
       </c>
       <c r="D798" t="inlineStr">
@@ -27385,12 +27385,12 @@
       </c>
       <c r="C799" t="inlineStr">
         <is>
-          <t>byte_slice_in_packed_struct_with_derive lint检测在导出一个或多个内置特征的压缩结构中使用字节切片字段（[u8]）或字符串切片字段（str）的情况。</t>
+          <t>byte_slice_in_packed_struct_with_derivelint检测在导出一个或多个内置特征的压缩struct中使用字节切片字段（[u8]）或字符串切片字段（str）的情况。</t>
         </is>
       </c>
       <c r="D799" t="inlineStr">
         <is>
-          <t>这以前被接受，但现在正在逐步取消，因为压缩结构中的字段不需要实现Copy才能派生。字节切片和字符串切片是一个罕见的例外，因为某些板条箱依赖于它们。</t>
+          <t>这以前被接受，但现在正在逐步取消，因为压缩结构中的字段不需要实现Copy才能派生。字节切片和字符串切片是一个罕见的例外，因为某些crates依赖于它们。</t>
         </is>
       </c>
       <c r="E799" t="inlineStr">
@@ -27416,7 +27416,7 @@
       </c>
       <c r="C800" t="inlineStr">
         <is>
-          <t>invalid_macro_export_arguments lint检测#[mmacro_export]与无效参数一起使用的情况。</t>
+          <t>invalid_macro_export_argumentslint检测#[mmacro_export]与无效参数一起使用的情况。</t>
         </is>
       </c>
       <c r="D800" t="inlineStr">

</xml_diff>

<commit_message>
remove line starts with "#" in lint examples
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -481,8 +481,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>#[allow(unused_mut)]
-fn foo() -&gt; usize {
+          <t>fn foo() -&gt; usize {
    let mut a = Vec::new();
    a.len()
 }</t>
@@ -490,9 +489,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>#![feature(lint_reasons)]
-#[expect(unused_mut)]
-fn foo() -&gt; usize {
+          <t>fn foo() -&gt; usize {
     let mut a = Vec::new();
     a.len()
 }</t>
@@ -582,22 +579,12 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t># #![feature(asm)]
-# #[cfg(any(target_arch = "x86", target_arch = "x86_64"))]
-# unsafe { let ptr = "".as_ptr();
-# use std::arch::asm;
-asm!("lea {}, [{}]", lateout(reg) _, in(reg) ptr);
-# }</t>
+          <t>asm!("lea {}, [{}]", lateout(reg) _, in(reg) ptr);</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t># #![feature(asm)]
-# #[cfg(any(target_arch = "x86", target_arch = "x86_64"))]
-# unsafe { let ptr = "".as_ptr();
-# use std::arch::asm;
-asm!("lea ({}), {}", in(reg) ptr, lateout(reg) _, options(att_syntax));
-# }</t>
+          <t>asm!("lea ({}), {}", in(reg) ptr, lateout(reg) _, options(att_syntax));</t>
         </is>
       </c>
     </row>
@@ -622,22 +609,12 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t># #![feature(asm)]
-# #[cfg(any(target_arch = "x86", target_arch = "x86_64"))]
-# unsafe { let ptr = "".as_ptr();
-# use std::arch::asm;
-asm!("lea ({}), {}", in(reg) ptr, lateout(reg) _, options(att_syntax));
-# }</t>
+          <t>asm!("lea ({}), {}", in(reg) ptr, lateout(reg) _, options(att_syntax));</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t># #![feature(asm)]
-# #[cfg(any(target_arch = "x86", target_arch = "x86_64"))]
-# unsafe { let ptr = "".as_ptr();
-# use std::arch::asm;
-asm!("lea {}, [{}]", lateout(reg) _, in(reg) ptr);
-# }</t>
+          <t>asm!("lea {}, [{}]", lateout(reg) _, in(reg) ptr);</t>
         </is>
       </c>
     </row>
@@ -691,9 +668,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t># let r = Ok::&lt;_, ()&gt;(());
-assert!(r.is_ok());
-# let r = Err::&lt;_, ()&gt;(());
+          <t>assert!(r.is_ok());
 assert!(r.is_err());</t>
         </is>
       </c>
@@ -794,8 +769,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>#[inline(always)]
-fn not_quite_hot_code(..) { ... }</t>
+          <t>fn not_quite_hot_code(..) { ... }</t>
         </is>
       </c>
       <c r="F11" t="inlineStr"/>
@@ -821,18 +795,13 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>#[deny(dead_code)]
-extern crate foo;
-#[forbid(dead_code)]
+          <t>extern crate foo;
 use foo::bar;</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>#[allow(unused_imports)]
-use foo::baz;
-#[allow(unused_imports)]
-#[macro_use]
+          <t>use foo::baz;
 extern crate baz;</t>
         </is>
       </c>
@@ -858,8 +827,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>#[deprecated(since = "forever")]
-fn something_else() { /* ... */ }</t>
+          <t>fn something_else() { /* ... */ }</t>
         </is>
       </c>
       <c r="F13" t="inlineStr"/>
@@ -885,18 +853,15 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>#[allow(dead_code)]
-fn not_quite_good_code() { }</t>
+          <t>fn not_quite_good_code() { }</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
           <t>// Good (as inner attribute)
-#![allow(dead_code)]
 fn this_is_fine() { }
 // or
 // Good (as outer attribute)
-#[allow(dead_code)]
 fn this_is_fine_too() { }</t>
         </is>
       </c>
@@ -956,16 +921,8 @@
           <t>限制性lints有时与其他lint形成对比，甚至与惯用的铁锈相反。这些linth只能在逐个皮棉的基础上启用，并经过仔细考虑。</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>#![deny(clippy::restriction)]</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>#![deny(clippy::as_conversions)]</t>
-        </is>
-      </c>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -988,14 +945,12 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>#[cfg_attr(rustfmt, rustfmt_skip)]
-fn main() { }</t>
+          <t>fn main() { }</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>#[rustfmt::skip]
-fn main() { }</t>
+          <t>fn main() { }</t>
         </is>
       </c>
     </row>
@@ -1020,18 +975,13 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>#[cfg(linux)]
-fn conditional() { }</t>
+          <t>fn conditional() { }</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t># mod hidden {
-#[cfg(target_os = "linux")]
-fn conditional() { }
-# }
+          <t>fn conditional() { }
 // or
-#[cfg(unix)]
 fn conditional() { }
 Check the Rust Reference for more details.</t>
         </is>
@@ -1056,18 +1006,8 @@
           <t>允许lint应该总是有原因的。应记录此原因，以确保其他人理解其原因</t>
         </is>
       </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>#![feature(lint_reasons)]
-#![allow(clippy::some_lint)]</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>#![feature(lint_reasons)]
-#![allow(clippy::some_lint, reason = "False positive rust-lang/rust-clippy#1002020")]</t>
-        </is>
-      </c>
+      <c r="E19" t="inlineStr"/>
+      <c r="F19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -1090,14 +1030,12 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>#[cfg(any(unix))]
-pub struct Bar;</t>
+          <t>pub struct Bar;</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>#[cfg(unix)]
-pub struct Bar;</t>
+          <t>pub struct Bar;</t>
         </is>
       </c>
     </row>
@@ -1122,9 +1060,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t># use std::sync::Mutex;
-# async fn baz() {}
-async fn foo(x: &amp;Mutex&lt;u32&gt;) {
+          <t>async fn foo(x: &amp;Mutex&lt;u32&gt;) {
   let mut guard = x.lock().unwrap();
   *guard += 1;
   baz().await;
@@ -1139,9 +1075,7 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t># use std::sync::Mutex;
-# async fn baz() {}
-async fn foo(x: &amp;Mutex&lt;u32&gt;) {
+          <t>async fn foo(x: &amp;Mutex&lt;u32&gt;) {
   {
     let mut guard = x.lock().unwrap();
     *guard += 1;
@@ -1179,9 +1113,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t># use std::cell::RefCell;
-# async fn baz() {}
-async fn foo(x: &amp;RefCell&lt;u32&gt;) {
+          <t>async fn foo(x: &amp;RefCell&lt;u32&gt;) {
   let mut y = x.borrow_mut();
   *y += 1;
   baz().await;
@@ -1196,9 +1128,7 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t># use std::cell::RefCell;
-# async fn baz() {}
-async fn foo(x: &amp;RefCell&lt;u32&gt;) {
+          <t>async fn foo(x: &amp;RefCell&lt;u32&gt;) {
   {
      let mut y = x.borrow_mut();
      *y += 1;
@@ -1242,7 +1172,6 @@
   # You can (optionally) specify a reason
   { path = "OtherCustomLockType", reason = "Relies on a thread local" }
 ]
-# async fn baz() {}
 struct CustomLockType;
 struct OtherCustomLockType;
 async fn foo() {
@@ -1275,15 +1204,13 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t># fn somefunc() -&gt; bool { true };
-if { true } { /* ... */ }
+          <t>if { true } { /* ... */ }
 if { let x = somefunc(); x } { /* ... */ }</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t># fn somefunc() -&gt; bool { true };
-if true { /* ... */ }
+          <t>if true { /* ... */ }
 let res = { let x = somefunc(); x };
 if res { /* ... */ }</t>
         </is>
@@ -1404,8 +1331,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t># let condition = false;
-if condition {
+          <t>if condition {
     1_i64
 } else {
     0
@@ -1414,10 +1340,8 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t># let condition = false;
-i64::from(condition);
+          <t>i64::from(condition);
 or
-# let condition = false;
 condition as i64;</t>
         </is>
       </c>
@@ -1449,8 +1373,7 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t># let s = &amp;String::new();
-let a: &amp;String = s;</t>
+          <t>let a: &amp;String = s;</t>
         </is>
       </c>
     </row>
@@ -1505,15 +1428,12 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t># let foo: u32 = 5;
-foo &lt;= i32::MAX as u32;</t>
+          <t>foo &lt;= i32::MAX as u32;</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t># let foo = 1;
-# #[allow(unused)]
-i32::try_from(foo).is_ok();</t>
+          <t>i32::try_from(foo).is_ok();</t>
         </is>
       </c>
     </row>
@@ -1564,8 +1484,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t># let (x, y) = (true, true);
-if x {
+          <t>if x {
     if y {
         // …
     }
@@ -1574,8 +1493,7 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t># let (x, y) = (true, true);
-if x &amp;&amp; y {
+          <t>if x &amp;&amp; y {
     // …
 }</t>
         </is>
@@ -1642,8 +1560,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t># let samples = vec![3, 1, 2];
-let mut sorted_samples = samples.clone();
+          <t>let mut sorted_samples = samples.clone();
 sorted_samples.sort();
 for sample in &amp;samples { // Oops, meant to use `sorted_samples`.
     println!("{sample}");
@@ -1652,8 +1569,7 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t># let samples = vec![3, 1, 2];
-let mut sorted_samples = samples.clone();
+          <t>let mut sorted_samples = samples.clone();
 sorted_samples.sort();
 for sample in &amp;sorted_samples {
     println!("{sample}");
@@ -1682,10 +1598,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t># fn a() {}
-# fn b() {}
-# fn c() {}
-fn f(x: u8, y: u8) {
+          <t>fn f(x: u8, y: u8) {
     if x &gt; y {
         a()
     } else if x &lt; y {
@@ -1699,9 +1612,6 @@
       <c r="F36" t="inlineStr">
         <is>
           <t>use std::cmp::Ordering;
-# fn a() {}
-# fn b() {}
-# fn c() {}
 fn f(x: u8, y: u8) {
      match x.cmp(&amp;y) {
          Ordering::Greater =&gt; a(),
@@ -1889,8 +1799,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>#[derive(Copy, Clone)]
-struct Countdown(u8);
+          <t>struct Countdown(u8);
 impl Iterator for Countdown {
     // ...
 }
@@ -1921,8 +1830,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>#[macro_export]
-macro_rules! print_message {
+          <t>macro_rules! print_message {
     () =&gt; {
         println!("{}", crate::MESSAGE);
     };
@@ -1932,8 +1840,7 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>#[macro_export]
-macro_rules! print_message {
+          <t>macro_rules! print_message {
     () =&gt; {
         println!("{}", $crate::MESSAGE);
     };
@@ -1941,7 +1848,6 @@
 pub const MESSAGE: &amp;str = "Hello!";
 Note that if the use of crate is intentional, an allow attribute can be applied to the
 macro definition, e.g.:
-#[allow(clippy::crate_in_macro_def)]
 macro_rules! ok { ... crate::foo ... }</t>
         </is>
       </c>
@@ -2057,17 +1963,13 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t># #[derive(Default)]
-# struct A { i: i32 }
-let mut a: A = Default::default();
+          <t>let mut a: A = Default::default();
 a.i = 42;</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t># #[derive(Default)]
-# struct A { i: i32 }
-let a = A {
+          <t>let a = A {
     i: 42,
     .. Default::default()
 };</t>
@@ -2095,9 +1997,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t># use std::marker::PhantomData;
-#[derive(Default)]
-struct S&lt;T&gt; {
+          <t>struct S&lt;T&gt; {
     _marker: PhantomData&lt;T&gt;
 }
 let _: S&lt;i32&gt; = S {
@@ -2107,8 +2007,7 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t># use std::marker::PhantomData;
-struct S&lt;T&gt; {
+          <t>struct S&lt;T&gt; {
     _marker: PhantomData&lt;T&gt;
 }
 let _: S&lt;i32&gt; = S {
@@ -2215,8 +2114,7 @@
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>#[repr(C)]
-union Foo {
+          <t>union Foo {
     a: i32,
     b: u32,
 }
@@ -2291,8 +2189,7 @@
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t># fn fun(_a: &amp;i32) {}
-let x: &amp;i32 = &amp;5;
+          <t>let x: &amp;i32 = &amp;5;
 fun(x);</t>
         </is>
       </c>
@@ -2400,8 +2297,7 @@
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>#[derive(Default)]
-struct Foo {
+          <t>struct Foo {
     bar: bool
 }</t>
         </is>
@@ -2428,8 +2324,7 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>#[derive(Hash)]
-struct Foo;
+          <t>struct Foo;
 impl PartialEq for Foo {
     ...
 }</t>
@@ -2458,8 +2353,7 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>#[derive(Ord, PartialEq, Eq)]
-struct Foo;
+          <t>struct Foo;
 impl PartialOrd for Foo {
     ...
 }</t>
@@ -2467,8 +2361,7 @@
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>#[derive(PartialEq, Eq)]
-struct Foo;
+          <t>struct Foo;
 impl PartialOrd for Foo {
     fn partial_cmp(&amp;self, other: &amp;Foo) -&gt; Option&lt;Ordering&gt; {
        Some(self.cmp(other))
@@ -2478,7 +2371,6 @@
     ...
 }
 or, if you don't need a custom ordering:
-#[derive(Ord, PartialOrd, PartialEq, Eq)]
 struct Foo;</t>
         </is>
       </c>
@@ -2504,8 +2396,7 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>#[derive(Copy)]
-struct Foo;
+          <t>struct Foo;
 impl Clone for Foo {
     // ..
 }</t>
@@ -2535,7 +2426,6 @@
       <c r="E59" t="inlineStr">
         <is>
           <t>use serde::Deserialize;
-#[derive(Deserialize)]
 pub struct Foo {
     // ..
 }
@@ -2572,8 +2462,7 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>#[derive(PartialEq)]
-struct Foo {
+          <t>struct Foo {
     i_am_eq: i32,
     i_am_eq_too: Vec&lt;String&gt;,
 }</t>
@@ -2581,8 +2470,7 @@
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>#[derive(PartialEq, Eq)]
-struct Foo {
+          <t>struct Foo {
     i_am_eq: i32,
     i_am_eq_too: Vec&lt;String&gt;,
 }</t>
@@ -2611,7 +2499,6 @@
       <c r="E61" t="inlineStr">
         <is>
           <t>An example clippy.toml configuration:
-# clippy.toml
 disallowed-macros = [
     # Can use a string as the path of the disallowed macro.
     "std::print",
@@ -2625,7 +2512,6 @@
 // Example code where clippy issues a warning
 println!("warns");
 // The diagnostic will contain the message "no serializing"
-#[derive(Serialize)]
 struct Data {
     name: String,
     value: usize,
@@ -2656,7 +2542,6 @@
       <c r="E62" t="inlineStr">
         <is>
           <t>An example clippy.toml configuration:
-# clippy.toml
 disallowed-methods = [
     # Can use a string as the path of the disallowed method.
     "std::boxed::Box::new",
@@ -2761,7 +2646,6 @@
       <c r="E65" t="inlineStr">
         <is>
           <t>An example clippy.toml configuration:
-# clippy.toml
 disallowed-types = [
     # Can use a string as the path of the disallowed type.
     "std::collections::BTreeMap",
@@ -3059,7 +2943,6 @@
           <t>fn simple_double_parens() -&gt; i32 {
     ((0))
 }
-# fn foo(bar: usize) {}
 foo((0));</t>
         </is>
       </c>
@@ -3068,7 +2951,6 @@
           <t>fn simple_no_parens() -&gt; i32 {
     0
 }
-# fn foo(bar: usize) {}
 foo(0);</t>
         </is>
       </c>
@@ -3188,7 +3070,6 @@
 mod a;
 mod b;
 // a.rs
-#[path = "./b.rs"]
 mod b;</t>
         </is>
       </c>
@@ -3223,10 +3104,7 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t># fn a() {}
-# fn b() {}
-# let x: i32 = 1;
-if x.is_positive() {
+          <t>if x.is_positive() {
     a();
 } else if x.is_negative() {
     b();
@@ -3235,10 +3113,7 @@
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t># fn a() {}
-# fn b() {}
-# let x: i32 = 1;
-if x.is_positive() {
+          <t>if x.is_positive() {
     a();
 } else if x.is_negative() {
     b();
@@ -3307,8 +3182,7 @@
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>#![feature(never_type)]
-struct Test(!);</t>
+          <t>struct Test(!);</t>
         </is>
       </c>
     </row>
@@ -3363,22 +3237,14 @@
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t># use std::collections::HashMap;
-# let mut map = HashMap::new();
-# let k = 1;
-# let v = 1;
-if !map.contains_key(&amp;k) {
+          <t>if !map.contains_key(&amp;k) {
     map.insert(k, v);
 }</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t># use std::collections::HashMap;
-# let mut map = HashMap::new();
-# let k = 1;
-# let v = 1;
-map.entry(k).or_insert(v);</t>
+          <t>map.entry(k).or_insert(v);</t>
         </is>
       </c>
     </row>
@@ -3403,9 +3269,7 @@
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t># #[cfg(target_pointer_width = "64")]
-#[repr(usize)]
-enum NonPortable {
+          <t>enum NonPortable {
     X = 0x1_0000_0000,
     Y = 0,
 }</t>
@@ -3744,8 +3608,7 @@
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>#[non_exhaustive]
-enum Foo {
+          <t>enum Foo {
     Bar,
     Baz
 }</t>
@@ -3781,8 +3644,7 @@
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>#[non_exhaustive]
-struct Foo {
+          <t>struct Foo {
     bar: u8,
     baz: String,
 }</t>
@@ -3845,17 +3707,13 @@
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t># use std::io::Write;
-# let bar = "furchtbar";
-writeln!(&amp;mut std::io::stderr(), "foo: {:?}", bar).unwrap();
+          <t>writeln!(&amp;mut std::io::stderr(), "foo: {:?}", bar).unwrap();
 writeln!(&amp;mut std::io::stdout(), "foo: {:?}", bar).unwrap();</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t># use std::io::Write;
-# let bar = "furchtbar";
-eprintln!("foo: {:?}", bar);
+          <t>eprintln!("foo: {:?}", bar);
 println!("foo: {:?}", bar);</t>
         </is>
       </c>
@@ -4207,17 +4065,13 @@
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t># let foo = true;
-# let bar = false;
-// &amp;&amp;! looks like a different operator
+          <t>// &amp;&amp;! looks like a different operator
 if foo &amp;&amp;! bar {}</t>
         </is>
       </c>
       <c r="F106" t="inlineStr">
         <is>
-          <t># let foo = true;
-# let bar = false;
-if foo &amp;&amp; !bar {}</t>
+          <t>if foo &amp;&amp; !bar {}</t>
         </is>
       </c>
     </row>
@@ -4310,14 +4164,12 @@
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t># use std::panic::Location;
-println!("error: {}", format!("something failed at {}", Location::caller()));</t>
+          <t>println!("error: {}", format!("something failed at {}", Location::caller()));</t>
         </is>
       </c>
       <c r="F109" t="inlineStr">
         <is>
-          <t># use std::panic::Location;
-println!("error: something failed at {}", Location::caller());</t>
+          <t>println!("error: something failed at {}", Location::caller());</t>
         </is>
       </c>
     </row>
@@ -4342,14 +4194,12 @@
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t># use std::panic::Location;
-println!("error: something failed at {}", Location::caller().to_string());</t>
+          <t>println!("error: something failed at {}", Location::caller().to_string());</t>
         </is>
       </c>
       <c r="F110" t="inlineStr">
         <is>
-          <t># use std::panic::Location;
-println!("error: something failed at {}", Location::caller());</t>
+          <t>println!("error: something failed at {}", Location::caller());</t>
         </is>
       </c>
     </row>
@@ -4374,10 +4224,7 @@
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t># let var = 42;
-# let width = 1;
-# let prec = 2;
-format!("{}", var);
+          <t>format!("{}", var);
 format!("{v:?}", v = var);
 format!("{0} {0}", var);
 format!("{0:1$}", var, width);
@@ -4386,8 +4233,7 @@
       </c>
       <c r="F111" t="inlineStr">
         <is>
-          <t># let var = 42;
-format!("{var} {}", 1+2);</t>
+          <t>format!("{var} {}", 1+2);</t>
         </is>
       </c>
     </row>
@@ -4606,16 +4452,13 @@
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t># use std::ffi::c_void;
-let ptr = Box::into_raw(Box::new(42usize)) as *mut c_void;
+          <t>let ptr = Box::into_raw(Box::new(42usize)) as *mut c_void;
 let _ = unsafe { Box::from_raw(ptr) };</t>
         </is>
       </c>
       <c r="F117" t="inlineStr">
         <is>
-          <t># use std::ffi::c_void;
-# let ptr = Box::into_raw(Box::new(42usize)) as *mut c_void;
-let _ = unsafe { Box::from_raw(ptr as *mut usize) };</t>
+          <t>let _ = unsafe { Box::from_raw(ptr as *mut usize) };</t>
         </is>
       </c>
     </row>
@@ -4739,10 +4582,7 @@
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t># let v: Vec&lt;usize&gt; = vec![];
-# fn a() {}
-# fn b() {}
-if !v.is_empty() {
+          <t>if !v.is_empty() {
     a()
 } else {
     b()
@@ -4751,10 +4591,7 @@
       </c>
       <c r="F121" t="inlineStr">
         <is>
-          <t># let v: Vec&lt;usize&gt; = vec![];
-# fn a() {}
-# fn b() {}
-if v.is_empty() {
+          <t>if v.is_empty() {
     b()
 } else {
     a()
@@ -4783,8 +4620,7 @@
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t># let v = vec![0];
-let a = if v.is_empty() {
+          <t>let a = if v.is_empty() {
     println!("true!");
     Some(42)
 } else {
@@ -4794,8 +4630,7 @@
       </c>
       <c r="F122" t="inlineStr">
         <is>
-          <t># let v = vec![0];
-let a = v.is_empty().then(|| {
+          <t>let a = v.is_empty().then(|| {
     println!("true!");
     42
 });</t>
@@ -4823,15 +4658,9 @@
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t># use std::collections::HashMap;
-# use std::hash::{Hash, BuildHasher};
-# trait Serialize {};
-impl&lt;K: Hash + Eq, V&gt; Serialize for HashMap&lt;K, V&gt; { }
+          <t>impl&lt;K: Hash + Eq, V&gt; Serialize for HashMap&lt;K, V&gt; { }
 pub fn foo(map: &amp;mut HashMap&lt;i32, i32&gt;) { }
 could be rewritten as
-# use std::collections::HashMap;
-# use std::hash::{Hash, BuildHasher};
-# trait Serialize {};
 impl&lt;K: Hash + Eq, V, S: BuildHasher&gt; Serialize for HashMap&lt;K, V, S&gt; { }
 pub fn foo&lt;S: BuildHasher&gt;(map: &amp;mut HashMap&lt;i32, i32, S&gt;) { }</t>
         </is>
@@ -4925,9 +4754,7 @@
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t># let end: u32 = 10;
-# let start: u32 = 5;
-let mut i: u32 = end - start;
+          <t>let mut i: u32 = end - start;
 if i != 0 {
     i -= 1;
 }</t>
@@ -4935,9 +4762,7 @@
       </c>
       <c r="F126" t="inlineStr">
         <is>
-          <t># let end: u32 = 10;
-# let start: u32 = 5;
-let mut i: u32 = end - start;
+          <t>let mut i: u32 = end - start;
 i = i.saturating_sub(1);</t>
         </is>
       </c>
@@ -4974,13 +4799,7 @@
       </c>
       <c r="F127" t="inlineStr">
         <is>
-          <t># struct Foo {
-#     x: i32,
-#     y: i32,
-# }
-# let x = 1;
-# let y = 2;
-Foo { x, y };</t>
+          <t>Foo { x, y };</t>
         </is>
       </c>
     </row>
@@ -5012,8 +4831,7 @@
       </c>
       <c r="F128" t="inlineStr">
         <is>
-          <t># let x = [1, 2, 3, 4];
-// Index within bounds
+          <t>// Index within bounds
 x[0];
 x[3];</t>
         </is>
@@ -5052,10 +4870,7 @@
       </c>
       <c r="F129" t="inlineStr">
         <is>
-          <t># #![allow(unused)]
-# let x = vec![0; 5];
-# let y = [0, 1, 2, 3];
-x.get(2);
+          <t>x.get(2);
 x.get(2..100);
 y.get(10);
 y.get(10..100);</t>
@@ -5147,7 +4962,6 @@
       <c r="E132" t="inlineStr">
         <is>
           <t>let infinite_iter = 0..;
-# #[allow(unused)]
 [0..].iter().zip(infinite_iter.take_while(|x| *x &gt; 5));</t>
         </is>
       </c>
@@ -5401,14 +5215,12 @@
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t># use std::time::{Instant, Duration};
-let time_passed = Instant::now() - Duration::from_secs(5);</t>
+          <t>let time_passed = Instant::now() - Duration::from_secs(5);</t>
         </is>
       </c>
       <c r="F139" t="inlineStr">
         <is>
-          <t># use std::time::{Instant, Duration};
-let time_passed = Instant::now().checked_sub(Duration::from_secs(5));</t>
+          <t>let time_passed = Instant::now().checked_sub(Duration::from_secs(5));</t>
         </is>
       </c>
     </row>
@@ -5433,16 +5245,12 @@
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t># let x = 1;
-# let y = 1;
-if x &gt;= y + 1 {}</t>
+          <t>if x &gt;= y + 1 {}</t>
         </is>
       </c>
       <c r="F140" t="inlineStr">
         <is>
-          <t># let x = 1;
-# let y = 1;
-if x &gt; y {}</t>
+          <t>if x &gt; y {}</t>
         </is>
       </c>
     </row>
@@ -5494,8 +5302,7 @@
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t># #[allow(unused)]
-unsafe {
+          <t>unsafe {
     std::str::from_utf8_unchecked(b"cl\x82ippy");
 }</t>
         </is>
@@ -5571,8 +5378,7 @@
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>#[cfg(test)]
-mod tests {
+          <t>mod tests {
     // [...]
 }
 fn my_function() {
@@ -5585,7 +5391,6 @@
           <t>fn my_function() {
     // [...]
 }
-#[cfg(test)]
 mod tests {
     // [...]
 }</t>
@@ -6043,12 +5848,10 @@
       </c>
       <c r="F157" t="inlineStr">
         <is>
-          <t># async fn context() {
-async fn foo() -&gt; Result&lt;(), ()&gt; {
+          <t>async fn foo() -&gt; Result&lt;(), ()&gt; {
     Ok(())
 }
-let _ = foo().await;
-# }</t>
+let _ = foo().await;</t>
         </is>
       </c>
     </row>
@@ -6212,21 +6015,15 @@
       </c>
       <c r="E162" t="inlineStr">
         <is>
-          <t># use std::{fs::File, io::{self, BufRead, BufReader}};
-# let _ = || -&gt; io::Result&lt;()&gt; {
-let mut lines = BufReader::new(File::open("some-path")?).lines().filter_map(Result::ok);
+          <t>let mut lines = BufReader::new(File::open("some-path")?).lines().filter_map(Result::ok);
 // If "some-path" points to a directory, the next statement never terminates:
-let first_line: Option&lt;String&gt; = lines.next();
-# Ok(()) };</t>
+let first_line: Option&lt;String&gt; = lines.next();</t>
         </is>
       </c>
       <c r="F162" t="inlineStr">
         <is>
-          <t># use std::{fs::File, io::{self, BufRead, BufReader}};
-# let _ = || -&gt; io::Result&lt;()&gt; {
-let mut lines = BufReader::new(File::open("some-path")?).lines().map_while(Result::ok);
-let first_line: Option&lt;String&gt; = lines.next();
-# Ok(()) };</t>
+          <t>let mut lines = BufReader::new(File::open("some-path")?).lines().map_while(Result::ok);
+let first_line: Option&lt;String&gt; = lines.next();</t>
         </is>
       </c>
     </row>
@@ -6251,16 +6048,12 @@
       </c>
       <c r="E163" t="inlineStr">
         <is>
-          <t># let _: u64 =
-61864918973511
-# ;</t>
+          <t>61864918973511</t>
         </is>
       </c>
       <c r="F163" t="inlineStr">
         <is>
-          <t># let _: u64 =
-61_864_918_973_511
-# ;</t>
+          <t>61_864_918_973_511</t>
         </is>
       </c>
     </row>
@@ -6312,16 +6105,12 @@
       </c>
       <c r="E165" t="inlineStr">
         <is>
-          <t># let _: u64 =
-618_64_9189_73_511
-# ;</t>
+          <t>618_64_9189_73_511</t>
         </is>
       </c>
       <c r="F165" t="inlineStr">
         <is>
-          <t># let _: u64 =
-61_864_918_973_511
-# ;</t>
+          <t>61_864_918_973_511</t>
         </is>
       </c>
     </row>
@@ -6427,8 +6216,7 @@
       </c>
       <c r="E169" t="inlineStr">
         <is>
-          <t>#[macro_use]
-use some_macro;</t>
+          <t>use some_macro;</t>
         </is>
       </c>
       <c r="F169" t="inlineStr"/>
@@ -6577,26 +6365,19 @@
       </c>
       <c r="E174" t="inlineStr">
         <is>
-          <t># let (input, min, max) = (0, -2, 1);
-if input &gt; max {
+          <t>if input &gt; max {
     max
 } else if input &lt; min {
     min
 } else {
     input
 }
-# ;
-# let (input, min, max) = (0, -2, 1);
 input.max(min).min(max)
-# ;
-# let (input, min, max) = (0, -2, 1);
 match input {
     x if x &gt; max =&gt; max,
     x if x &lt; min =&gt; min,
     x =&gt; x,
 }
-# ;
-# let (input, min, max) = (0, -2, 1);
 let mut x = input;
 if x &lt; min { x = min; }
 if x &gt; max { x = max; }</t>
@@ -6604,9 +6385,7 @@
       </c>
       <c r="F174" t="inlineStr">
         <is>
-          <t># let (input, min, max) = (0, -2, 1);
-input.clamp(min, max)
-# ;</t>
+          <t>input.clamp(min, max)</t>
         </is>
       </c>
     </row>
@@ -6677,16 +6456,12 @@
       </c>
       <c r="E176" t="inlineStr">
         <is>
-          <t># let w = Some(0);
-let v = if let Some(v) = w { v } else { return };</t>
+          <t>let v = if let Some(v) = w { v } else { return };</t>
         </is>
       </c>
       <c r="F176" t="inlineStr">
         <is>
-          <t># fn main () {
-# let w = Some(0);
-let Some(v) = w else { return };
-# }</t>
+          <t>let Some(v) = w else { return };</t>
         </is>
       </c>
     </row>
@@ -6757,17 +6532,14 @@
       </c>
       <c r="F178" t="inlineStr">
         <is>
-          <t>#[non_exhaustive]
-struct S {
+          <t>struct S {
     pub a: i32,
     pub b: i32,
 }
-#[non_exhaustive]
 enum E {
     A,
     B,
 }
-#[non_exhaustive]
 struct T(pub i32, pub i32);</t>
         </is>
       </c>
@@ -6858,14 +6630,12 @@
       </c>
       <c r="E181" t="inlineStr">
         <is>
-          <t># let data : &amp;[i32] = &amp;[1, 2, 3];
-let newlen = data.len() * std::mem::size_of::&lt;i32&gt;();</t>
+          <t>let newlen = data.len() * std::mem::size_of::&lt;i32&gt;();</t>
         </is>
       </c>
       <c r="F181" t="inlineStr">
         <is>
-          <t># let data : &amp;[i32] = &amp;[1, 2, 3];
-let newlen = std::mem::size_of_val(data);</t>
+          <t>let newlen = std::mem::size_of_val(data);</t>
         </is>
       </c>
     </row>
@@ -6958,25 +6728,17 @@
       </c>
       <c r="E184" t="inlineStr">
         <is>
-          <t># fn do_stuff() -&gt; Option&lt;String&gt; { Some(String::new()) }
-# fn log_err_msg(foo: String) -&gt; Option&lt;String&gt; { Some(foo) }
-# fn format_msg(foo: String) -&gt; String { String::new() }
-let x: Option&lt;String&gt; = do_stuff();
+          <t>let x: Option&lt;String&gt; = do_stuff();
 x.map(log_err_msg);
-# let x: Option&lt;String&gt; = do_stuff();
 x.map(|msg| log_err_msg(format_msg(msg)));</t>
         </is>
       </c>
       <c r="F184" t="inlineStr">
         <is>
-          <t># fn do_stuff() -&gt; Option&lt;String&gt; { Some(String::new()) }
-# fn log_err_msg(foo: String) -&gt; Option&lt;String&gt; { Some(foo) }
-# fn format_msg(foo: String) -&gt; String { String::new() }
-let x: Option&lt;String&gt; = do_stuff();
+          <t>let x: Option&lt;String&gt; = do_stuff();
 if let Some(msg) = x {
     log_err_msg(msg);
 }
-# let x: Option&lt;String&gt; = do_stuff();
 if let Some(msg) = x {
     log_err_msg(format_msg(msg));
 }</t>
@@ -7004,25 +6766,17 @@
       </c>
       <c r="E185" t="inlineStr">
         <is>
-          <t># fn do_stuff() -&gt; Result&lt;String, String&gt; { Ok(String::new()) }
-# fn log_err_msg(foo: String) -&gt; Result&lt;String, String&gt; { Ok(foo) }
-# fn format_msg(foo: String) -&gt; String { String::new() }
-let x: Result&lt;String, String&gt; = do_stuff();
+          <t>let x: Result&lt;String, String&gt; = do_stuff();
 x.map(log_err_msg);
-# let x: Result&lt;String, String&gt; = do_stuff();
 x.map(|msg| log_err_msg(format_msg(msg)));</t>
         </is>
       </c>
       <c r="F185" t="inlineStr">
         <is>
-          <t># fn do_stuff() -&gt; Result&lt;String, String&gt; { Ok(String::new()) }
-# fn log_err_msg(foo: String) -&gt; Result&lt;String, String&gt; { Ok(foo) }
-# fn format_msg(foo: String) -&gt; String { String::new() }
-let x: Result&lt;String, String&gt; = do_stuff();
+          <t>let x: Result&lt;String, String&gt; = do_stuff();
 if let Ok(msg) = x {
     log_err_msg(msg);
 };
-# let x: Result&lt;String, String&gt; = do_stuff();
 if let Ok(msg) = x {
     log_err_msg(format_msg(msg));
 };</t>
@@ -7090,9 +6844,7 @@
       </c>
       <c r="E187" t="inlineStr">
         <is>
-          <t># use std::mem;
-# use std::rc::Rc;
-mem::forget(Rc::new(55))</t>
+          <t>mem::forget(Rc::new(55))</t>
         </is>
       </c>
       <c r="F187" t="inlineStr"/>
@@ -7151,7 +6903,6 @@
         <is>
           <t>use std::mem;
 ///# fn may_panic(v: Vec&lt;i32&gt;) -&gt; Vec&lt;i32&gt; { v }
-#[allow(deprecated, invalid_value)]
 fn myfunc (v: &amp;mut Vec&lt;i32&gt;) {
     let taken_v = unsafe { mem::replace(v, mem::uninitialized()) };
     let new_v = may_panic(taken_v); // undefined behavior on panic
@@ -7398,16 +7149,14 @@
       </c>
       <c r="E197" t="inlineStr">
         <is>
-          <t># struct Service { ready: bool }
-fn call(service: Service) {
+          <t>fn call(service: Service) {
     assert!(service.ready);
 }</t>
         </is>
       </c>
       <c r="F197" t="inlineStr">
         <is>
-          <t># struct Service { ready: bool }
-fn call(service: Service) {
+          <t>fn call(service: Service) {
     assert!(service.ready, "`service.poll_ready()` must be called first to ensure that service is ready to receive requests");
 }</t>
         </is>
@@ -7434,23 +7183,13 @@
       </c>
       <c r="E198" t="inlineStr">
         <is>
-          <t># struct Foo {
-#     random_number: usize,
-# }
-# impl Foo {
-fn new() -&gt; Self {
+          <t>fn new() -&gt; Self {
     Self { random_number: 42 }
 }
-# }
 Could be a const fn:
-# struct Foo {
-#     random_number: usize,
-# }
-# impl Foo {
 const fn new() -&gt; Self {
     Self { random_number: 42 }
-}
-# }</t>
+}</t>
         </is>
       </c>
       <c r="F198" t="inlineStr"/>
@@ -7499,7 +7238,6 @@
       <c r="E200" t="inlineStr">
         <is>
           <t>An example clippy.toml configuration:
-# clippy.toml
 enforced-import-renames = [ { path = "serde_json::Value", rename = "JsonValue" }]
 use serde_json::Value;</t>
         </is>
@@ -7533,8 +7271,6 @@
         <is>
           <t>pub fn foo() {} // missing #[inline]
 fn ok() {} // ok
-#[inline] pub fn bar() {} // ok
-#[inline(always)] pub fn baz() {} // ok
 pub trait Bar {
   fn bar(); // ok
   fn def_bar() {} // missing #[inline]
@@ -7584,8 +7320,6 @@
     fn required();
     fn provided() {}
 }
-# struct Type;
-#[warn(clippy::missing_trait_methods)]
 impl Trait for Type {
     fn required() { /* ... */ }
 }</t>
@@ -7597,8 +7331,6 @@
     fn required();
     fn provided() {}
 }
-# struct Type;
-#[warn(clippy::missing_trait_methods)]
 impl Trait for Type {
     fn required() { /* ... */ }
     fn provided() { /* ... */ }
@@ -7637,8 +7369,7 @@
       </c>
       <c r="F203" t="inlineStr">
         <is>
-          <t># let mut x = 0;
-let tmp = {
+          <t>let tmp = {
     x = 1;
     1
 };
@@ -7667,9 +7398,7 @@
       </c>
       <c r="E204" t="inlineStr">
         <is>
-          <t># fn b() -&gt; bool { true }
-# fn c() -&gt; bool { true }
-let a = b() || panic!() || c();
+          <t>let a = b() || panic!() || c();
 // `c()` is dead, `panic!()` is only called if `b()` returns `false`
 let x = (a, b, c, panic!());
 // can simply be replaced by `panic!()`</t>
@@ -7864,8 +7593,6 @@
         <is>
           <t>debug_assert_eq!(vec![3].pop(), Some(3));
 // or
-# let mut x = 5;
-# fn takes_a_mut_parameter(_: &amp;mut u32) -&gt; bool { unimplemented!() }
 debug_assert!(takes_a_mut_parameter(&amp;mut x));</t>
         </is>
       </c>
@@ -7892,16 +7619,12 @@
       </c>
       <c r="E210" t="inlineStr">
         <is>
-          <t># let y = true;
-# use std::sync::Mutex;
-let x = Mutex::new(&amp;y);</t>
+          <t>let x = Mutex::new(&amp;y);</t>
         </is>
       </c>
       <c r="F210" t="inlineStr">
         <is>
-          <t># let y = true;
-# use std::sync::atomic::AtomicBool;
-let x = AtomicBool::new(y);</t>
+          <t>let x = AtomicBool::new(y);</t>
         </is>
       </c>
     </row>
@@ -7926,14 +7649,12 @@
       </c>
       <c r="E211" t="inlineStr">
         <is>
-          <t># use std::sync::Mutex;
-let x = Mutex::new(0usize);</t>
+          <t>let x = Mutex::new(0usize);</t>
         </is>
       </c>
       <c r="F211" t="inlineStr">
         <is>
-          <t># use std::sync::atomic::AtomicUsize;
-let x = AtomicUsize::new(0usize);</t>
+          <t>let x = AtomicUsize::new(0usize);</t>
         </is>
       </c>
     </row>
@@ -8005,8 +7726,7 @@
       </c>
       <c r="E213" t="inlineStr">
         <is>
-          <t># let mut y = 1;
-let x = &amp;mut &amp;mut y;</t>
+          <t>let x = &amp;mut &amp;mut y;</t>
         </is>
       </c>
       <c r="F213" t="inlineStr"/>
@@ -8032,16 +7752,12 @@
       </c>
       <c r="E214" t="inlineStr">
         <is>
-          <t># let mut vec = Vec::new();
-# let mut value = 5;
-vec.push(&amp;mut value);</t>
+          <t>vec.push(&amp;mut value);</t>
         </is>
       </c>
       <c r="F214" t="inlineStr">
         <is>
-          <t># let mut vec = Vec::new();
-# let value = 5;
-vec.push(&amp;value);</t>
+          <t>vec.push(&amp;value);</t>
         </is>
       </c>
     </row>
@@ -8120,20 +7836,16 @@
       </c>
       <c r="E216" t="inlineStr">
         <is>
-          <t># let x = true;
-if x {
+          <t>if x {
     false
 } else {
     true
-}
-# ;</t>
+}</t>
         </is>
       </c>
       <c r="F216" t="inlineStr">
         <is>
-          <t># let x = true;
-!x
-# ;</t>
+          <t>!x</t>
         </is>
       </c>
     </row>
@@ -8188,10 +7900,7 @@
       </c>
       <c r="E218" t="inlineStr">
         <is>
-          <t># fn must_keep(x: i32, y: i32) -&gt; bool { x == y }
-# let x = 32; let y = 10;
-# let mut skip: bool;
-if must_keep(x, y) {
+          <t>if must_keep(x, y) {
     skip = false;
 } else {
     skip = true;
@@ -8200,10 +7909,7 @@
       </c>
       <c r="F218" t="inlineStr">
         <is>
-          <t># fn must_keep(x: i32, y: i32) -&gt; bool { x == y }
-# let x = 32; let y = 10;
-# let mut skip: bool;
-skip = !must_keep(x, y);</t>
+          <t>skip = !must_keep(x, y);</t>
         </is>
       </c>
     </row>
@@ -8262,10 +7968,7 @@
       </c>
       <c r="E220" t="inlineStr">
         <is>
-          <t># fn condition() -&gt; bool { false }
-# fn update_condition() {}
-# let x = false;
-while condition() {
+          <t>while condition() {
     update_condition();
     if x {
         // ...
@@ -8275,9 +7978,6 @@
     println!("Hello, world");
 }
 Could be rewritten as
-# fn condition() -&gt; bool { false }
-# fn update_condition() {}
-# let x = false;
 while condition() {
     update_condition();
     if x {
@@ -8286,7 +7986,6 @@
     }
 }
 As another example, the following code
-# fn waiting() -&gt; bool { false }
 loop {
     if waiting() {
         continue;
@@ -8296,7 +7995,6 @@
     # break;
 }
 Could be rewritten as
-# fn waiting() -&gt; bool { false }
 loop {
     if waiting() {
         continue;
@@ -8536,13 +8234,7 @@
       </c>
       <c r="E226" t="inlineStr">
         <is>
-          <t># struct Point {
-#     x: i32,
-#     y: i32,
-#     z: i32,
-# }
-# let zero_point = Point { x: 0, y: 0, z: 0 };
-Point {
+          <t>Point {
     x: 1,
     y: 1,
     z: 1,
@@ -8590,8 +8282,6 @@
       <c r="F227" t="inlineStr">
         <is>
           <t>use std::cmp::Ordering;
-# let a = 1.0;
-# let b = f64::NAN;
 let _not_less_or_equal = match a.partial_cmp(&amp;b) {
     None | Some(Ordering::Greater) =&gt; true,
     _ =&gt; false,
@@ -8726,8 +8416,7 @@
       </c>
       <c r="F231" t="inlineStr">
         <is>
-          <t># use std::sync::atomic::{AtomicUsize, Ordering::SeqCst};
-static STATIC_ATOM: AtomicUsize = AtomicUsize::new(15);
+          <t>static STATIC_ATOM: AtomicUsize = AtomicUsize::new(15);
 STATIC_ATOM.store(9, SeqCst);
 assert_eq!(STATIC_ATOM.load(SeqCst), 9); // use a `static` item to refer to the same instance</t>
         </is>
@@ -9089,10 +8778,7 @@
     } else {
         f(a - 1, b + 1)
     }
-}
-# fn main() {
-#     print!("{}", f(1, 1));
-# }</t>
+}</t>
         </is>
       </c>
       <c r="F243" t="inlineStr">
@@ -9103,10 +8789,7 @@
     } else {
         f(a - 1)
     }
-}
-# fn main() {
-#     print!("{}", f(1));
-# }</t>
+}</t>
         </is>
       </c>
     </row>
@@ -9159,9 +8842,7 @@
       </c>
       <c r="E245" t="inlineStr">
         <is>
-          <t># let optional: Option&lt;u32&gt; = Some(0);
-# fn do_complicated_function() -&gt; u32 { 5 };
-let _ = if let Some(foo) = optional {
+          <t>let _ = if let Some(foo) = optional {
     foo
 } else {
     5
@@ -9177,8 +8858,6 @@
     y*y
 };
 should be
-# let optional: Option&lt;u32&gt; = Some(0);
-# fn do_complicated_function() -&gt; u32 { 5 };
 let _ = optional.map_or(5, |foo| foo);
 let _ = optional.map_or(5, |val| val + 1);
 let _ = optional.map_or_else(||{
@@ -9210,9 +8889,7 @@
       </c>
       <c r="E246" t="inlineStr">
         <is>
-          <t># let a = 1;
-# let b = 2;
-a + b &lt; a;</t>
+          <t>a + b &lt; a;</t>
         </is>
       </c>
       <c r="F246" t="inlineStr"/>
@@ -9509,16 +9186,13 @@
       </c>
       <c r="E256" t="inlineStr">
         <is>
-          <t>#[derive(Clone, Copy)]
-struct TooLarge([u8; 2048]);
+          <t>struct TooLarge([u8; 2048]);
 fn foo(v: TooLarge) {}</t>
         </is>
       </c>
       <c r="F256" t="inlineStr">
         <is>
-          <t># #[derive(Clone, Copy)]
-# struct TooLarge([u8; 2048]);
-fn foo(v: &amp;TooLarge) {}</t>
+          <t>fn foo(v: &amp;TooLarge) {}</t>
         </is>
       </c>
     </row>
@@ -9917,18 +9591,14 @@
       </c>
       <c r="E268" t="inlineStr">
         <is>
-          <t># let x = 0;
-# let y = 1;
-for i in x..(y+1) {
+          <t>for i in x..(y+1) {
     // ..
 }</t>
         </is>
       </c>
       <c r="F268" t="inlineStr">
         <is>
-          <t># let x = 0;
-# let y = 1;
-for i in x..=y {
+          <t>for i in x..=y {
     // ..
 }</t>
         </is>
@@ -9955,18 +9625,14 @@
       </c>
       <c r="E269" t="inlineStr">
         <is>
-          <t># let x = 0;
-# let y = 1;
-for i in x..=(y-1) {
+          <t>for i in x..=(y-1) {
     // ..
 }</t>
         </is>
       </c>
       <c r="F269" t="inlineStr">
         <is>
-          <t># let x = 0;
-# let y = 1;
-for i in x..y {
+          <t>for i in x..y {
     // ..
 }</t>
         </is>
@@ -10174,14 +9840,7 @@
       </c>
       <c r="E275" t="inlineStr">
         <is>
-          <t># use std::path::Path;
-# #[derive(Clone)]
-# struct Foo;
-# impl Foo {
-#     fn new() -&gt; Self { Foo {} }
-# }
-# fn call(x: Foo) {}
-{
+          <t>{
     let x = Foo::new();
     call(x.clone());
     call(x.clone()); // this can just pass `x`
@@ -10671,8 +10330,7 @@
       </c>
       <c r="F290" t="inlineStr">
         <is>
-          <t># {
-// It's better to have the `#[must_use]` attribute on the method like this:
+          <t>// It's better to have the `#[must_use]` attribute on the method like this:
 pub struct Bar;
 impl Bar {
     #[must_use]
@@ -10680,17 +10338,13 @@
         Self
     }
 }
-# }
-# {
 // Or on the type definition like this:
-#[must_use]
 pub struct Bar;
 impl Bar {
     pub fn bar(&amp;self) -&gt; Self {
         Self
     }
-}
-# }</t>
+}</t>
         </is>
       </c>
     </row>
@@ -10790,16 +10444,12 @@
       </c>
       <c r="E293" t="inlineStr">
         <is>
-          <t># fn f(_: u32) {}
-# let x = 0;
-unsafe { f(x) };</t>
+          <t>unsafe { f(x) };</t>
         </is>
       </c>
       <c r="F293" t="inlineStr">
         <is>
-          <t># fn f(_: u32) {}
-# let x = 0;
-unsafe { f(x); }</t>
+          <t>unsafe { f(x); }</t>
         </is>
       </c>
     </row>
@@ -10824,16 +10474,12 @@
       </c>
       <c r="E294" t="inlineStr">
         <is>
-          <t># fn f(_: u32) {}
-# let x = 0;
-unsafe { f(x); }</t>
+          <t>unsafe { f(x); }</t>
         </is>
       </c>
       <c r="F294" t="inlineStr">
         <is>
-          <t># fn f(_: u32) {}
-# let x = 0;
-unsafe { f(x) };</t>
+          <t>unsafe { f(x) };</t>
         </is>
       </c>
     </row>
@@ -10919,14 +10565,12 @@
       </c>
       <c r="E297" t="inlineStr">
         <is>
-          <t># let x = 1;
-let x = &amp;x;</t>
+          <t>let x = &amp;x;</t>
         </is>
       </c>
       <c r="F297" t="inlineStr">
         <is>
-          <t># let x = 1;
-let y = &amp;x; // use different variable name</t>
+          <t>let y = &amp;x; // use different variable name</t>
         </is>
       </c>
     </row>
@@ -10981,17 +10625,13 @@
       </c>
       <c r="E299" t="inlineStr">
         <is>
-          <t># let y = 1;
-# let z = 2;
-let x = y;
+          <t>let x = y;
 let x = z; // shadows the earlier binding</t>
         </is>
       </c>
       <c r="F299" t="inlineStr">
         <is>
-          <t># let y = 1;
-# let z = 2;
-let x = y;
+          <t>let x = y;
 let w = z; // use different variable name</t>
         </is>
       </c>
@@ -11122,9 +10762,7 @@
       </c>
       <c r="E303" t="inlineStr">
         <is>
-          <t># use std::ptr::copy_nonoverlapping;
-# use std::mem::size_of;
-const SIZE: usize = 128;
+          <t>const SIZE: usize = 128;
 let x = [2u8; SIZE];
 let mut y = [2u8; SIZE];
 unsafe { copy_nonoverlapping(x.as_ptr(), y.as_mut_ptr(), size_of::&lt;u8&gt;() * SIZE) };</t>
@@ -11202,9 +10840,7 @@
       </c>
       <c r="E305" t="inlineStr">
         <is>
-          <t># use core::iter::repeat;
-# let len = 4;
-let mut vec1 = Vec::with_capacity(len);
+          <t>let mut vec1 = Vec::with_capacity(len);
 vec1.resize(len, 0);
 let mut vec1 = Vec::with_capacity(len);
 vec1.resize(vec1.capacity(), 0);
@@ -11214,8 +10850,7 @@
       </c>
       <c r="F305" t="inlineStr">
         <is>
-          <t># let len = 4;
-let mut vec1 = vec![0; len];
+          <t>let mut vec1 = vec![0; len];
 let mut vec2 = vec![0; len];</t>
         </is>
       </c>
@@ -11276,8 +10911,7 @@
       </c>
       <c r="F307" t="inlineStr">
         <is>
-          <t># extern crate alloc;
-use alloc::vec::Vec;</t>
+          <t>use alloc::vec::Vec;</t>
         </is>
       </c>
     </row>
@@ -11302,8 +10936,7 @@
       </c>
       <c r="E308" t="inlineStr">
         <is>
-          <t># extern crate alloc;
-use alloc::slice::from_ref;</t>
+          <t>use alloc::slice::from_ref;</t>
         </is>
       </c>
       <c r="F308" t="inlineStr">
@@ -11664,12 +11297,7 @@
       </c>
       <c r="F319" t="inlineStr">
         <is>
-          <t># struct Vec3 {
-#     x: f64,
-#     y: f64,
-#     z: f64,
-# }
-// same as above except:
+          <t>// same as above except:
 impl PartialEq for Vec3 {
     fn eq(&amp;self, other: &amp;Self) -&gt; bool {
         // Note we now compare other.x to self.x
@@ -11825,17 +11453,13 @@
       </c>
       <c r="E324" t="inlineStr">
         <is>
-          <t># let mut a = 1;
-# let mut b = 2;
-a = b;
+          <t>a = b;
 b = a;</t>
         </is>
       </c>
       <c r="F324" t="inlineStr">
         <is>
-          <t># let mut a = 1;
-# let mut b = 2;
-std::mem::swap(&amp;mut a, &amp;mut b);</t>
+          <t>std::mem::swap(&amp;mut a, &amp;mut b);</t>
         </is>
       </c>
     </row>
@@ -11978,11 +11602,9 @@
       </c>
       <c r="E328" t="inlineStr">
         <is>
-          <t>#[test]
-fn my_cool_test() {
+          <t>fn my_cool_test() {
     // [...]
 }
-#[cfg(test)]
 mod tests {
     // [...]
 }</t>
@@ -11990,8 +11612,7 @@
       </c>
       <c r="F328" t="inlineStr">
         <is>
-          <t>#[cfg(test)]
-mod tests {
+          <t>mod tests {
     #[test]
     fn my_cool_test() {
         // [...]
@@ -12021,16 +11642,12 @@
       </c>
       <c r="E329" t="inlineStr">
         <is>
-          <t># let c = 'c';
-# let radix = 10;
-let is_digit = c.to_digit(radix).is_some();</t>
+          <t>let is_digit = c.to_digit(radix).is_some();</t>
         </is>
       </c>
       <c r="F329" t="inlineStr">
         <is>
-          <t># let c = 'c';
-# let radix = 10;
-let is_digit = c.is_digit(radix);</t>
+          <t>let is_digit = c.is_digit(radix);</t>
         </is>
       </c>
     </row>
@@ -12063,8 +11680,7 @@
       </c>
       <c r="F330" t="inlineStr">
         <is>
-          <t>#[repr(C)]
-struct MoreOftenUseful {
+          <t>struct MoreOftenUseful {
     some_field: usize,
     last: [u32; 0],
 }</t>
@@ -12861,18 +12477,14 @@
       </c>
       <c r="E355" t="inlineStr">
         <is>
-          <t># let option = Some(0);
-# fn do_something_with(_x: usize) {}
-if option.is_some() {
+          <t>if option.is_some() {
     do_something_with(option.unwrap())
 }</t>
         </is>
       </c>
       <c r="F355" t="inlineStr">
         <is>
-          <t># let option = Some(0);
-# fn do_something_with(_x: usize) {}
-if let Some(value) = option {
+          <t>if let Some(value) = option {
     do_something_with(value)
 }</t>
         </is>
@@ -12899,9 +12511,7 @@
       </c>
       <c r="E356" t="inlineStr">
         <is>
-          <t># let option = Some(0);
-# fn do_something_with(_x: usize) {}
-if option.is_none() {
+          <t>if option.is_none() {
     do_something_with(option.unwrap())
 }
 This code will always panic. The if condition should probably be inverted.</t>
@@ -13082,8 +12692,7 @@
       </c>
       <c r="F361" t="inlineStr">
         <is>
-          <t># fn foo(_x: &amp;[u8]) {}
-foo(&amp;[1, 2]);</t>
+          <t>foo(&amp;[1, 2]);</t>
         </is>
       </c>
     </row>
@@ -13140,14 +12749,12 @@
       <c r="E363" t="inlineStr">
         <is>
           <t>use std::cmp::Ordering::*;
-# fn foo(_: std::cmp::Ordering) {}
 foo(Less);</t>
         </is>
       </c>
       <c r="F363" t="inlineStr">
         <is>
           <t>use std::cmp::Ordering;
-# fn foo(_: Ordering) {}
 foo(Ordering::Less)</t>
         </is>
       </c>
@@ -13235,10 +12842,8 @@
       </c>
       <c r="E366" t="inlineStr">
         <is>
-          <t># let name = "World";
-print!("Hello {}!\n", name);
+          <t>print!("Hello {}!\n", name);
 use println!() instead
-# let name = "World";
 println!("Hello {}!", name);</t>
         </is>
       </c>
@@ -13317,8 +12922,7 @@
       </c>
       <c r="E369" t="inlineStr">
         <is>
-          <t># let foo = "bar";
-println!("{:?}", foo);</t>
+          <t>println!("{:?}", foo);</t>
         </is>
       </c>
       <c r="F369" t="inlineStr"/>
@@ -13372,16 +12976,12 @@
       </c>
       <c r="E371" t="inlineStr">
         <is>
-          <t># use std::fmt::Write;
-# let mut buf = String::new();
-writeln!(buf, "");</t>
+          <t>writeln!(buf, "");</t>
         </is>
       </c>
       <c r="F371" t="inlineStr">
         <is>
-          <t># use std::fmt::Write;
-# let mut buf = String::new();
-writeln!(buf);</t>
+          <t>writeln!(buf);</t>
         </is>
       </c>
     </row>
@@ -13406,18 +13006,12 @@
       </c>
       <c r="E372" t="inlineStr">
         <is>
-          <t># use std::fmt::Write;
-# let mut buf = String::new();
-# let name = "World";
-write!(buf, "Hello {}!\n", name);</t>
+          <t>write!(buf, "Hello {}!\n", name);</t>
         </is>
       </c>
       <c r="F372" t="inlineStr">
         <is>
-          <t># use std::fmt::Write;
-# let mut buf = String::new();
-# let name = "World";
-writeln!(buf, "Hello {}!", name);</t>
+          <t>writeln!(buf, "Hello {}!", name);</t>
         </is>
       </c>
     </row>
@@ -13442,16 +13036,12 @@
       </c>
       <c r="E373" t="inlineStr">
         <is>
-          <t># use std::fmt::Write;
-# let mut buf = String::new();
-writeln!(buf, "{}", "foo");</t>
+          <t>writeln!(buf, "{}", "foo");</t>
         </is>
       </c>
       <c r="F373" t="inlineStr">
         <is>
-          <t># use std::fmt::Write;
-# let mut buf = String::new();
-writeln!(buf, "foo");</t>
+          <t>writeln!(buf, "foo");</t>
         </is>
       </c>
     </row>
@@ -13506,16 +13096,14 @@
       </c>
       <c r="E375" t="inlineStr">
         <is>
-          <t># use std::collections::HashMap;
-fn unique_words(text: &amp;str) -&gt; HashMap&lt;&amp;str, ()&gt; {
+          <t>fn unique_words(text: &amp;str) -&gt; HashMap&lt;&amp;str, ()&gt; {
     todo!();
 }</t>
         </is>
       </c>
       <c r="F375" t="inlineStr">
         <is>
-          <t># use std::collections::HashSet;
-fn unique_words(text: &amp;str) -&gt; HashSet&lt;&amp;str&gt; {
+          <t>fn unique_words(text: &amp;str) -&gt; HashSet&lt;&amp;str&gt; {
     todo!();
 }</t>
         </is>
@@ -13542,8 +13130,7 @@
       </c>
       <c r="E376" t="inlineStr">
         <is>
-          <t># This `Cargo.toml` is missing a description field:
-[package]
+          <t>[package]
 name = "clippy"
 version = "0.0.212"
 repository = "https://github.com/rust-lang/rust-clippy"
@@ -13552,7 +13139,6 @@
 keywords = ["clippy", "lint", "plugin"]
 categories = ["development-tools", "development-tools::cargo-plugins"]
 Should include a description field like:
-# This `Cargo.toml` includes all common metadata
 [package]
 name = "clippy"
 version = "0.0.212"
@@ -13587,8 +13173,7 @@
       </c>
       <c r="E377" t="inlineStr">
         <is>
-          <t># The `Cargo.toml` with feature name redundancy
-[features]
+          <t>[features]
 default = ["use-abc", "with-def", "ghi-support"]
 use-abc = []  // redundant
 with-def = []   // redundant
@@ -13626,8 +13211,7 @@
       </c>
       <c r="E378" t="inlineStr">
         <is>
-          <t># The `Cargo.toml` with negative feature names
-[features]
+          <t>[features]
 default = []
 no-abc = []
 not-def = []</t>
@@ -13663,8 +13247,7 @@
       </c>
       <c r="E379" t="inlineStr">
         <is>
-          <t># This will pull in both winapi v0.3.x and v0.2.x, triggering a warning.
-[dependencies]
+          <t>[dependencies]
 ctrlc = "=3.1.0"
 ansi_term = "=0.11.0"</t>
         </is>
@@ -13788,7 +13371,6 @@
     }
 }
 // Or
-#[allow(clippy::cast_possible_truncation)]
 fn as_u16(x: u64) -&gt; u16 {
     x as u16
 }</t>
@@ -13941,8 +13523,7 @@
       </c>
       <c r="F388" t="inlineStr">
         <is>
-          <t># fn fun() -&gt; i32 { 1 }
-let _ = fun as usize;</t>
+          <t>let _ = fun as usize;</t>
         </is>
       </c>
     </row>
@@ -14448,8 +14029,7 @@
       </c>
       <c r="E403" t="inlineStr">
         <is>
-          <t># struct Color;
-fn foo(x: u32, y: u32, name: &amp;str, c: Color, w: f32, h: f32, a: f32, b: f32) {
+          <t>fn foo(x: u32, y: u32, name: &amp;str, c: Color, w: f32, h: f32, a: f32, b: f32) {
     // ..
 }</t>
         </is>
@@ -14547,8 +14127,7 @@
       </c>
       <c r="E406" t="inlineStr">
         <is>
-          <t>#[must_use]
-fn useless() { }</t>
+          <t>fn useless() { }</t>
         </is>
       </c>
       <c r="F406" t="inlineStr"/>
@@ -14574,8 +14153,7 @@
       </c>
       <c r="E407" t="inlineStr">
         <is>
-          <t>#[must_use]
-fn double_must_use() -&gt; Result&lt;(), ()&gt; {
+          <t>fn double_must_use() -&gt; Result&lt;(), ()&gt; {
     unimplemented!();
 }</t>
         </is>
@@ -14633,7 +14211,6 @@
           <t>pub fn read_u8() -&gt; Result&lt;u8, ()&gt; { Err(()) }
 should become
 use std::fmt;
-#[derive(Debug)]
 pub struct EndOfStream;
 impl fmt::Display for EndOfStream {
     fn fmt(&amp;self, f: &amp;mut fmt::Formatter&lt;'_&gt;) -&gt; fmt::Result {
@@ -14796,18 +14373,14 @@
       </c>
       <c r="E413" t="inlineStr">
         <is>
-          <t># let src = vec![1];
-# let mut dst = vec![0; 65];
-for i in 0..src.len() {
+          <t>for i in 0..src.len() {
     dst[i + 64] = src[i];
 }</t>
         </is>
       </c>
       <c r="F413" t="inlineStr">
         <is>
-          <t># let src = vec![1];
-# let mut dst = vec![0; 65];
-dst[64..(src.len() + 64)].clone_from_slice(&amp;src[..]);</t>
+          <t>dst[64..(src.len() + 64)].clone_from_slice(&amp;src[..]);</t>
         </is>
       </c>
     </row>
@@ -14869,7 +14442,6 @@
       <c r="E415" t="inlineStr">
         <is>
           <t>// with `y` a `Vec` or slice:
-# let y = vec![1];
 for x in y.iter() {
     // ..
 }</t>
@@ -14877,8 +14449,7 @@
       </c>
       <c r="F415" t="inlineStr">
         <is>
-          <t># let y = vec![1];
-for x in &amp;y {
+          <t>for x in &amp;y {
     // ..
 }</t>
         </is>
@@ -14905,13 +14476,11 @@
       </c>
       <c r="E416" t="inlineStr">
         <is>
-          <t># let y = vec![1];
-// with `y` a `Vec` or slice:
+          <t>// with `y` a `Vec` or slice:
 for x in y.into_iter() {
     // ..
 }
 can be rewritten to
-# let y = vec![1];
 for x in y {
     // ..
 }</t>
@@ -14968,8 +14537,7 @@
       </c>
       <c r="E418" t="inlineStr">
         <is>
-          <t># let y = Some(1);
-loop {
+          <t>loop {
     let x = match y {
         Some(x) =&gt; x,
         None =&gt; break,
@@ -15005,9 +14573,7 @@
       </c>
       <c r="E419" t="inlineStr">
         <is>
-          <t># let v = vec![1];
-# fn bar(bar: usize, baz: usize) {}
-let mut i = 0;
+          <t>let mut i = 0;
 for item in &amp;v {
     bar(i, *item);
     i += 1;
@@ -15016,9 +14582,7 @@
       </c>
       <c r="F419" t="inlineStr">
         <is>
-          <t># let v = vec![1];
-# fn bar(bar: usize, baz: usize) {}
-for (i, item) in v.iter().enumerate() { bar(i, *item); }</t>
+          <t>for (i, item) in v.iter().enumerate() { bar(i, *item); }</t>
         </is>
       </c>
     </row>
@@ -15450,9 +15014,7 @@
       </c>
       <c r="E432" t="inlineStr">
         <is>
-          <t># fn bar(stool: &amp;str) {}
-# let x = Some("abc");
-match x {
+          <t>match x {
     Some(ref foo) =&gt; bar(foo),
     _ =&gt; (),
 }</t>
@@ -15460,9 +15022,7 @@
       </c>
       <c r="F432" t="inlineStr">
         <is>
-          <t># fn bar(stool: &amp;str) {}
-# let x = Some("abc");
-if let Some(ref foo) = x {
+          <t>if let Some(ref foo) = x {
     bar(foo);
 }</t>
         </is>
@@ -15490,17 +15050,11 @@
       <c r="E433" t="inlineStr">
         <is>
           <t>Using match:
-# fn bar(foo: &amp;usize) {}
-# let other_ref: usize = 1;
-# let x: Option&lt;&amp;usize&gt; = Some(&amp;1);
 match x {
     Some(ref foo) =&gt; bar(foo),
     _ =&gt; bar(&amp;other_ref),
 }
 Using if let with else:
-# fn bar(foo: &amp;usize) {}
-# let other_ref: usize = 1;
-# let x: Option&lt;&amp;usize&gt; = Some(&amp;1);
 if let Some(ref foo) = x {
     bar(foo);
 } else {
@@ -15569,9 +15123,7 @@
       </c>
       <c r="E435" t="inlineStr">
         <is>
-          <t># fn foo() {}
-# fn bar() {}
-let condition: bool = true;
+          <t>let condition: bool = true;
 match condition {
     true =&gt; foo(),
     false =&gt; bar(),
@@ -15580,9 +15132,7 @@
       </c>
       <c r="F435" t="inlineStr">
         <is>
-          <t># fn foo() {}
-# fn bar() {}
-let condition: bool = true;
+          <t>let condition: bool = true;
 if condition {
     foo();
 } else {
@@ -15708,9 +15258,7 @@
       </c>
       <c r="E439" t="inlineStr">
         <is>
-          <t># enum Foo { A(usize), B(usize) }
-# let x = Foo::B(1);
-match x {
+          <t>match x {
     Foo::A(_) =&gt; {},
     _ =&gt; {},
 }</t>
@@ -15718,9 +15266,7 @@
       </c>
       <c r="F439" t="inlineStr">
         <is>
-          <t># enum Foo { A(usize), B(usize) }
-# let x = Foo::B(1);
-match x {
+          <t>match x {
     Foo::A(_) =&gt; {},
     Foo::B(_) =&gt; {},
 }</t>
@@ -15748,9 +15294,7 @@
       </c>
       <c r="E440" t="inlineStr">
         <is>
-          <t># enum Foo { A, B, C }
-# let x = Foo::B;
-match x {
+          <t>match x {
     Foo::A =&gt; {},
     Foo::B =&gt; {},
     _ =&gt; {},
@@ -15759,9 +15303,7 @@
       </c>
       <c r="F440" t="inlineStr">
         <is>
-          <t># enum Foo { A, B, C }
-# let x = Foo::B;
-match x {
+          <t>match x {
     Foo::A =&gt; {},
     Foo::B =&gt; {},
     Foo::C =&gt; {},
@@ -15790,8 +15332,7 @@
       </c>
       <c r="E441" t="inlineStr">
         <is>
-          <t># let s = "foo";
-match s {
+          <t>match s {
     "a" =&gt; {},
     "bar" | _ =&gt; {},
 }</t>
@@ -15799,8 +15340,7 @@
       </c>
       <c r="F441" t="inlineStr">
         <is>
-          <t># let s = "foo";
-match s {
+          <t>match s {
     "a" =&gt; {},
     _ =&gt; {},
 }</t>
@@ -15868,9 +15408,7 @@
       </c>
       <c r="E443" t="inlineStr">
         <is>
-          <t># let a = 1;
-# let b = 2;
-match (a, b) {
+          <t>match (a, b) {
     (c, d) =&gt; {
         // useless match
     }
@@ -15879,9 +15417,7 @@
       </c>
       <c r="F443" t="inlineStr">
         <is>
-          <t># let a = 1;
-# let b = 2;
-let (c, d) = (a, b);</t>
+          <t>let (c, d) = (a, b);</t>
         </is>
       </c>
     </row>
@@ -15906,8 +15442,7 @@
       </c>
       <c r="E444" t="inlineStr">
         <is>
-          <t># struct A { a: i32 }
-let a = A { a: 5 };
+          <t>let a = A { a: 5 };
 match a {
     A { a: 5, .. } =&gt; {},
     _ =&gt; {},
@@ -15916,9 +15451,7 @@
       </c>
       <c r="F444" t="inlineStr">
         <is>
-          <t># struct A { a: i32 }
-# let a = A { a: 5 };
-match a {
+          <t>match a {
     A { a: 5 } =&gt; {},
     _ =&gt; {},
 }</t>
@@ -15946,9 +15479,7 @@
       </c>
       <c r="E445" t="inlineStr">
         <is>
-          <t># use std::task::Poll;
-# use std::net::{IpAddr, Ipv4Addr, Ipv6Addr};
-if let Ok(_) = Ok::&lt;i32, i32&gt;(42) {}
+          <t>if let Ok(_) = Ok::&lt;i32, i32&gt;(42) {}
 if let Err(_) = Err::&lt;i32, i32&gt;(42) {}
 if let None = None::&lt;()&gt; {}
 if let Some(_) = Some(42) {}
@@ -15964,9 +15495,7 @@
       </c>
       <c r="F445" t="inlineStr">
         <is>
-          <t># use std::task::Poll;
-# use std::net::{IpAddr, Ipv4Addr, Ipv6Addr};
-if Ok::&lt;i32, i32&gt;(42).is_ok() {}
+          <t>if Ok::&lt;i32, i32&gt;(42).is_ok() {}
 if Err::&lt;i32, i32&gt;(42).is_err() {}
 if None::&lt;()&gt;.is_none() {}
 if Some(42).is_some() {}
@@ -16245,8 +15774,7 @@
       </c>
       <c r="E452" t="inlineStr">
         <is>
-          <t># let text = "Foo";
-match &amp;*text.to_ascii_lowercase() {
+          <t>match &amp;*text.to_ascii_lowercase() {
     "foo" =&gt; {},
     "Bar" =&gt; {},
     _ =&gt; {},
@@ -16255,8 +15783,7 @@
       </c>
       <c r="F452" t="inlineStr">
         <is>
-          <t># let text = "Foo";
-match &amp;*text.to_ascii_lowercase() {
+          <t>match &amp;*text.to_ascii_lowercase() {
     "foo" =&gt; {},
     "bar" =&gt; {},
     _ =&gt; {},
@@ -16285,15 +15812,7 @@
       </c>
       <c r="E453" t="inlineStr">
         <is>
-          <t># use std::sync::Mutex;
-# struct State {}
-# impl State {
-#     fn foo(&amp;self) -&gt; bool {
-#         true
-#     }
-#     fn bar(&amp;self) {}
-# }
-let mutex = Mutex::new(State {});
+          <t>let mutex = Mutex::new(State {});
 match mutex.lock().unwrap().foo() {
     true =&gt; {
         mutex.lock().unwrap().bar(); // Deadlock!
@@ -16305,15 +15824,7 @@
       </c>
       <c r="F453" t="inlineStr">
         <is>
-          <t># use std::sync::Mutex;
-# struct State {}
-# impl State {
-#     fn foo(&amp;self) -&gt; bool {
-#         true
-#     }
-#     fn bar(&amp;self) {}
-# }
-let mutex = Mutex::new(State {});
+          <t>let mutex = Mutex::new(State {});
 let is_foo = mutex.lock().unwrap().foo();
 match is_foo {
     true =&gt; {
@@ -16519,15 +16030,13 @@
       </c>
       <c r="E459" t="inlineStr">
         <is>
-          <t># let vec = vec!["string".to_string()];
-vec.iter().cloned().take(10);
+          <t>vec.iter().cloned().take(10);
 vec.iter().cloned().last();</t>
         </is>
       </c>
       <c r="F459" t="inlineStr">
         <is>
-          <t># let vec = vec!["string".to_string()];
-vec.iter().take(10).cloned();
+          <t>vec.iter().take(10).cloned();
 vec.iter().last().cloned();</t>
         </is>
       </c>
@@ -16583,17 +16092,13 @@
       </c>
       <c r="E461" t="inlineStr">
         <is>
-          <t># let option = Some(1);
-# let result: Result&lt;usize, ()&gt; = Ok(1);
-option.unwrap();
+          <t>option.unwrap();
 result.unwrap();</t>
         </is>
       </c>
       <c r="F461" t="inlineStr">
         <is>
-          <t># let option = Some(1);
-# let result: Result&lt;usize, ()&gt; = Ok(1);
-option?;
+          <t>option?;
 // or
 result?;</t>
         </is>
@@ -16620,17 +16125,13 @@
       </c>
       <c r="E462" t="inlineStr">
         <is>
-          <t># let option = Some(1);
-# let result: Result&lt;usize, ()&gt; = Ok(1);
-option.expect("one");
+          <t>option.expect("one");
 result.expect("one");</t>
         </is>
       </c>
       <c r="F462" t="inlineStr">
         <is>
-          <t># let option = Some(1);
-# let result: Result&lt;usize, ()&gt; = Ok(1);
-option?;
+          <t>option?;
 // or
 result?;</t>
         </is>
@@ -16661,7 +16162,6 @@
 impl X {
     fn add(&amp;self, other: &amp;X) -&gt; X {
         // ..
-# X
     }
 }</t>
         </is>
@@ -16689,11 +16189,9 @@
       </c>
       <c r="E464" t="inlineStr">
         <is>
-          <t># struct X;
-impl X {
+          <t>impl X {
     fn as_str(self) -&gt; &amp;'static str {
         // ..
-# ""
     }
 }</t>
         </is>
@@ -16721,14 +16219,12 @@
       </c>
       <c r="E465" t="inlineStr">
         <is>
-          <t># let x = Ok::&lt;_, ()&gt;(());
-x.ok().expect("why did I do this again?");</t>
+          <t>x.ok().expect("why did I do this again?");</t>
         </is>
       </c>
       <c r="F465" t="inlineStr">
         <is>
-          <t># let x = Ok::&lt;_, ()&gt;(());
-x.expect("why did I do this again?");</t>
+          <t>x.expect("why did I do this again?");</t>
         </is>
       </c>
     </row>
@@ -16785,15 +16281,13 @@
       </c>
       <c r="E467" t="inlineStr">
         <is>
-          <t># let x = Some(1);
-x.unwrap_or_else(Default::default);
+          <t>x.unwrap_or_else(Default::default);
 x.unwrap_or_else(u32::default);</t>
         </is>
       </c>
       <c r="F467" t="inlineStr">
         <is>
-          <t># let x = Some(1);
-x.unwrap_or_default();</t>
+          <t>x.unwrap_or_default();</t>
         </is>
       </c>
     </row>
@@ -16818,19 +16312,13 @@
       </c>
       <c r="E468" t="inlineStr">
         <is>
-          <t># let option = Some(1);
-# let result: Result&lt;usize, ()&gt; = Ok(1);
-# fn some_function(foo: ()) -&gt; usize { 1 }
-option.map(|a| a + 1).unwrap_or(0);
+          <t>option.map(|a| a + 1).unwrap_or(0);
 result.map(|a| a + 1).unwrap_or_else(some_function);</t>
         </is>
       </c>
       <c r="F468" t="inlineStr">
         <is>
-          <t># let option = Some(1);
-# let result: Result&lt;usize, ()&gt; = Ok(1);
-# fn some_function(foo: ()) -&gt; usize { 1 }
-option.map_or(0, |a| a + 1);
+          <t>option.map_or(0, |a| a + 1);
 result.map_or_else(some_function, |a| a + 1);</t>
         </is>
       </c>
@@ -16856,14 +16344,12 @@
       </c>
       <c r="E469" t="inlineStr">
         <is>
-          <t># let opt = Some(1);
-opt.map_or(None, |a| Some(a + 1));</t>
+          <t>opt.map_or(None, |a| Some(a + 1));</t>
         </is>
       </c>
       <c r="F469" t="inlineStr">
         <is>
-          <t># let opt = Some(1);
-opt.and_then(|a| Some(a + 1));</t>
+          <t>opt.and_then(|a| Some(a + 1));</t>
         </is>
       </c>
     </row>
@@ -16888,14 +16374,12 @@
       </c>
       <c r="E470" t="inlineStr">
         <is>
-          <t># let r: Result&lt;u32, &amp;str&gt; = Ok(1);
-assert_eq!(Some(1), r.map_or(None, Some));</t>
+          <t>assert_eq!(Some(1), r.map_or(None, Some));</t>
         </is>
       </c>
       <c r="F470" t="inlineStr">
         <is>
-          <t># let r: Result&lt;u32, &amp;str&gt; = Ok(1);
-assert_eq!(Some(1), r.ok());</t>
+          <t>assert_eq!(Some(1), r.ok());</t>
         </is>
       </c>
     </row>
@@ -16920,18 +16404,14 @@
       </c>
       <c r="E471" t="inlineStr">
         <is>
-          <t># fn opt() -&gt; Option&lt;&amp;'static str&gt; { Some("42") }
-# fn res() -&gt; Result&lt;&amp;'static str, &amp;'static str&gt; { Ok("42") }
-let _ = opt().and_then(|s| Some(s.len()));
+          <t>let _ = opt().and_then(|s| Some(s.len()));
 let _ = res().and_then(|s| if s.len() == 42 { Ok(10) } else { Ok(20) });
 let _ = res().or_else(|s| if s.len() == 42 { Err(10) } else { Err(20) });</t>
         </is>
       </c>
       <c r="F471" t="inlineStr">
         <is>
-          <t># fn opt() -&gt; Option&lt;&amp;'static str&gt; { Some("42") }
-# fn res() -&gt; Result&lt;&amp;'static str, &amp;'static str&gt; { Ok("42") }
-let _ = opt().map(|s| s.len());
+          <t>let _ = opt().map(|s| s.len());
 let _ = res().map(|s| if s.len() == 42 { 10 } else { 20 });
 let _ = res().map_err(|s| if s.len() == 42 { 10 } else { 20 });</t>
         </is>
@@ -16958,14 +16438,12 @@
       </c>
       <c r="E472" t="inlineStr">
         <is>
-          <t># let vec = vec![1];
-vec.iter().filter(|x| **x == 0).next();</t>
+          <t>vec.iter().filter(|x| **x == 0).next();</t>
         </is>
       </c>
       <c r="F472" t="inlineStr">
         <is>
-          <t># let vec = vec![1];
-vec.iter().find(|x| **x == 0);</t>
+          <t>vec.iter().find(|x| **x == 0);</t>
         </is>
       </c>
     </row>
@@ -16990,14 +16468,12 @@
       </c>
       <c r="E473" t="inlineStr">
         <is>
-          <t># let vec = vec![1];
-vec.iter().skip_while(|x| **x == 0).next();</t>
+          <t>vec.iter().skip_while(|x| **x == 0).next();</t>
         </is>
       </c>
       <c r="F473" t="inlineStr">
         <is>
-          <t># let vec = vec![1];
-vec.iter().find(|x| **x != 0);</t>
+          <t>vec.iter().find(|x| **x != 0);</t>
         </is>
       </c>
     </row>
@@ -17030,9 +16506,7 @@
       </c>
       <c r="F474" t="inlineStr">
         <is>
-          <t># let vec = vec![vec![1]];
-# let opt = Some(5);
-vec.iter().flat_map(|x| x.iter());
+          <t>vec.iter().flat_map(|x| x.iter());
 opt.and_then(|x| Some(x * 2));</t>
         </is>
       </c>
@@ -17058,16 +16532,14 @@
       </c>
       <c r="E475" t="inlineStr">
         <is>
-          <t># #![allow(unused)]
-(0_i32..10)
+          <t>(0_i32..10)
     .filter(|n| n.checked_add(1).is_some())
     .map(|n| n.checked_add(1).unwrap());</t>
         </is>
       </c>
       <c r="F475" t="inlineStr">
         <is>
-          <t># #[allow(unused)]
-(0_i32..10).filter_map(|n| n.checked_add(1));</t>
+          <t>(0_i32..10).filter_map(|n| n.checked_add(1));</t>
         </is>
       </c>
     </row>
@@ -17152,10 +16624,8 @@
       </c>
       <c r="E478" t="inlineStr">
         <is>
-          <t># let iter = vec![vec![0]].into_iter();
-iter.flat_map(|x| x);
+          <t>iter.flat_map(|x| x);
 Can be written as
-# let iter = vec![vec![0]].into_iter();
 iter.flatten();</t>
         </is>
       </c>
@@ -17178,8 +16648,7 @@
       <c r="D479" t="inlineStr"/>
       <c r="E479" t="inlineStr">
         <is>
-          <t># #![allow(unused)]
-let vec = vec![1];
+          <t>let vec = vec![1];
 vec.iter().find(|x| **x == 0).is_some();
 "hello world".find("world").is_none();</t>
         </is>
@@ -17188,7 +16657,6 @@
         <is>
           <t>let vec = vec![1];
 vec.iter().any(|x| *x == 0);
-# #[allow(unused)]
 !"hello world".contains("world");</t>
         </is>
       </c>
@@ -17246,14 +16714,12 @@
       </c>
       <c r="E481" t="inlineStr">
         <is>
-          <t># let foo = Some(String::new());
-foo.unwrap_or(String::from("empty"));</t>
+          <t>foo.unwrap_or(String::from("empty"));</t>
         </is>
       </c>
       <c r="F481" t="inlineStr">
         <is>
-          <t># let foo = Some(String::new());
-foo.unwrap_or_else(|| String::from("empty"));</t>
+          <t>foo.unwrap_or_else(|| String::from("empty"));</t>
         </is>
       </c>
     </row>
@@ -17278,24 +16744,17 @@
       </c>
       <c r="E482" t="inlineStr">
         <is>
-          <t># let fallback = "fallback";
-// Result
-# type Error = &amp;'static str;
-# let result: Result&lt;&amp;str, Error&gt; = Err("error");
+          <t>// Result
 let value = result.or::&lt;Error&gt;(Ok(fallback)).unwrap();
 // Option
-# let option: Option&lt;&amp;str&gt; = None;
 let value = option.or(Some(fallback)).unwrap();</t>
         </is>
       </c>
       <c r="F482" t="inlineStr">
         <is>
-          <t># let fallback = "fallback";
-// Result
-# let result: Result&lt;&amp;str, &amp;str&gt; = Err("error");
+          <t>// Result
 let value = result.unwrap_or(fallback);
 // Option
-# let option: Option&lt;&amp;str&gt; = None;
 let value = option.unwrap_or(fallback);</t>
         </is>
       </c>
@@ -17321,21 +16780,14 @@
       </c>
       <c r="E483" t="inlineStr">
         <is>
-          <t># let foo = Some(String::new());
-# let err_code = "418";
-# let err_msg = "I'm a teapot";
-foo.expect(&amp;format!("Err {}: {}", err_code, err_msg));
+          <t>foo.expect(&amp;format!("Err {}: {}", err_code, err_msg));
 // or
-# let foo = Some(String::new());
 foo.expect(format!("Err {}: {}", err_code, err_msg).as_str());</t>
         </is>
       </c>
       <c r="F483" t="inlineStr">
         <is>
-          <t># let foo = Some(String::new());
-# let err_code = "418";
-# let err_msg = "I'm a teapot";
-foo.unwrap_or_else(|| panic!("Err {}: {}", err_code, err_msg));</t>
+          <t>foo.unwrap_or_else(|| panic!("Err {}: {}", err_code, err_msg));</t>
         </is>
       </c>
     </row>
@@ -17386,16 +16838,13 @@
       </c>
       <c r="E485" t="inlineStr">
         <is>
-          <t># use std::rc::Rc;
-let x = Rc::new(1);
+          <t>let x = Rc::new(1);
 x.clone();</t>
         </is>
       </c>
       <c r="F485" t="inlineStr">
         <is>
-          <t># use std::rc::Rc;
-# let x = Rc::new(1);
-Rc::clone(&amp;x);</t>
+          <t>Rc::clone(&amp;x);</t>
         </is>
       </c>
     </row>
@@ -17450,27 +16899,19 @@
       <c r="E487" t="inlineStr">
         <is>
           <t>In an impl block:
-# struct Foo;
-# struct NotAFoo;
 impl Foo {
     fn new() -&gt; NotAFoo {
-# NotAFoo
     }
 }
-# struct Foo;
 struct Bar(Foo);
 impl Foo {
     // Bad. The type name must contain `Self`
     fn new() -&gt; Bar {
-# Bar(Foo)
     }
 }
-# struct Foo;
-# struct FooError;
 impl Foo {
     // Good. Return type contains `Self`
     fn new() -&gt; Result&lt;Foo, FooError&gt; {
-# Ok(Foo)
     }
 }
 Or in a trait definition:
@@ -17595,18 +17036,12 @@
       </c>
       <c r="E491" t="inlineStr">
         <is>
-          <t># use std::collections::HashSet;
-# let mut s = HashSet::new();
-# s.insert(1);
-let x = s.iter().nth(0);</t>
+          <t>let x = s.iter().nth(0);</t>
         </is>
       </c>
       <c r="F491" t="inlineStr">
         <is>
-          <t># use std::collections::HashSet;
-# let mut s = HashSet::new();
-# s.insert(1);
-let x = s.iter().next();</t>
+          <t>let x = s.iter().next();</t>
         </is>
       </c>
     </row>
@@ -17699,15 +17134,13 @@
       </c>
       <c r="E494" t="inlineStr">
         <is>
-          <t># use std::collections::HashSet;
-let mut foo = vec![0, 1, 2, 3];
+          <t>let mut foo = vec![0, 1, 2, 3];
 let bar: HashSet&lt;usize&gt; = foo.drain(..).collect();</t>
         </is>
       </c>
       <c r="F494" t="inlineStr">
         <is>
-          <t># use std::collections::HashSet;
-let foo = vec![0, 1, 2, 3];
+          <t>let foo = vec![0, 1, 2, 3];
 let bar: HashSet&lt;usize&gt; = foo.into_iter().collect();</t>
         </is>
       </c>
@@ -17903,14 +17336,12 @@
       </c>
       <c r="E500" t="inlineStr">
         <is>
-          <t># let name = "_";
-name.chars().last() == Some('_') || name.chars().next_back() == Some('-');</t>
+          <t>name.chars().last() == Some('_') || name.chars().next_back() == Some('-');</t>
         </is>
       </c>
       <c r="F500" t="inlineStr">
         <is>
-          <t># let name = "_";
-name.ends_with('_') || name.ends_with('-');</t>
+          <t>name.ends_with('_') || name.ends_with('-');</t>
         </is>
       </c>
     </row>
@@ -17935,15 +17366,13 @@
       </c>
       <c r="E501" t="inlineStr">
         <is>
-          <t># fn do_stuff(x: &amp;[i32]) {}
-let x: &amp;[i32] = &amp;[1, 2, 3, 4, 5];
+          <t>let x: &amp;[i32] = &amp;[1, 2, 3, 4, 5];
 do_stuff(x.as_ref());</t>
         </is>
       </c>
       <c r="F501" t="inlineStr">
         <is>
-          <t># fn do_stuff(x: &amp;[i32]) {}
-let x: &amp;[i32] = &amp;[1, 2, 3, 4, 5];
+          <t>let x: &amp;[i32] = &amp;[1, 2, 3, 4, 5];
 do_stuff(x);</t>
         </is>
       </c>
@@ -17969,8 +17398,7 @@
       </c>
       <c r="E502" t="inlineStr">
         <is>
-          <t># #[allow(unused)]
-(0..3).fold(false, |acc, x| acc || x &gt; 2);</t>
+          <t>(0..3).fold(false, |acc, x| acc || x &gt; 2);</t>
         </is>
       </c>
       <c r="F502" t="inlineStr">
@@ -18062,14 +17490,12 @@
       </c>
       <c r="E505" t="inlineStr">
         <is>
-          <t># let vec = vec![3, 4, 5];
-(&amp;vec).into_iter();</t>
+          <t>(&amp;vec).into_iter();</t>
         </is>
       </c>
       <c r="F505" t="inlineStr">
         <is>
-          <t># let vec = vec![3, 4, 5];
-(&amp;vec).iter();</t>
+          <t>(&amp;vec).iter();</t>
         </is>
       </c>
     </row>
@@ -18153,17 +17579,13 @@
       </c>
       <c r="E508" t="inlineStr">
         <is>
-          <t># let y: u32 = 0;
-# let x: u32 = 100;
-let add = x.checked_add(y).unwrap_or(u32::MAX);
+          <t>let add = x.checked_add(y).unwrap_or(u32::MAX);
 let sub = x.checked_sub(y).unwrap_or(u32::MIN);</t>
         </is>
       </c>
       <c r="F508" t="inlineStr">
         <is>
-          <t># let y: u32 = 0;
-# let x: u32 = 100;
-let add = x.saturating_add(y);
+          <t>let add = x.saturating_add(y);
 let sub = x.saturating_sub(y);</t>
         </is>
       </c>
@@ -18215,26 +17637,20 @@
       </c>
       <c r="E510" t="inlineStr">
         <is>
-          <t># || {
-let metadata = std::fs::metadata("foo.txt")?;
+          <t>let metadata = std::fs::metadata("foo.txt")?;
 let filetype = metadata.file_type();
 if filetype.is_file() {
     // read file
-}
-# Ok::&lt;_, std::io::Error&gt;(())
-# };</t>
+}</t>
         </is>
       </c>
       <c r="F510" t="inlineStr">
         <is>
-          <t># || {
-let metadata = std::fs::metadata("foo.txt")?;
+          <t>let metadata = std::fs::metadata("foo.txt")?;
 let filetype = metadata.file_type();
 if !filetype.is_dir() {
     // read file
-}
-# Ok::&lt;_, std::io::Error&gt;(())
-# };</t>
+}</t>
         </is>
       </c>
     </row>
@@ -18259,13 +17675,9 @@
       </c>
       <c r="E511" t="inlineStr">
         <is>
-          <t># let opt = Some("".to_string());
-opt.as_ref().map(String::as_str)
-# ;
+          <t>opt.as_ref().map(String::as_str)
 Can be written as
-# let opt = Some("".to_string());
-opt.as_deref()
-# ;</t>
+opt.as_deref()</t>
         </is>
       </c>
       <c r="F511" t="inlineStr"/>
@@ -18291,17 +17703,13 @@
       </c>
       <c r="E512" t="inlineStr">
         <is>
-          <t># let a = [1, 2, 3];
-# let b = vec![1, 2, 3];
-a[2..].iter().next();
+          <t>a[2..].iter().next();
 b.iter().next();</t>
         </is>
       </c>
       <c r="F512" t="inlineStr">
         <is>
-          <t># let a = [1, 2, 3];
-# let b = vec![1, 2, 3];
-a.get(2);
+          <t>a.get(2);
 b.get(0);</t>
         </is>
       </c>
@@ -18327,15 +17735,13 @@
       </c>
       <c r="E513" t="inlineStr">
         <is>
-          <t># let mut string = String::new();
-string.insert_str(0, "R");
+          <t>string.insert_str(0, "R");
 string.push_str("R");</t>
         </is>
       </c>
       <c r="F513" t="inlineStr">
         <is>
-          <t># let mut string = String::new();
-string.insert(0, 'R');
+          <t>string.insert(0, 'R');
 string.push('R');</t>
         </is>
       </c>
@@ -18494,14 +17900,12 @@
       </c>
       <c r="E518" t="inlineStr">
         <is>
-          <t># let iter = vec![Some(1)].into_iter();
-iter.filter_map(|x| x);</t>
+          <t>iter.filter_map(|x| x);</t>
         </is>
       </c>
       <c r="F518" t="inlineStr">
         <is>
-          <t># let iter = vec![Some(1)].into_iter();
-iter.flatten();</t>
+          <t>iter.flatten();</t>
         </is>
       </c>
     </row>
@@ -18558,14 +17962,12 @@
       </c>
       <c r="E520" t="inlineStr">
         <is>
-          <t># #[allow(unused)]
-"Hello".bytes().nth(3);</t>
+          <t>"Hello".bytes().nth(3);</t>
         </is>
       </c>
       <c r="F520" t="inlineStr">
         <is>
-          <t># #[allow(unused)]
-"Hello".as_bytes().get(3);</t>
+          <t>"Hello".as_bytes().get(3);</t>
         </is>
       </c>
     </row>
@@ -18624,8 +18026,7 @@
       </c>
       <c r="E522" t="inlineStr">
         <is>
-          <t># #![allow(unused)]
-let some_vec = vec![0, 1, 2, 3];
+          <t>let some_vec = vec![0, 1, 2, 3];
 some_vec.iter().count();
 &amp;some_vec[..].iter().count();</t>
         </is>
@@ -18659,8 +18060,7 @@
       </c>
       <c r="E523" t="inlineStr">
         <is>
-          <t># use std::borrow::Cow;
-let s = "Hello world!";
+          <t>let s = "Hello world!";
 let cow = Cow::Borrowed(s);
 let data = cow.to_owned();
 assert!(matches!(data, Cow::Borrowed(_)))</t>
@@ -18668,13 +18068,11 @@
       </c>
       <c r="F523" t="inlineStr">
         <is>
-          <t># use std::borrow::Cow;
-let s = "Hello world!";
+          <t>let s = "Hello world!";
 let cow = Cow::Borrowed(s);
 let data = cow.clone();
 assert!(matches!(data, Cow::Borrowed(_)))
 or
-# use std::borrow::Cow;
 let s = "Hello world!";
 let cow = Cow::Borrowed(s);
 let _data: String = cow.into_owned();</t>
@@ -18702,16 +18100,14 @@
       </c>
       <c r="E524" t="inlineStr">
         <is>
-          <t># let s = "";
-for x in s.splitn(1, ":") {
+          <t>for x in s.splitn(1, ":") {
     // ..
 }</t>
         </is>
       </c>
       <c r="F524" t="inlineStr">
         <is>
-          <t># let s = "";
-for x in s.splitn(2, ":") {
+          <t>for x in s.splitn(2, ":") {
     // ..
 }</t>
         </is>
@@ -19130,14 +18526,12 @@
       </c>
       <c r="E537" t="inlineStr">
         <is>
-          <t># let vec = vec![1_u8];
-let count = vec.iter().filter(|x| **x == 0u8).count();</t>
+          <t>let count = vec.iter().filter(|x| **x == 0u8).count();</t>
         </is>
       </c>
       <c r="F537" t="inlineStr">
         <is>
-          <t># let vec = vec![1_u8];
-let count = bytecount::count(&amp;vec, 0u8);</t>
+          <t>let count = bytecount::count(&amp;vec, 0u8);</t>
         </is>
       </c>
     </row>
@@ -19330,7 +18724,6 @@
         <is>
           <t>Before:
 use std::fmt;
-#[derive(Debug)]
 enum Error {
     Indivisible,
     Remainder(u8),
@@ -19366,7 +18759,6 @@
       <c r="F543" t="inlineStr">
         <is>
           <t>use std::{fmt, num::ParseIntError};
-#[derive(Debug)]
 enum Error {
    Indivisible(ParseIntError),
    Remainder(u8),
@@ -19529,14 +18921,12 @@
       </c>
       <c r="E547" t="inlineStr">
         <is>
-          <t># let x = vec![1];
-let _ = x.iter().zip(0..x.len());</t>
+          <t>let _ = x.iter().zip(0..x.len());</t>
         </is>
       </c>
       <c r="F547" t="inlineStr">
         <is>
-          <t># let x = vec![1];
-let _ = x.iter().enumerate();</t>
+          <t>let _ = x.iter().enumerate();</t>
         </is>
       </c>
     </row>
@@ -19627,13 +19017,7 @@
       </c>
       <c r="E550" t="inlineStr">
         <is>
-          <t># use std::hash::Hash;
-# use std::collections::hash_map::DefaultHasher;
-# enum Foo { Empty, WithValue(u8) }
-# use Foo::*;
-# let mut state = DefaultHasher::new();
-# let my_enum = Foo::Empty;
-match my_enum {
+          <t>match my_enum {
 	Empty =&gt; ().hash(&amp;mut state),
 	WithValue(x) =&gt; x.hash(&amp;mut state),
 }</t>
@@ -19641,13 +19025,7 @@
       </c>
       <c r="F550" t="inlineStr">
         <is>
-          <t># use std::hash::Hash;
-# use std::collections::hash_map::DefaultHasher;
-# enum Foo { Empty, WithValue(u8) }
-# use Foo::*;
-# let mut state = DefaultHasher::new();
-# let my_enum = Foo::Empty;
-match my_enum {
+          <t>match my_enum {
 	Empty =&gt; 0_u8.hash(&amp;mut state),
 	WithValue(x) =&gt; x.hash(&amp;mut state),
 }</t>
@@ -19675,18 +19053,12 @@
       </c>
       <c r="E551" t="inlineStr">
         <is>
-          <t># struct A;
-# impl A { fn foo(&amp;self) {} }
-# let mut vec: Vec&lt;A&gt; = Vec::new();
-vec.sort_by(|a, b| a.foo().cmp(&amp;b.foo()));</t>
+          <t>vec.sort_by(|a, b| a.foo().cmp(&amp;b.foo()));</t>
         </is>
       </c>
       <c r="F551" t="inlineStr">
         <is>
-          <t># struct A;
-# impl A { fn foo(&amp;self) {} }
-# let mut vec: Vec&lt;A&gt; = Vec::new();
-vec.sort_by_key(|a| a.foo());</t>
+          <t>vec.sort_by_key(|a| a.foo());</t>
         </is>
       </c>
     </row>
@@ -19741,13 +19113,10 @@
       </c>
       <c r="E553" t="inlineStr">
         <is>
-          <t># use std::io::Read;
-# use std::fs::File;
-let mut f = File::open("foo.txt").unwrap();
+          <t>let mut f = File::open("foo.txt").unwrap();
 let mut bytes = Vec::new();
 f.read_to_end(&amp;mut bytes).unwrap();
 Can be written more concisely as
-# use std::fs;
 let mut bytes = fs::read("foo.txt").unwrap();</t>
         </is>
       </c>
@@ -19774,15 +19143,13 @@
       </c>
       <c r="E554" t="inlineStr">
         <is>
-          <t># use std::collections::HashMap;
-let map: HashMap&lt;u32, u32&gt; = HashMap::new();
+          <t>let map: HashMap&lt;u32, u32&gt; = HashMap::new();
 let values = map.iter().map(|(_, value)| value).collect::&lt;Vec&lt;_&gt;&gt;();</t>
         </is>
       </c>
       <c r="F554" t="inlineStr">
         <is>
-          <t># use std::collections::HashMap;
-let map: HashMap&lt;u32, u32&gt; = HashMap::new();
+          <t>let map: HashMap&lt;u32, u32&gt; = HashMap::new();
 let values = map.values().collect::&lt;Vec&lt;_&gt;&gt;();</t>
         </is>
       </c>
@@ -19852,16 +19219,14 @@
       </c>
       <c r="E556" t="inlineStr">
         <is>
-          <t># use std::io;
-fn foo&lt;T: io::Seek&gt;(t: &amp;mut T) {
+          <t>fn foo&lt;T: io::Seek&gt;(t: &amp;mut T) {
     t.seek(io::SeekFrom::Start(0));
 }</t>
         </is>
       </c>
       <c r="F556" t="inlineStr">
         <is>
-          <t># use std::io;
-fn foo&lt;T: io::Seek&gt;(t: &amp;mut T) {
+          <t>fn foo&lt;T: io::Seek&gt;(t: &amp;mut T) {
     t.rewind();
 }</t>
         </is>
@@ -19888,14 +19253,12 @@
       </c>
       <c r="E557" t="inlineStr">
         <is>
-          <t># let iterator = vec![1].into_iter();
-let len = iterator.collect::&lt;Vec&lt;_&gt;&gt;().len();</t>
+          <t>let len = iterator.collect::&lt;Vec&lt;_&gt;&gt;().len();</t>
         </is>
       </c>
       <c r="F557" t="inlineStr">
         <is>
-          <t># let iterator = vec![1].into_iter();
-let len = iterator.count();</t>
+          <t>let len = iterator.count();</t>
         </is>
       </c>
     </row>
@@ -19982,14 +19345,12 @@
       </c>
       <c r="E560" t="inlineStr">
         <is>
-          <t># let foo = [0; 10];
-foo.iter().rev().next();</t>
+          <t>foo.iter().rev().next();</t>
         </is>
       </c>
       <c r="F560" t="inlineStr">
         <is>
-          <t># let foo = [0; 10];
-foo.iter().next_back();</t>
+          <t>foo.iter().next_back();</t>
         </is>
       </c>
     </row>
@@ -20014,12 +19375,7 @@
       </c>
       <c r="E561" t="inlineStr">
         <is>
-          <t># struct Foo {
-#     a: i32,
-#     b: i32,
-#     c: i32,
-# }
-let f = Foo { a: 0, b: 0, c: 0 };
+          <t>let f = Foo { a: 0, b: 0, c: 0 };
 match f {
     Foo { a: _, b: 0, .. } =&gt; {},
     Foo { a: _, b: _, c: _ } =&gt; {},
@@ -20028,12 +19384,7 @@
       </c>
       <c r="F561" t="inlineStr">
         <is>
-          <t># struct Foo {
-#     a: i32,
-#     b: i32,
-#     c: i32,
-# }
-let f = Foo { a: 0, b: 0, c: 0 };
+          <t>let f = Foo { a: 0, b: 0, c: 0 };
 match f {
     Foo { b: 0, .. } =&gt; {},
     Foo { .. } =&gt; {},
@@ -20119,16 +19470,12 @@
       </c>
       <c r="E564" t="inlineStr">
         <is>
-          <t># let _ =
-0x1a9BAcD
-# ;</t>
+          <t>0x1a9BAcD</t>
         </is>
       </c>
       <c r="F564" t="inlineStr">
         <is>
-          <t># let _ =
-0x1A9BACD
-# ;</t>
+          <t>0x1A9BACD</t>
         </is>
       </c>
     </row>
@@ -20153,16 +19500,12 @@
       </c>
       <c r="E565" t="inlineStr">
         <is>
-          <t># let _ =
-123832i32
-# ;</t>
+          <t>123832i32</t>
         </is>
       </c>
       <c r="F565" t="inlineStr">
         <is>
-          <t># let _ =
-123832_i32
-# ;</t>
+          <t>123832_i32</t>
         </is>
       </c>
     </row>
@@ -20187,16 +19530,12 @@
       </c>
       <c r="E566" t="inlineStr">
         <is>
-          <t># let _ =
-123832_i32
-# ;</t>
+          <t>123832_i32</t>
         </is>
       </c>
       <c r="F566" t="inlineStr">
         <is>
-          <t># let _ =
-123832i32
-# ;</t>
+          <t>123832i32</t>
         </is>
       </c>
     </row>
@@ -20227,7 +19566,6 @@
     println!("{}", a);
 }
 prints 123, while in C:
-#include &lt;stdio.h&gt;
 int main() {
     int a = 0123;
     printf("%d\n", a);
@@ -20288,8 +19626,7 @@
       </c>
       <c r="E569" t="inlineStr">
         <is>
-          <t># let v = Some("abc");
-match v {
+          <t>match v {
     Some(x) =&gt; (),
     y @ _ =&gt; (),
 }</t>
@@ -20297,8 +19634,7 @@
       </c>
       <c r="F569" t="inlineStr">
         <is>
-          <t># let v = Some("abc");
-match v {
+          <t>match v {
     Some(x) =&gt; (),
     y =&gt; (),
 }</t>
@@ -20326,9 +19662,7 @@
       </c>
       <c r="E570" t="inlineStr">
         <is>
-          <t># struct TupleStruct(u32, u32, u32);
-# let t = TupleStruct(1, 2, 3);
-match t {
+          <t>match t {
     TupleStruct(0, .., _) =&gt; (),
     _ =&gt; (),
 }</t>
@@ -20336,9 +19670,7 @@
       </c>
       <c r="F570" t="inlineStr">
         <is>
-          <t># struct TupleStruct(u32, u32, u32);
-# let t = TupleStruct(1, 2, 3);
-match t {
+          <t>match t {
     TupleStruct(0, ..) =&gt; (),
     _ =&gt; (),
 }</t>
@@ -20428,8 +19760,7 @@
       </c>
       <c r="E573" t="inlineStr">
         <is>
-          <t># let a = 0.0;
-a + 1.0;</t>
+          <t>a + 1.0;</t>
         </is>
       </c>
       <c r="F573" t="inlineStr"/>
@@ -20520,8 +19851,7 @@
       </c>
       <c r="E576" t="inlineStr">
         <is>
-          <t># let x = 1;
-if (x &amp; 1 == 2) { }</t>
+          <t>if (x &amp; 1 == 2) { }</t>
         </is>
       </c>
       <c r="F576" t="inlineStr"/>
@@ -20547,8 +19877,7 @@
       </c>
       <c r="E577" t="inlineStr">
         <is>
-          <t># let x = 1;
-if (x | 1 &gt; 3) {  }</t>
+          <t>if (x | 1 &gt; 3) {  }</t>
         </is>
       </c>
       <c r="F577" t="inlineStr"/>
@@ -20574,8 +19903,7 @@
       </c>
       <c r="E578" t="inlineStr">
         <is>
-          <t># let x = 1;
-if x &amp; 0b1111 == 0 { }</t>
+          <t>if x &amp; 0b1111 == 0 { }</t>
         </is>
       </c>
       <c r="F578" t="inlineStr"/>
@@ -20601,16 +19929,12 @@
       </c>
       <c r="E579" t="inlineStr">
         <is>
-          <t># let x = 1;
-# let y = 2;
-if x == y || x &lt; y {}</t>
+          <t>if x == y || x &lt; y {}</t>
         </is>
       </c>
       <c r="F579" t="inlineStr">
         <is>
-          <t># let x = 1;
-# let y = 2;
-if x &lt;= y {}</t>
+          <t>if x &lt;= y {}</t>
         </is>
       </c>
     </row>
@@ -20635,17 +19959,13 @@
       </c>
       <c r="E580" t="inlineStr">
         <is>
-          <t># use std::time::Duration;
-# let duration = Duration::new(5, 0);
-let micros = duration.subsec_nanos() / 1_000;
+          <t>let micros = duration.subsec_nanos() / 1_000;
 let millis = duration.subsec_nanos() / 1_000_000;</t>
         </is>
       </c>
       <c r="F580" t="inlineStr">
         <is>
-          <t># use std::time::Duration;
-# let duration = Duration::new(5, 0);
-let micros = duration.subsec_micros();
+          <t>let micros = duration.subsec_micros();
 let millis = duration.subsec_millis();</t>
         </is>
       </c>
@@ -20671,11 +19991,8 @@
       </c>
       <c r="E581" t="inlineStr">
         <is>
-          <t># let x = 1;
-if x + 1 == x + 1 {}
+          <t>if x + 1 == x + 1 {}
 // or
-# let a = 3;
-# let b = 4;
 assert_eq!(a, a);</t>
         </is>
       </c>
@@ -20795,8 +20112,7 @@
       </c>
       <c r="E585" t="inlineStr">
         <is>
-          <t># let x = 1;
-x / 1 + 0 * 1 - 0 | 0;</t>
+          <t>x / 1 + 0 * 1 - 0 | 0;</t>
         </is>
       </c>
       <c r="F585" t="inlineStr"/>
@@ -20854,14 +20170,12 @@
       </c>
       <c r="E587" t="inlineStr">
         <is>
-          <t># let x = 1.0;
-if x == f32::NAN { }</t>
+          <t>if x == f32::NAN { }</t>
         </is>
       </c>
       <c r="F587" t="inlineStr">
         <is>
-          <t># let x = 1.0f32;
-if x.is_nan() { }</t>
+          <t>if x.is_nan() { }</t>
         </is>
       </c>
     </row>
@@ -20886,16 +20200,12 @@
       </c>
       <c r="E588" t="inlineStr">
         <is>
-          <t># let x = "foo";
-# let y = String::from("foo");
-if x.to_owned() == y {}</t>
+          <t>if x.to_owned() == y {}</t>
         </is>
       </c>
       <c r="F588" t="inlineStr">
         <is>
-          <t># let x = "foo";
-# let y = String::from("foo");
-if x == y {}</t>
+          <t>if x == y {}</t>
         </is>
       </c>
     </row>
@@ -20928,9 +20238,7 @@
       </c>
       <c r="F589" t="inlineStr">
         <is>
-          <t># let x = 1.2331f64;
-# let y = 1.2332f64;
-let error_margin = f64::EPSILON; // Use an epsilon for comparison
+          <t>let error_margin = f64::EPSILON; // Use an epsilon for comparison
 // Or, if Rust &lt;= 1.42, use `std::f64::EPSILON` constant instead.
 // let error_margin = std::f64::EPSILON;
 if (y - 1.23f64).abs() &lt; error_margin { }
@@ -20966,9 +20274,7 @@
       </c>
       <c r="F590" t="inlineStr">
         <is>
-          <t># let x: f64 = 1.0;
-# const ONE: f64 = 1.00;
-let error_margin = f64::EPSILON; // Use an epsilon for comparison
+          <t>let error_margin = f64::EPSILON; // Use an epsilon for comparison
 // Or, if Rust &lt;= 1.42, use `std::f64::EPSILON` constant instead.
 // let error_margin = std::f64::EPSILON;
 if (x - ONE).abs() &lt; error_margin { }</t>
@@ -20996,8 +20302,7 @@
       </c>
       <c r="E591" t="inlineStr">
         <is>
-          <t># let x = 1;
-let a = x % 1;
+          <t>let a = x % 1;
 let a = x % -1;</t>
         </is>
       </c>
@@ -21206,14 +20511,12 @@
       </c>
       <c r="E598" t="inlineStr">
         <is>
-          <t># let p: *const [i32] = &amp;[];
-unsafe { std::mem::transmute::&lt;*const [i32], *const [u16]&gt;(p) };</t>
+          <t>unsafe { std::mem::transmute::&lt;*const [i32], *const [u16]&gt;(p) };</t>
         </is>
       </c>
       <c r="F598" t="inlineStr">
         <is>
-          <t># let p: *const [i32] = &amp;[];
-p as *const [u16];</t>
+          <t>p as *const [u16];</t>
         </is>
       </c>
     </row>
@@ -21428,14 +20731,12 @@
       </c>
       <c r="E605" t="inlineStr">
         <is>
-          <t># use core::num::NonZeroU32;
-let _non_zero: NonZeroU32 = unsafe { std::mem::transmute(123) };</t>
+          <t>let _non_zero: NonZeroU32 = unsafe { std::mem::transmute(123) };</t>
         </is>
       </c>
       <c r="F605" t="inlineStr">
         <is>
-          <t># use core::num::NonZeroU32;
-let _non_zero = unsafe { NonZeroU32::new_unchecked(123) };</t>
+          <t>let _non_zero = unsafe { NonZeroU32::new_unchecked(123) };</t>
         </is>
       </c>
     </row>
@@ -21601,8 +20902,7 @@
       </c>
       <c r="F610" t="inlineStr">
         <is>
-          <t>#[repr(C)]
-struct Foo&lt;T&gt;(u32, T);
+          <t>struct Foo&lt;T&gt;(u32, T);
 let _ = unsafe { core::mem::transmute::&lt;Foo&lt;u32&gt;, Foo&lt;i32&gt;&gt;(Foo(0u32, 0u32)) };</t>
         </is>
       </c>
@@ -21791,8 +21091,7 @@
       </c>
       <c r="E616" t="inlineStr">
         <is>
-          <t># use std::collections::LinkedList;
-let x: LinkedList&lt;usize&gt; = LinkedList::new();</t>
+          <t>let x: LinkedList&lt;usize&gt; = LinkedList::new();</t>
         </is>
       </c>
       <c r="F616" t="inlineStr"/>
@@ -21848,8 +21147,7 @@
       </c>
       <c r="E618" t="inlineStr">
         <is>
-          <t># use std::rc::Rc;
-fn foo(bar: Rc&lt;&amp;usize&gt;) {}</t>
+          <t>fn foo(bar: Rc&lt;&amp;usize&gt;) {}</t>
         </is>
       </c>
       <c r="F618" t="inlineStr">
@@ -21879,8 +21177,7 @@
       </c>
       <c r="E619" t="inlineStr">
         <is>
-          <t># use std::rc::Rc;
-fn foo(interned: Rc&lt;String&gt;) { ... }</t>
+          <t>fn foo(interned: Rc&lt;String&gt;) { ... }</t>
         </is>
       </c>
       <c r="F619" t="inlineStr">
@@ -21910,8 +21207,7 @@
       </c>
       <c r="E620" t="inlineStr">
         <is>
-          <t># use std::rc::Rc;
-struct Foo {
+          <t>struct Foo {
     inner: Rc&lt;Vec&lt;Vec&lt;Box&lt;(u32, u32, u32, u32)&gt;&gt;&gt;&gt;,
 }</t>
         </is>
@@ -22001,10 +21297,7 @@
       </c>
       <c r="E623" t="inlineStr">
         <is>
-          <t># fn foo() {};
-# fn bar() {};
-# fn baz() {};
-if {
+          <t>if {
     foo();
 } == {
     bar();
@@ -22012,17 +21305,12 @@
     baz();
 }
 is equal to
-# fn foo() {};
-# fn bar() {};
-# fn baz() {};
 {
     foo();
     bar();
     baz();
 }
 For asserts:
-# fn foo() {};
-# fn bar() {};
 assert_eq!({ foo(); }, { bar(); });
 will always succeed</t>
         </is>
@@ -22079,8 +21367,7 @@
       </c>
       <c r="E625" t="inlineStr">
         <is>
-          <t># #![allow(unused)]
-[1, 2, 3].into_iter().for_each(|n| { *n; });</t>
+          <t>[1, 2, 3].into_iter().for_each(|n| { *n; });</t>
         </is>
       </c>
       <c r="F625" t="inlineStr"/>
@@ -22133,8 +21420,7 @@
       </c>
       <c r="E627" t="inlineStr">
         <is>
-          <t>#![deny(box_pointers)]
-struct Foo {
+          <t>struct Foo {
     x: Box&lt;isize&gt;,
 }</t>
         </is>
@@ -22200,8 +21486,7 @@
       </c>
       <c r="E629" t="inlineStr">
         <is>
-          <t>#![deny(unsafe_code)]
-fn main() {
+          <t>fn main() {
     unsafe {
     }
 }</t>
@@ -22230,8 +21515,7 @@
       </c>
       <c r="E630" t="inlineStr">
         <is>
-          <t>#![deny(missing_docs)]
-pub fn foo() {}</t>
+          <t>pub fn foo() {}</t>
         </is>
       </c>
       <c r="F630" t="inlineStr"/>
@@ -22257,11 +21541,9 @@
       </c>
       <c r="E631" t="inlineStr">
         <is>
-          <t>#![deny(missing_copy_implementations)]
-pub struct Foo {
+          <t>pub struct Foo {
     pub field: i32
-}
-# fn main() {}</t>
+}</t>
         </is>
       </c>
       <c r="F631" t="inlineStr"/>
@@ -22287,9 +21569,7 @@
       </c>
       <c r="E632" t="inlineStr">
         <is>
-          <t>#![deny(missing_debug_implementations)]
-pub struct Foo;
-# fn main() {}</t>
+          <t>pub struct Foo;</t>
         </is>
       </c>
       <c r="F632" t="inlineStr"/>
@@ -22315,8 +21595,7 @@
       </c>
       <c r="E633" t="inlineStr">
         <is>
-          <t>#![deny(anonymous_parameters)]
-// edition 2015
+          <t>// edition 2015
 pub trait Foo {
     fn foo(usize);
 }
@@ -22346,8 +21625,7 @@
       </c>
       <c r="E634" t="inlineStr">
         <is>
-          <t>#[no_mangle]
-const FOO: i32 = 5;</t>
+          <t>const FOO: i32 = 5;</t>
         </is>
       </c>
       <c r="F634" t="inlineStr"/>
@@ -22373,8 +21651,7 @@
       </c>
       <c r="E635" t="inlineStr">
         <is>
-          <t>#[no_mangle]
-fn foo&lt;T&gt;(t: T) {
+          <t>fn foo&lt;T&gt;(t: T) {
 }</t>
         </is>
       </c>
@@ -22447,8 +21724,7 @@
       </c>
       <c r="E638" t="inlineStr">
         <is>
-          <t>#[track_caller]
-async fn foo() {}</t>
+          <t>async fn foo() {}</t>
         </is>
       </c>
       <c r="F638" t="inlineStr"/>
@@ -22474,8 +21750,7 @@
       </c>
       <c r="E639" t="inlineStr">
         <is>
-          <t>#![deny(unreachable_pub)]
-mod foo {
+          <t>mod foo {
     pub mod bar {
     }
 }</t>
@@ -22530,8 +21805,7 @@
       </c>
       <c r="E641" t="inlineStr">
         <is>
-          <t>#![feature(trivial_bounds)]
-pub struct A where i32: Copy;</t>
+          <t>pub struct A where i32: Copy;</t>
         </is>
       </c>
       <c r="F641" t="inlineStr"/>
@@ -22619,8 +21893,7 @@
       </c>
       <c r="E644" t="inlineStr">
         <is>
-          <t>#![deny(keyword_idents)]
-// edition 2015
+          <t>// edition 2015
 fn dyn() {}</t>
         </is>
       </c>
@@ -22645,11 +21918,7 @@
           <t>尽管鼓励人们尝试不稳定的特征，但其中一些特征是不完整或有缺陷的。此lint表示该功能尚未完成，您可能会遇到问题。</t>
         </is>
       </c>
-      <c r="E645" t="inlineStr">
-        <is>
-          <t>#![feature(generic_const_exprs)]</t>
-        </is>
-      </c>
+      <c r="E645" t="inlineStr"/>
       <c r="F645" t="inlineStr"/>
     </row>
     <row r="646">
@@ -22673,8 +21942,7 @@
       </c>
       <c r="E646" t="inlineStr">
         <is>
-          <t># #![allow(unused)]
-unsafe {
+          <t>unsafe {
     let x: &amp;'static i32 = std::mem::zeroed();
 }</t>
         </is>
@@ -22735,8 +22003,7 @@
       </c>
       <c r="E648" t="inlineStr">
         <is>
-          <t># #![allow(unused)]
-use std::ptr;
+          <t>use std::ptr;
 unsafe {
     let x = &amp;*ptr::null::&lt;i32&gt;();
     let x = ptr::addr_of!(*ptr::null::&lt;i32&gt;());
@@ -22767,8 +22034,7 @@
       </c>
       <c r="E649" t="inlineStr">
         <is>
-          <t># #![feature(asm_experimental_arch)]
-use std::arch::asm;
+          <t>use std::arch::asm;
 fn main() {
     unsafe {
         asm!("foo: bar");
@@ -22828,9 +22094,7 @@
       </c>
       <c r="E651" t="inlineStr">
         <is>
-          <t>#![deny(deref_into_dyn_supertrait)]
-#![allow(dead_code)]
-use core::ops::Deref;
+          <t>use core::ops::Deref;
 trait A {}
 trait B: A {}
 impl&lt;'a&gt; Deref for dyn 'a + B {
@@ -22868,9 +22132,7 @@
       </c>
       <c r="E652" t="inlineStr">
         <is>
-          <t># fn operation_that_requires_mutex_to_be_unlocked() {} // just to make it compile
-# let mutex = std::sync::Mutex::new(1); // just to make it compile
-let mut lock_guard = mutex.lock();
+          <t>let mut lock_guard = mutex.lock();
 std::mem::drop(&amp;lock_guard); // Should have been drop(lock_guard), mutex
 // still locked
 operation_that_requires_mutex_to_be_unlocked();</t>
@@ -22982,8 +22244,7 @@
       </c>
       <c r="E656" t="inlineStr">
         <is>
-          <t>#![deny(enum_intrinsics_non_enums)]
-core::mem::discriminant::&lt;i32&gt;(&amp;123);</t>
+          <t>core::mem::discriminant::&lt;i32&gt;(&amp;123);</t>
         </is>
       </c>
       <c r="F656" t="inlineStr"/>
@@ -23036,8 +22297,7 @@
       </c>
       <c r="E658" t="inlineStr">
         <is>
-          <t>#![deny(text_direction_codepoint_in_literal)]
-fn main() {
+          <t>fn main() {
     println!("{:?}", '‮');
 }</t>
         </is>
@@ -23176,9 +22436,7 @@
       </c>
       <c r="E662" t="inlineStr">
         <is>
-          <t># #![allow(unused)]
-# use std::ffi::CString;
-let c_str = CString::new("foo").unwrap().as_ptr();</t>
+          <t>let c_str = CString::new("foo").unwrap().as_ptr();</t>
         </is>
       </c>
       <c r="F662" t="inlineStr"/>
@@ -23206,7 +22464,6 @@
         <is>
           <t>trait A {}
 trait B {}
-#[warn(multiple_supertrait_upcastable)]
 trait C: A + B {}</t>
         </is>
       </c>
@@ -23311,9 +22568,7 @@
       </c>
       <c r="E667" t="inlineStr">
         <is>
-          <t># #![allow(unused)]
-#![deny(non_ascii_idents)]
-fn main() {
+          <t>fn main() {
     let föö = 1;
 }</t>
         </is>
@@ -23341,8 +22596,7 @@
       </c>
       <c r="E668" t="inlineStr">
         <is>
-          <t># #![allow(unused)]
-const µ: f64 = 0.000001;</t>
+          <t>const µ: f64 = 0.000001;</t>
         </is>
       </c>
       <c r="F668" t="inlineStr"/>
@@ -23451,9 +22705,7 @@
       </c>
       <c r="E672" t="inlineStr">
         <is>
-          <t># #![allow(unused)]
-#![warn(noop_method_call)]
-struct Foo;
+          <t>struct Foo;
 let foo = &amp;Foo;
 let clone: &amp;Foo = foo.clone();</t>
         </is>
@@ -23481,8 +22733,7 @@
       </c>
       <c r="E673" t="inlineStr">
         <is>
-          <t># #![allow(unused)]
-struct Foo;
+          <t>struct Foo;
 let foo = &amp;&amp;Foo;
 let clone: &amp;Foo = foo.clone();</t>
         </is>
@@ -23510,8 +22761,7 @@
       </c>
       <c r="E674" t="inlineStr">
         <is>
-          <t>#![feature(type_alias_impl_trait)]
-trait Duh {}
+          <t>trait Duh {}
 impl Duh for i32 {}
 trait Trait {
     type Assoc: Duh;
@@ -23687,8 +22937,7 @@
       </c>
       <c r="E680" t="inlineStr">
         <is>
-          <t>#![deny(variant_size_differences)]
-enum En {
+          <t>enum En {
     V0(u8),
     VBig([u8; 1024]),
 }</t>
@@ -23745,8 +22994,7 @@
       </c>
       <c r="E682" t="inlineStr">
         <is>
-          <t># #![allow(unused)]
-pub extern "C" fn str_type(p: &amp;str) { }</t>
+          <t>pub extern "C" fn str_type(p: &amp;str) { }</t>
         </is>
       </c>
       <c r="F682" t="inlineStr"/>
@@ -23772,10 +23020,8 @@
       </c>
       <c r="E683" t="inlineStr">
         <is>
-          <t># use core::sync::atomic::{AtomicU8, Ordering};
-let atom = AtomicU8::new(0);
-let value = atom.load(Ordering::Release);
-# let _ = value;</t>
+          <t>let atom = AtomicU8::new(0);
+let value = atom.load(Ordering::Release);</t>
         </is>
       </c>
       <c r="F683" t="inlineStr"/>
@@ -23832,8 +23078,7 @@
       </c>
       <c r="E685" t="inlineStr">
         <is>
-          <t>#![deny(unused_results)]
-fn foo&lt;T&gt;() -&gt; T { panic!() }
+          <t>fn foo&lt;T&gt;() -&gt; T { panic!() }
 fn main() {
     foo::&lt;usize&gt;();
 }</t>
@@ -23943,12 +23188,10 @@
       </c>
       <c r="E689" t="inlineStr">
         <is>
-          <t>#![deny(unused_import_braces)]
-use test::{A};
+          <t>use test::{A};
 pub mod test {
     pub struct A;
-}
-# fn main() {}</t>
+}</t>
         </is>
       </c>
       <c r="F689" t="inlineStr"/>
@@ -24002,9 +23245,7 @@
       </c>
       <c r="E691" t="inlineStr">
         <is>
-          <t>#![forbid(warnings)]
-#![deny(bad_style)]
-fn main() {}</t>
+          <t>fn main() {}</t>
         </is>
       </c>
       <c r="F691" t="inlineStr"/>
@@ -24030,8 +23271,7 @@
       </c>
       <c r="E692" t="inlineStr">
         <is>
-          <t>#[inline = "this is not valid"]
-fn foo() {}</t>
+          <t>fn foo() {}</t>
         </is>
       </c>
       <c r="F692" t="inlineStr"/>
@@ -24057,8 +23297,7 @@
       </c>
       <c r="E693" t="inlineStr">
         <is>
-          <t>#[repr(u32, u64)]
-enum Foo {
+          <t>enum Foo {
     Variant1,
 }</t>
         </is>
@@ -24086,8 +23325,7 @@
       </c>
       <c r="E694" t="inlineStr">
         <is>
-          <t>#![deny(meta_variable_misuse)]
-macro_rules! foo {
+          <t>macro_rules! foo {
     () =&gt; {};
     ($( $i:ident = $($j:ident),+ );*) =&gt; { $( $( $i = $k; )+ )* };
 }
@@ -24183,8 +23421,7 @@
       </c>
       <c r="E697" t="inlineStr">
         <is>
-          <t># #![allow(unused)]
-let x = 1 / 0;</t>
+          <t>let x = 1 / 0;</t>
         </is>
       </c>
       <c r="F697" t="inlineStr"/>
@@ -24236,10 +23473,7 @@
       </c>
       <c r="E699" t="inlineStr">
         <is>
-          <t>#![feature(must_not_suspend)]
-#![warn(must_not_suspend)]
-#[must_not_suspend]
-struct SyncThing {}
+          <t>struct SyncThing {}
 async fn yield_now() {}
 pub async fn uhoh() {
     let guard = SyncThing {};
@@ -24270,9 +23504,7 @@
       </c>
       <c r="E700" t="inlineStr">
         <is>
-          <t>#![deny(unused_extern_crates)]
-#![deny(warnings)]
-extern crate proc_macro;</t>
+          <t>extern crate proc_macro;</t>
         </is>
       </c>
       <c r="F700" t="inlineStr"/>
@@ -24298,8 +23530,7 @@
       </c>
       <c r="E701" t="inlineStr">
         <is>
-          <t>#![deny(unused_crate_dependencies)]
-This will produce:
+          <t>This will produce:
 error: external crate `regex` unused in `lint_example`: remove the dependency or add `use regex as _;`
   |
 note: the lint level is defined here
@@ -24332,8 +23563,7 @@
       </c>
       <c r="E702" t="inlineStr">
         <is>
-          <t>#![deny(unused_qualifications)]
-mod foo {
+          <t>mod foo {
     pub fn bar() {}
 }
 fn main() {
@@ -24363,11 +23593,7 @@
           <t>指定不存在的lint通常是错误的。检查拼写，并在lint列表中查找正确的名称。如果您使用的是旧版本的编译器，而lint仅在新版本中可用，则使用Alsoconsider。</t>
         </is>
       </c>
-      <c r="E703" t="inlineStr">
-        <is>
-          <t>#![allow(not_a_real_lint)]</t>
-        </is>
-      </c>
+      <c r="E703" t="inlineStr"/>
       <c r="F703" t="inlineStr"/>
     </row>
     <row r="704">
@@ -24391,9 +23617,7 @@
       </c>
       <c r="E704" t="inlineStr">
         <is>
-          <t>#![feature(lint_reasons)]
-#[expect(unused_variables)]
-let x = 10;
+          <t>let x = 10;
 println!("{}", x);</t>
         </is>
       </c>
@@ -24497,11 +23721,7 @@
           <t>未使用的属性可能表明该属性被放置在错误的位置。请考虑将其删除或放置在正确的位置。还要考虑您是打算使用应用于属性所在项的内部属性（带！，如#！[allow（unused）]），还是要使用应用于该属性后面项的外部属性（不带！，例如#[allow）]）。</t>
         </is>
       </c>
-      <c r="E708" t="inlineStr">
-        <is>
-          <t>#![ignore]</t>
-        </is>
-      </c>
+      <c r="E708" t="inlineStr"/>
       <c r="F708" t="inlineStr"/>
     </row>
     <row r="709">
@@ -24525,8 +23745,7 @@
       </c>
       <c r="E709" t="inlineStr">
         <is>
-          <t>#[warn(unused_tuple_struct_fields)]
-struct S(i32, i32, i32);
+          <t>struct S(i32, i32, i32);
 let s = S(1, 2, 3);
 let _ = (s.0, s.2);</t>
         </is>
@@ -24706,8 +23925,7 @@
       </c>
       <c r="E715" t="inlineStr">
         <is>
-          <t>#[warn(unused_macro_rules)]
-macro_rules! unused_empty {
+          <t>macro_rules! unused_empty {
     (hello) =&gt; { println!("Hello, world!") }; // This rule is unused
     () =&gt; { println!("empty") }; // This rule is used
 }
@@ -24739,8 +23957,7 @@
       </c>
       <c r="E716" t="inlineStr">
         <is>
-          <t>#![deny(warnings)]
-fn foo() {}</t>
+          <t>fn foo() {}</t>
         </is>
       </c>
       <c r="F716" t="inlineStr"/>
@@ -24784,8 +24001,7 @@
       </c>
       <c r="E718" t="inlineStr">
         <is>
-          <t>#![feature(test_accepted_feature)]
-fn main() {}</t>
+          <t>fn main() {}</t>
         </is>
       </c>
       <c r="F718" t="inlineStr"/>
@@ -24811,8 +24027,7 @@
       </c>
       <c r="E719" t="inlineStr">
         <is>
-          <t>#![crate_type="lol"]
-fn main() {}</t>
+          <t>fn main() {}</t>
         </is>
       </c>
       <c r="F719" t="inlineStr"/>
@@ -24838,8 +24053,7 @@
       </c>
       <c r="E720" t="inlineStr">
         <is>
-          <t>#![deny(trivial_casts)]
-let x: &amp;u32 = &amp;42;
+          <t>let x: &amp;u32 = &amp;42;
 let y = x as *const u32;</t>
         </is>
       </c>
@@ -24866,8 +24080,7 @@
       </c>
       <c r="E721" t="inlineStr">
         <is>
-          <t>#![deny(trivial_numeric_casts)]
-let x = 42_i32 as i32;</t>
+          <t>let x = 42_i32 as i32;</t>
         </is>
       </c>
       <c r="F721" t="inlineStr"/>
@@ -24893,15 +24106,13 @@
       </c>
       <c r="E722" t="inlineStr">
         <is>
-          <t># #![allow(unused)]
-struct SemiPriv;
+          <t>struct SemiPriv;
 mod m1 {
     struct Priv;
     impl super::SemiPriv {
         pub fn f(_: Priv) {}
     }
-}
-# fn main() {}</t>
+}</t>
         </is>
       </c>
       <c r="F722" t="inlineStr"/>
@@ -24927,8 +24138,7 @@
       </c>
       <c r="E723" t="inlineStr">
         <is>
-          <t>#![feature(const_mut_refs)]
-const FOO: () = unsafe {
+          <t>const FOO: () = unsafe {
     let x = &amp;[0_u8; 4];
     let y = x.as_ptr().cast::&lt;u32&gt;();
     let mut z = 123;
@@ -25047,11 +24257,7 @@
           <t>要解决此问题，请删除lint或使用新名称。这有助于避免对已失效的lints的混淆，并有助于保持重命名的lints的一致性。</t>
         </is>
       </c>
-      <c r="E727" t="inlineStr">
-        <is>
-          <t>#![deny(raw_pointer_derive)]</t>
-        </is>
-      </c>
+      <c r="E727" t="inlineStr"/>
       <c r="F727" t="inlineStr"/>
     </row>
     <row r="728">
@@ -25254,8 +24460,7 @@
       </c>
       <c r="E734" t="inlineStr">
         <is>
-          <t>#[deprecated]
-fn foo() {}
+          <t>fn foo() {}
 fn bar() {
     foo();
 }</t>
@@ -25364,8 +24569,7 @@
       </c>
       <c r="E738" t="inlineStr">
         <is>
-          <t>#![deny(single_use_lifetimes)]
-fn foo&lt;'a&gt;(x: &amp;'a u32) {}</t>
+          <t>fn foo&lt;'a&gt;(x: &amp;'a u32) {}</t>
         </is>
       </c>
       <c r="F738" t="inlineStr"/>
@@ -25391,8 +24595,7 @@
       </c>
       <c r="E739" t="inlineStr">
         <is>
-          <t>#[deny(unused_lifetimes)]
-pub fn foo&lt;'a&gt;() {}</t>
+          <t>pub fn foo&lt;'a&gt;() {}</t>
         </is>
       </c>
       <c r="F739" t="inlineStr"/>
@@ -25447,9 +24650,7 @@
       </c>
       <c r="E741" t="inlineStr">
         <is>
-          <t>#![deny(elided_lifetimes_in_paths)]
-#![deny(warnings)]
-struct Foo&lt;'a&gt; {
+          <t>struct Foo&lt;'a&gt; {
     x: &amp;'a u32
 }
 fn foo(x: &amp;Foo) {
@@ -25507,8 +24708,7 @@
       </c>
       <c r="E743" t="inlineStr">
         <is>
-          <t>#![deny(absolute_paths_not_starting_with_crate)]
-mod foo {
+          <t>mod foo {
     pub fn bar() {}
 }
 fn main() {
@@ -25687,19 +24887,15 @@
       <c r="E749" t="inlineStr">
         <is>
           <t>// foo.rs
-#![crate_type = "proc-macro"]
 extern crate proc_macro;
 use proc_macro::*;
-#[proc_macro_derive(Foo)]
 pub fn foo1(a: TokenStream) -&gt; TokenStream {
     drop(a);
     "mod __bar { static mut BAR: Option&lt;Something&gt; = None; }".parse().unwrap()
 }
 // bar.rs
-#[macro_use]
 extern crate foo;
 struct Something;
-#[derive(Foo)]
 struct Another;
 fn main() {}
 This will produce:
@@ -25737,9 +24933,7 @@
       </c>
       <c r="E750" t="inlineStr">
         <is>
-          <t>#![deny(macro_use_extern_crate)]
-#[macro_use]
-extern crate serde_json;
+          <t>extern crate serde_json;
 fn main() {
     let _ = json!{{}};
 }
@@ -25817,10 +25011,7 @@
       </c>
       <c r="E752" t="inlineStr">
         <is>
-          <t># #![allow(unused)]
-#![deny(explicit_outlives_requirements)]
-#![deny(warnings)]
-struct SharedRef&lt;'a, T&gt;
+          <t>struct SharedRef&lt;'a, T&gt;
 where
     T: 'a,
 {
@@ -25851,11 +25042,9 @@
       </c>
       <c r="E753" t="inlineStr">
         <is>
-          <t>#![deny(indirect_structural_match)]
-struct NoDerive(i32);
+          <t>struct NoDerive(i32);
 impl PartialEq for NoDerive { fn eq(&amp;self, _: &amp;Self) -&gt; bool { false } }
 impl Eq for NoDerive { }
-#[derive(PartialEq, Eq)]
 struct WrapParam&lt;T&gt;(T);
 const WRAP_INDIRECT_PARAM: &amp; &amp;WrapParam&lt;NoDerive&gt; = &amp; &amp;WrapParam(NoDerive(0));
 fn main() {
@@ -25907,8 +25096,7 @@
       </c>
       <c r="E755" t="inlineStr">
         <is>
-          <t>#![deny(pointer_structural_match)]
-fn foo(a: usize, b: usize) -&gt; usize { a + b }
+          <t>fn foo(a: usize, b: usize) -&gt; usize { a + b }
 const FOO: fn(usize, usize) -&gt; usize = foo;
 fn main() {
     match FOO {
@@ -25941,9 +25129,7 @@
       </c>
       <c r="E756" t="inlineStr">
         <is>
-          <t>#![deny(nontrivial_structural_match)]
-#[derive(Copy, Clone, Debug)]
-struct NoDerive(u32);
+          <t>struct NoDerive(u32);
 impl PartialEq for NoDerive { fn eq(&amp;self, _: &amp;Self) -&gt; bool { false } }
 impl Eq for NoDerive { }
 fn main() {
@@ -26013,9 +25199,7 @@
       </c>
       <c r="E758" t="inlineStr">
         <is>
-          <t>#[cfg(test)]
-extern crate test;
-#[bench]
+          <t>extern crate test;
 fn name(b: &amp;mut test::Bencher) {
     b.iter(|| 123)
 }</t>
@@ -26044,10 +25228,7 @@
       </c>
       <c r="E759" t="inlineStr">
         <is>
-          <t>#![feature(no_sanitize)]
-#[inline(always)]
-#[no_sanitize(address)]
-fn x() {}
+          <t>fn x() {}
 fn main() {
     x()
 }</t>
@@ -26076,8 +25257,7 @@
       </c>
       <c r="E760" t="inlineStr">
         <is>
-          <t>#[cfg(target_arch="x86_64")]
-use std::arch::asm;
+          <t>use std::arch::asm;
 fn main() {
     #[cfg(target_arch="x86_64")]
     unsafe {
@@ -26119,8 +25299,7 @@
       </c>
       <c r="E761" t="inlineStr">
         <is>
-          <t>#[cfg(target_arch="x86_64")]
-use std::arch::asm;
+          <t>use std::arch::asm;
 fn main() {
     #[cfg(target_arch="x86_64")]
     unsafe {
@@ -26163,8 +25342,7 @@
       </c>
       <c r="E762" t="inlineStr">
         <is>
-          <t>#![deny(unsafe_op_in_unsafe_fn)]
-unsafe fn foo() {}
+          <t>unsafe fn foo() {}
 unsafe fn bar() {
     foo();
 }
@@ -26194,8 +25372,7 @@
       </c>
       <c r="E763" t="inlineStr">
         <is>
-          <t># #![allow(unused)]
-enum E {
+          <t>enum E {
     A,
 }
 impl Drop for E {
@@ -26232,9 +25409,7 @@
       </c>
       <c r="E764" t="inlineStr">
         <is>
-          <t>#![feature(strict_provenance)]
-#![warn(fuzzy_provenance_casts)]
-fn main() {
+          <t>fn main() {
     let _dangling = 16_usize as *const u8;
 }</t>
         </is>
@@ -26262,9 +25437,7 @@
       </c>
       <c r="E765" t="inlineStr">
         <is>
-          <t>#![feature(strict_provenance)]
-#![warn(lossy_provenance_casts)]
-fn main() {
+          <t>fn main() {
     let x: u8 = 37;
     let _addr: usize = &amp;x as *const u8 as usize;
 }</t>
@@ -26387,7 +25560,6 @@
       <c r="E769" t="inlineStr">
         <is>
           <t>struct X;
-#[deprecated = "message"]
 impl Default for X {
     fn default() -&gt; Self {
         X
@@ -26418,13 +25590,10 @@
       </c>
       <c r="E770" t="inlineStr">
         <is>
-          <t>#![feature(asm_experimental_arch, naked_functions)]
-use std::arch::asm;
-#[naked]
+          <t>use std::arch::asm;
 pub fn default_abi() -&gt; u32 {
     unsafe { asm!("", options(noreturn)); }
 }
-#[naked]
 pub extern "Rust" fn rust_abi() -&gt; u32 {
     unsafe { asm!("", options(noreturn)); }
 }</t>
@@ -26453,11 +25622,7 @@
       </c>
       <c r="E771" t="inlineStr">
         <is>
-          <t>#![feature(staged_api)]
-#[derive(Clone)]
-#[stable(feature = "x", since = "1")]
-struct S {}
-#[unstable(feature = "y", issue = "none")]
+          <t>struct S {}
 impl Copy for S {}</t>
         </is>
       </c>
@@ -26484,8 +25649,7 @@
       </c>
       <c r="E772" t="inlineStr">
         <is>
-          <t>#![deny(semicolon_in_expressions_from_macros)]
-macro_rules! foo {
+          <t>macro_rules! foo {
     () =&gt; { true; }
 }
 fn main() {
@@ -26519,9 +25683,7 @@
       </c>
       <c r="E773" t="inlineStr">
         <is>
-          <t>#[serde(rename_all = "camelCase")]
-#[derive(Deserialize)]
-struct S { /* fields */ }
+          <t>struct S { /* fields */ }
 produces:
 warning: derive helper attribute is used before it is introduced
   --&gt; $DIR/legacy-derive-helpers.rs:1:3
@@ -26586,11 +25748,7 @@
           <t>#！[crate_type]和#！[crate_name]属性需要在编译器中进行破解，才能在宏扩展后更改所使用的crate类型和crat名称。这两个属性都不能与Cargo结合使用，因为它在命令行上显式传递--crate type和--crate name。这些值必须与源代码中使用的值匹配，以防止出现错误。若要修复警告，请在运行grustc时在命令行中使用--crate类型，而不是#！[cfg_attr（…，crate_type=“…”）]和--机箱名称，而不是#！[cfg_attr（…，crate_name=“…”）]。</t>
         </is>
       </c>
-      <c r="E775" t="inlineStr">
-        <is>
-          <t>#![cfg_attr(debug_assertions, crate_type = "lib")]</t>
-        </is>
-      </c>
+      <c r="E775" t="inlineStr"/>
       <c r="F775" t="inlineStr"/>
     </row>
     <row r="776">
@@ -26615,7 +25773,6 @@
       <c r="E776" t="inlineStr">
         <is>
           <t>rustc --check-cfg 'names()'
-#[cfg(widnows)]
 fn foo() {}
 This will produce:
 warning: unknown condition name used
@@ -26650,9 +25807,7 @@
       </c>
       <c r="E777" t="inlineStr">
         <is>
-          <t>#![deny(repr_transparent_external_private_fields)]
-use foo::NonExhaustiveZst;
-#[repr(transparent)]
+          <t>use foo::NonExhaustiveZst;
 struct Bar(u32, ([u32; 0], NonExhaustiveZst));
 This will produce:
 error: zero-sized fields in repr(transparent) cannot contain external non-exhaustive types
@@ -26694,8 +25849,7 @@
       </c>
       <c r="E778" t="inlineStr">
         <is>
-          <t>#[cfg(FALSE)]
-macro foo() {}</t>
+          <t>macro foo() {}</t>
         </is>
       </c>
       <c r="F778" t="inlineStr"/>
@@ -26721,8 +25875,7 @@
       </c>
       <c r="E779" t="inlineStr">
         <is>
-          <t>#![deny(ambiguous_glob_reexports)]
-pub mod foo {
+          <t>pub mod foo {
     pub type X = u8;
 }
 pub mod bar {
@@ -26784,8 +25937,7 @@
       </c>
       <c r="E781" t="inlineStr">
         <is>
-          <t>#![deny(rust_2021_incompatible_closure_captures)]
-use std::thread;
+          <t>use std::thread;
 struct Pointer(*mut i32);
 unsafe impl Send for Pointer {}
 fn main() {
@@ -26820,8 +25972,7 @@
       </c>
       <c r="E782" t="inlineStr">
         <is>
-          <t>#![deny(missing_abi)]
-extern fn foo() {}</t>
+          <t>extern fn foo() {}</t>
         </is>
       </c>
       <c r="F782" t="inlineStr"/>
@@ -26847,8 +25998,7 @@
       </c>
       <c r="E783" t="inlineStr">
         <is>
-          <t>#![deny(warnings)]
-pub mod submodule {
+          <t>pub mod submodule {
     #![doc(test(no_crate_inject))]
 }</t>
         </is>
@@ -26916,8 +26066,7 @@
       </c>
       <c r="E785" t="inlineStr">
         <is>
-          <t>#![deny(rust_2021_incompatible_or_patterns)]
-macro_rules! match_any {
+          <t>macro_rules! match_any {
     ( $expr:expr , $( $( $pat:pat )|+ =&gt; $expr_arm:expr ),+ ) =&gt; {
         match $expr {
             $(
@@ -26956,8 +26105,7 @@
       </c>
       <c r="E786" t="inlineStr">
         <is>
-          <t>#![deny(rust_2021_prelude_collisions)]
-trait Foo {
+          <t>trait Foo {
     fn try_into(self) -&gt; Result&lt;String, !&gt;;
 }
 impl Foo for &amp;str {
@@ -26997,8 +26145,7 @@
       </c>
       <c r="E787" t="inlineStr">
         <is>
-          <t>#![deny(rust_2021_prefixes_incompatible_syntax)]
-macro_rules! m {
+          <t>macro_rules! m {
     (z $x:expr) =&gt; ();
 }
 m!(z"hey");</t>
@@ -27093,13 +26240,11 @@
       <c r="E790" t="inlineStr">
         <is>
           <t>// crate A
-#[non_exhaustive]
 pub enum Bar {
     A,
     B, // added variant in non breaking change
 }
 // in crate B
-#![feature(non_exhaustive_omitted_patterns_lint)]
 match Bar::A {
     Bar::A =&gt; {},
     #[warn(non_exhaustive_omitted_patterns)]
@@ -27144,8 +26289,7 @@
       </c>
       <c r="E791" t="inlineStr">
         <is>
-          <t>#![deny(text_direction_codepoint_in_comment)]
-fn main() {
+          <t>fn main() {
     println!("{:?}"); // '‮');
 }</t>
         </is>
@@ -27173,9 +26317,7 @@
       </c>
       <c r="E792" t="inlineStr">
         <is>
-          <t>#[test]
-#[test]
-fn foo() {}
+          <t>fn foo() {}
 This will produce:
 warning: duplicated attribute
  --&gt; src/lib.rs:2:1
@@ -27265,11 +26407,7 @@
           <t>为了测试不稳定棉绒的性能，需要一个永久不稳定的棉绒。此lint可用于从编译器中触发与不稳定lint相关的警告和错误。</t>
         </is>
       </c>
-      <c r="E795" t="inlineStr">
-        <is>
-          <t>#![allow(test_unstable_lint)]</t>
-        </is>
-      </c>
+      <c r="E795" t="inlineStr"/>
       <c r="F795" t="inlineStr"/>
     </row>
     <row r="796">
@@ -27293,8 +26431,7 @@
       </c>
       <c r="E796" t="inlineStr">
         <is>
-          <t>#![warn(ffi_unwind_calls)]
-extern "C-unwind" {
+          <t>extern "C-unwind" {
     fn foo();
 }
 fn bar() {
@@ -27327,8 +26464,7 @@
       </c>
       <c r="E797" t="inlineStr">
         <is>
-          <t>#![deny(named_arguments_used_positionally)]
-fn main() {
+          <t>fn main() {
     let _x = 5;
     println!("{}", _x = 1); // Prints 1, will trigger lint
     println!("{}", _x); // Prints 5, no lint emitted
@@ -27359,8 +26495,7 @@
       </c>
       <c r="E798" t="inlineStr">
         <is>
-          <t>#![deny(implied_bounds_entailment)]
-trait Trait {
+          <t>trait Trait {
     fn get&lt;'s&gt;(s: &amp;'s str, _: &amp;'static &amp;'static ()) -&gt; &amp;'static str;
 }
 impl Trait for () {
@@ -27395,9 +26530,7 @@
       </c>
       <c r="E799" t="inlineStr">
         <is>
-          <t>#[repr(packed)]
-#[derive(Hash)]
-struct FlexZeroSlice {
+          <t>struct FlexZeroSlice {
     width: u8,
     data: [u8],
 }</t>
@@ -27426,14 +26559,11 @@
       </c>
       <c r="E800" t="inlineStr">
         <is>
-          <t>#![deny(invalid_macro_export_arguments)]
-#[macro_export(invalid_parameter)]
-macro_rules! myMacro {
+          <t>macro_rules! myMacro {
    () =&gt; {
         // [...]
    }
-}
-#[macro_export(too, many, items)]</t>
+}</t>
         </is>
       </c>
       <c r="F800" t="inlineStr"/>

</xml_diff>

<commit_message>
add just default whitelist
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -3288,7 +3288,7 @@
       <c r="C80" t="inlineStr"/>
       <c r="D80" t="inlineStr">
         <is>
-          <t>检查没有变体的枚举。截至本文撰写之时，never_type仍然是唯一的实验性API。因此，只有启用了never_type，才会触发此lint。</t>
+          <t>检查没有变体的枚举。截至本文撰写之时，never_type仍然是唯一的实验性API。因此，此lint仅在启用never_type时触发。</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
@@ -4959,7 +4959,7 @@
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>由于构造函数中字段的顺序不会影响结果实例，如下例所示，#[drivee（Debug，PartialEq，Eq）]struct Foo{x:i32，y:i32；}let x=1；设y=2；//这个断言永远不会失败：assert_eq！（Foo{x，y}，Foo{y，x}）；不一致的顺序可能会造成混乱，降低可读性和一致性。</t>
+          <t>由于构造函数中字段的顺序不会影响结果实例，如下例所示，structFoo｛x:i32，y:i32｝让x＝1；设y=2；//这个断言永远不会失败：assert_eq！（Foo{x，y}，Foo{y，x}）；不一致的顺序可能会造成混乱，降低可读性和一致性。</t>
         </is>
       </c>
       <c r="F127" t="inlineStr">
@@ -9525,7 +9525,7 @@
       <c r="C257" t="inlineStr"/>
       <c r="D257" t="inlineStr">
         <is>
-          <t>检查不是应用到的类型的精确表示的模式。要满足此lint，您必须调整与匹配的表达式或模式本身，以及调整后的模式引入的绑定。为了进行匹配，您必须使用*运算符取消对表达式的引用，或者根据引用的可变性修改模式以显式匹配&amp;&lt;pattern&gt;或&amp;mut&lt;pattern&gt;。对于绑定，您需要使用相反的方法。如果您希望复制值，可以将它们保留为纯绑定，但必须使用ref mut＜variable＞或ref＜variable＜在匹配的结构中构造引用。如果您正在寻找更详细地了解所有权语义的方法，建议您查看可用的IDE选项，以突出显示代码中的类型、生命周期和引用语义。即使在各种模式匹配机制之外，可用的工具也会以通用的方式暴露这些东西。当然，这个lint仍然可以用来突出感兴趣的领域，并确保很好地理解所有权语义。</t>
+          <t>检查不是应用到的类型的精确表示的模式。要满足此lint，您必须调整与匹配的表达式或模式本身，以及调整后的模式引入的绑定。为了进行匹配，您必须使用*运算符取消对表达式的引用，或者根据引用的可变性修改模式以显式匹配&amp;&lt;pattern&gt;或&amp;mut&lt;pattern&gt;。对于绑定，您需要使用相反的方法。如果您希望复制值，可以将它们保留为纯绑定，但必须使用ref mut＜variable＞或ref＜variable＜在匹配的结构中构造引用。如果您正在寻找更详细地了解所有权语义的方法，建议您查看可用的IDE选项，以突出显示代码中的类型、生命周期和引用语义。即使在各种模式匹配机制之外，可用的工具也会以通用的方式暴露这些东西。当然，这个lint仍然可以用来突出感兴趣的领域，并确保对所有权语义有很好的理解。</t>
         </is>
       </c>
       <c r="E257" t="inlineStr">
@@ -19317,7 +19317,7 @@
       <c r="C542" t="inlineStr"/>
       <c r="D542" t="inlineStr">
         <is>
-          <t>在Iterator或Option上检查map（|x|x.clone（））ordereferencing闭包对Copy类型的使用情况，并建议改用cloned（）或copied（）</t>
+          <t>在Iterator或Option上检查map（|x|x.clone（））orderreference闭包对Copy类型的使用情况，并建议改用cloned（）或copied（）</t>
         </is>
       </c>
       <c r="E542" t="inlineStr">
@@ -21236,7 +21236,7 @@
       </c>
       <c r="E599" t="inlineStr">
         <is>
-          <t>很容易错误地在一种类型和apointer之间转换为该类型。</t>
+          <t>很容易在一个类型和该类型的apointer之间错误地转换。</t>
         </is>
       </c>
       <c r="F599" t="inlineStr">
@@ -21602,7 +21602,7 @@
       </c>
       <c r="E610" t="inlineStr">
         <is>
-          <t>这种转化的结果是没有定义的。</t>
+          <t>这种transmite的结果没有定义。</t>
         </is>
       </c>
       <c r="F610" t="inlineStr">
@@ -21630,7 +21630,7 @@
       <c r="C611" t="inlineStr"/>
       <c r="D611" t="inlineStr">
         <is>
-          <t>检查将接收空指针的transmate调用。</t>
+          <t>检查将接收空指针的transmite调用。</t>
         </is>
       </c>
       <c r="E611" t="inlineStr">
@@ -22550,7 +22550,7 @@
       </c>
       <c r="E641" t="inlineStr">
         <is>
-          <t>通常情况下，你不会写一个你知道永远都是错误的或永远都不是真的特质。但是，当使用宏时，宏可能不知道在生成代码时约束是否成立。目前，如果约束始终为真，编译器不会提醒您，如果约束从不为真，则会生成错误。trivial_bounds功能在这两种情况下都会将其更改为警告，使宏在生成代码时具有更大的自由度和灵活性，同时在编写非宏代码时仍会发出出错的信号。有关更多详细信息，请参阅RFC 2056。此功能目前仅在夜间频道可用，请参阅跟踪问题#48214。</t>
+          <t>通常情况下，你不会写一个你知道永远都是错误的或永远都不是真的特质。但是，当使用宏时，宏可能不知道在生成代码时约束是否成立。目前，如果约束始终为真，编译器不会提醒您，如果约束从不为真，则会生成错误。trivial_bounds功能在这两种情况下都会将其更改为警告，使宏在生成代码时具有更大的自由度和灵活性，同时在编写非宏代码时仍会发出出错的信号。有关更多详细信息，请参阅RFC 2056。此功能目前仅在nighty频道上可用，请参阅跟踪问题#48214。</t>
         </is>
       </c>
       <c r="F641" t="inlineStr">
@@ -25056,7 +25056,7 @@
       </c>
       <c r="E724" t="inlineStr">
         <is>
-          <t>依赖项可以标记为“私有”，表示它们不会在机箱的公共接口中导出。货航可以使用它来独立解决这些依赖关系，因为它可以假设不需要将它们与使用相同依赖关系的其他包统一。此lint表示违反了该约定。要解决此问题，请避免在公共接口中暴露依赖项。或者，将依赖项切换为公共依赖项。请注意，仅在夜间频道上提供对此的支持。有关更多详细信息，请参阅RFC 1977以及Cargo文档。</t>
+          <t>依赖项可以标记为“私有”，表示它们不会在机箱的公共接口中导出。货航可以使用它来独立解决这些依赖关系，因为它可以假设不需要将它们与使用相同依赖关系的其他包统一。此lint表示违反了该约定。要解决此问题，请避免在公共接口中暴露依赖项。或者，将依赖项切换为公共依赖项。请注意，仅在nighty频道上提供对此的支持。有关更多详细信息，请参阅RFC 1977以及Cargo文档。</t>
         </is>
       </c>
       <c r="F724" t="inlineStr">
@@ -25645,7 +25645,7 @@
       </c>
       <c r="E744" t="inlineStr">
         <is>
-          <t>以前版本的编译器接受模式中的浮点文字，但后来确定这是一个错误。与“结构相等”相比，比较浮点值的要求在模式中可能不明确。通常，您可以使用火柴保护来解决此问题，例如：#let x=42.0；match x｛y if y==5.0=&gt;｛｝_=&gt;｛}｝这是一个未来不兼容的lint，将来将其转换为硬错误。有关更多详细信息，请参阅第41620期。</t>
+          <t>以前版本的编译器接受模式中的浮点文字，但后来确定这是一个错误。与“结构相等”相比，比较浮点值的要求在模式中可能不明确。通常，您可以使用匹配保护来解决此问题，例如：match x｛y if y==5.0=&gt;｛｝_=&gt;｛}｝这是一个未来不兼容的lint，可以在未来将其转换为硬错误。有关更多详细信息，请参阅第41620期。</t>
         </is>
       </c>
       <c r="F744" t="inlineStr">
@@ -26622,7 +26622,7 @@
       </c>
       <c r="E773" t="inlineStr">
         <is>
-          <t>由于历史原因，类似这样的属性可以工作，但属性扩展通常以左到右的顺序工作，因此，为了解决#[serde]，编译器必须尝试在项目的尚未扩展部分“展望未来”，但这种尝试并不总是可靠的。要修复警告，请将helper属性放在其相应的派生之后#[driven（Deserialize）]#[serde（rename_all=“camelCase”）]struct S｛/*fields*/｝</t>
+          <t>由于历史原因，类似这样的属性可以工作，但属性扩展通常按左到右的顺序工作，因此，为了解决#[serde]问题，编译器必须尝试在项目的尚未扩展部分“展望未来”，但这种尝试并不总是可靠的。要修复警告，请将helper属性放在其相应的derive.struct S｛/*fields*/｝之后</t>
         </is>
       </c>
       <c r="F773" t="inlineStr">
@@ -26793,7 +26793,7 @@
       </c>
       <c r="E778" t="inlineStr">
         <is>
-          <t>活动属性（如#[cfg]或过程宏属性）的输入必须是有效语法。以前，编译器只有在解析#[cfg]门并扩展过程宏之后才允许使用不稳定的语法功能。为了避免依赖不稳定的句法，请将不稳定语法的使用移到编译器不解析语法的位置，例如函数式宏。##！[deniy（unstatible_syntax_pre_expansion）]macro_rules！identity｛（$（$tokens:tt）*）=&gt;｛$（$tokens）*｝#[cfg（FALSE）]identity！｛macro foo（）｛｝｝这是一个未来不兼容的lint，可以在未来将其转换为一个硬错误。有关更多详细信息，请参阅第65860期。</t>
+          <t>活动属性（如#[cfg]或过程宏属性）的输入必须是有效语法。以前，编译器只有在解析#[cfg]门并扩展过程宏之后才允许使用不稳定的语法功能。为了避免依赖不稳定的句法，请将不稳定语法的使用移到编译器不解析语法的位置，例如函数类macro.macro_rules！身份｛（$（$tokens:tt）*）=&gt;｛$（$tokens）*｝｝身份！｛macro foo（）｛｝｝这是一个未来不兼容的lint，可以在未来将其转换为一个硬错误。有关更多详细信息，请参阅第65860期。</t>
         </is>
       </c>
       <c r="F778" t="inlineStr">

</xml_diff>